<commit_message>
adjusting rune_management for release
</commit_message>
<xml_diff>
--- a/summoners_war_0_1_0/output/xlsx_reports/speed_charts.xlsx
+++ b/summoners_war_0_1_0/output/xlsx_reports/speed_charts.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\Google Drive\Games\Summoner's War\BKsDBTools-0.1.0\summoners_war_0_1_0\output\xlsx_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\BKsDBTools\summoners_war_0_1_0\output\xlsx_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18230" windowHeight="7010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="7005"/>
   </bookViews>
   <sheets>
     <sheet name="Speed Calculators" sheetId="1" r:id="rId1"/>
-    <sheet name="Speed Ranges" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Monster</t>
   </si>
@@ -103,51 +102,6 @@
   </si>
   <si>
     <t>How to Speed Tune + What are Ticks?</t>
-  </si>
-  <si>
-    <t>(trition, tiana), -&gt; Atk bar booster -&gt; immunity / buffers -&gt; strippers -&gt; debuffers -&gt; dmg</t>
-  </si>
-  <si>
-    <t>fastest atk bar booster</t>
-  </si>
-  <si>
-    <t>Slowest Damage should be</t>
-  </si>
-  <si>
-    <t>slowest atk bar booster</t>
-  </si>
-  <si>
-    <t>fastest immunity / buffers</t>
-  </si>
-  <si>
-    <t>slowest immunity / buffers</t>
-  </si>
-  <si>
-    <t>fastest dmg</t>
-  </si>
-  <si>
-    <t>fastest stripper</t>
-  </si>
-  <si>
-    <t>slowest stripper</t>
-  </si>
-  <si>
-    <t>fastest debuffer</t>
-  </si>
-  <si>
-    <t>slowest debuffer</t>
-  </si>
-  <si>
-    <t>Tick 7 - 100% bar</t>
-  </si>
-  <si>
-    <t>Tick 6 - 100% bar</t>
-  </si>
-  <si>
-    <t>Tick 5 - 100% bar</t>
-  </si>
-  <si>
-    <t>Tick 4 - 100% bar</t>
   </si>
   <si>
     <t>3: Atk bar % @ tick for a given combat speed</t>
@@ -259,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,12 +250,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -749,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -824,7 +772,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
@@ -929,7 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1236,114 +1183,114 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="8.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="5.90625" customWidth="1"/>
-    <col min="11" max="12" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="32" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="52" t="s">
-        <v>42</v>
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="51" t="s">
+        <v>27</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
+      <c r="P1" s="101"/>
+      <c r="Q1" s="101"/>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
       <c r="U1" s="11"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
-        <v>69</v>
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="103" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="104" t="s">
+      <c r="D2" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="102"/>
+      <c r="G2" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="92"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="91"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="83" t="s">
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="84" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87">
+      <c r="D3" s="85"/>
+      <c r="E3" s="86">
+        <v>0.24</v>
+      </c>
+      <c r="F3" s="87">
+        <v>0.15</v>
+      </c>
+      <c r="G3" s="85"/>
+      <c r="H3" s="87">
         <v>0</v>
       </c>
-      <c r="F3" s="88">
-        <v>0.15</v>
-      </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="88">
-        <v>0</v>
-      </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="53" t="s">
+      <c r="I3" s="88"/>
+      <c r="J3" s="52" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="9">
@@ -1381,1354 +1328,1354 @@
       </c>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="51"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="50"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="99">
+      <c r="D4" s="98">
         <v>104</v>
       </c>
-      <c r="E4" s="100">
+      <c r="E4" s="99">
         <f>SUM($D4*(1+$E$3+$F$3))</f>
-        <v>119.6</v>
-      </c>
-      <c r="F4" s="100"/>
-      <c r="G4" s="93">
+        <v>144.56</v>
+      </c>
+      <c r="F4" s="99"/>
+      <c r="G4" s="92">
         <v>89</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H4" s="65">
         <f>SUM($H$3)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="76">
+      <c r="I4" s="75">
         <f>SUM(($E4+$G4)*(1+$H4))</f>
-        <v>208.6</v>
-      </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55">
+        <v>233.56</v>
+      </c>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54">
         <f>SUM($I4*(0.07*1))</f>
-        <v>14.602</v>
-      </c>
-      <c r="L4" s="55">
+        <v>16.349200000000003</v>
+      </c>
+      <c r="L4" s="54">
         <f>SUM($I4*(0.07*2))</f>
-        <v>29.204000000000001</v>
-      </c>
-      <c r="M4" s="55">
+        <v>32.698400000000007</v>
+      </c>
+      <c r="M4" s="54">
         <f>SUM($I4*(0.07*3))</f>
-        <v>43.806000000000004</v>
-      </c>
-      <c r="N4" s="55">
+        <v>49.047600000000003</v>
+      </c>
+      <c r="N4" s="54">
         <f>SUM($I4*(0.07*4))</f>
-        <v>58.408000000000001</v>
-      </c>
-      <c r="O4" s="55">
+        <v>65.396800000000013</v>
+      </c>
+      <c r="O4" s="54">
         <f>SUM($I4*(0.07*5))</f>
-        <v>73.010000000000005</v>
-      </c>
-      <c r="P4" s="55">
+        <v>81.746000000000009</v>
+      </c>
+      <c r="P4" s="54">
         <f>SUM($I4*(0.07*6))</f>
-        <v>87.612000000000009</v>
-      </c>
-      <c r="Q4" s="55">
+        <v>98.095200000000006</v>
+      </c>
+      <c r="Q4" s="54">
         <f>SUM($I4*(0.07*7))</f>
-        <v>102.21400000000001</v>
-      </c>
-      <c r="R4" s="55">
+        <v>114.44440000000002</v>
+      </c>
+      <c r="R4" s="54">
         <f>SUM($I4*(0.07*8))</f>
-        <v>116.816</v>
-      </c>
-      <c r="S4" s="55">
+        <v>130.79360000000003</v>
+      </c>
+      <c r="S4" s="54">
         <f>SUM($I4*(0.07*9))</f>
-        <v>131.41800000000001</v>
-      </c>
-      <c r="T4" s="55">
+        <v>147.14280000000002</v>
+      </c>
+      <c r="T4" s="54">
         <f>SUM($I4*(0.07*10))</f>
-        <v>146.02000000000001</v>
-      </c>
-      <c r="U4" s="56">
+        <v>163.49200000000002</v>
+      </c>
+      <c r="U4" s="55">
         <f>SUM($I4*(0.07*11))</f>
-        <v>160.62199999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+        <v>179.84120000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>62</v>
+      <c r="B5" s="50" t="s">
+        <v>47</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="67">
+      <c r="D5" s="66">
         <v>126</v>
       </c>
-      <c r="E5" s="100">
+      <c r="E5" s="99">
         <f>SUM($D5*(1+$E$3+$F$3))</f>
-        <v>144.89999999999998</v>
-      </c>
-      <c r="F5" s="100"/>
-      <c r="G5" s="93">
+        <v>175.14</v>
+      </c>
+      <c r="F5" s="99"/>
+      <c r="G5" s="92">
         <v>190</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="65">
         <f t="shared" ref="H5:H21" si="0">SUM($H$3)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="76">
+      <c r="I5" s="75">
         <f>SUM(($E5+$G5)*(1+$H5))</f>
-        <v>334.9</v>
-      </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55">
+        <v>365.14</v>
+      </c>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54">
         <f t="shared" ref="K5:K21" si="1">SUM($I5*(0.07*1))</f>
-        <v>23.443000000000001</v>
-      </c>
-      <c r="L5" s="55">
+        <v>25.559800000000003</v>
+      </c>
+      <c r="L5" s="54">
         <f t="shared" ref="L5:L21" si="2">SUM($I5*(0.07*2))</f>
-        <v>46.886000000000003</v>
-      </c>
-      <c r="M5" s="55">
+        <v>51.119600000000005</v>
+      </c>
+      <c r="M5" s="54">
         <f t="shared" ref="M5:M21" si="3">SUM($I5*(0.07*3))</f>
-        <v>70.329000000000008</v>
-      </c>
-      <c r="N5" s="55">
+        <v>76.679400000000001</v>
+      </c>
+      <c r="N5" s="54">
         <f t="shared" ref="N5:N21" si="4">SUM($I5*(0.07*4))</f>
-        <v>93.772000000000006</v>
-      </c>
-      <c r="O5" s="55">
+        <v>102.23920000000001</v>
+      </c>
+      <c r="O5" s="54">
         <f t="shared" ref="O5:O21" si="5">SUM($I5*(0.07*5))</f>
-        <v>117.215</v>
-      </c>
-      <c r="P5" s="55">
+        <v>127.79900000000001</v>
+      </c>
+      <c r="P5" s="54">
         <f t="shared" ref="P5:P21" si="6">SUM($I5*(0.07*6))</f>
-        <v>140.65800000000002</v>
-      </c>
-      <c r="Q5" s="55">
+        <v>153.3588</v>
+      </c>
+      <c r="Q5" s="54">
         <f t="shared" ref="Q5:Q21" si="7">SUM($I5*(0.07*7))</f>
-        <v>164.101</v>
-      </c>
-      <c r="R5" s="55">
+        <v>178.9186</v>
+      </c>
+      <c r="R5" s="54">
         <f t="shared" ref="R5:R21" si="8">SUM($I5*(0.07*8))</f>
-        <v>187.54400000000001</v>
-      </c>
-      <c r="S5" s="55">
+        <v>204.47840000000002</v>
+      </c>
+      <c r="S5" s="54">
         <f t="shared" ref="S5:S21" si="9">SUM($I5*(0.07*9))</f>
-        <v>210.98700000000002</v>
-      </c>
-      <c r="T5" s="55">
+        <v>230.03820000000005</v>
+      </c>
+      <c r="T5" s="54">
         <f t="shared" ref="T5:T21" si="10">SUM($I5*(0.07*10))</f>
-        <v>234.43</v>
-      </c>
-      <c r="U5" s="56">
+        <v>255.59800000000001</v>
+      </c>
+      <c r="U5" s="55">
         <f t="shared" ref="U5:U21" si="11">SUM($I5*(0.07*11))</f>
-        <v>257.87299999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>52</v>
+        <v>281.15780000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>37</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="65">
+      <c r="D6" s="64">
         <v>116</v>
       </c>
-      <c r="E6" s="100">
+      <c r="E6" s="99">
         <f t="shared" ref="E6:E21" si="12">SUM($D6*(1+$E$3+$F$3))</f>
-        <v>133.39999999999998</v>
-      </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="93">
+        <v>161.23999999999998</v>
+      </c>
+      <c r="F6" s="99"/>
+      <c r="G6" s="92">
         <v>156</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="76">
+      <c r="I6" s="75">
         <f t="shared" ref="I6:I21" si="13">SUM(($E6+$G6)*(1+$H6))</f>
-        <v>289.39999999999998</v>
-      </c>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55">
+        <v>317.24</v>
+      </c>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54">
         <f t="shared" si="1"/>
-        <v>20.257999999999999</v>
-      </c>
-      <c r="L6" s="55">
+        <v>22.206800000000001</v>
+      </c>
+      <c r="L6" s="54">
         <f t="shared" si="2"/>
-        <v>40.515999999999998</v>
-      </c>
-      <c r="M6" s="55">
+        <v>44.413600000000002</v>
+      </c>
+      <c r="M6" s="54">
         <f t="shared" si="3"/>
-        <v>60.774000000000001</v>
-      </c>
-      <c r="N6" s="55">
+        <v>66.620400000000004</v>
+      </c>
+      <c r="N6" s="54">
         <f t="shared" si="4"/>
-        <v>81.031999999999996</v>
-      </c>
-      <c r="O6" s="55">
+        <v>88.827200000000005</v>
+      </c>
+      <c r="O6" s="54">
         <f t="shared" si="5"/>
-        <v>101.29</v>
-      </c>
-      <c r="P6" s="55">
+        <v>111.03400000000002</v>
+      </c>
+      <c r="P6" s="54">
         <f t="shared" si="6"/>
-        <v>121.548</v>
-      </c>
-      <c r="Q6" s="55">
+        <v>133.24080000000001</v>
+      </c>
+      <c r="Q6" s="54">
         <f t="shared" si="7"/>
-        <v>141.80600000000001</v>
-      </c>
-      <c r="R6" s="55">
+        <v>155.44760000000002</v>
+      </c>
+      <c r="R6" s="54">
         <f t="shared" si="8"/>
-        <v>162.06399999999999</v>
-      </c>
-      <c r="S6" s="55">
+        <v>177.65440000000001</v>
+      </c>
+      <c r="S6" s="54">
         <f t="shared" si="9"/>
-        <v>182.32200000000003</v>
-      </c>
-      <c r="T6" s="55">
+        <v>199.86120000000005</v>
+      </c>
+      <c r="T6" s="54">
         <f t="shared" si="10"/>
-        <v>202.58</v>
-      </c>
-      <c r="U6" s="56">
+        <v>222.06800000000004</v>
+      </c>
+      <c r="U6" s="55">
         <f t="shared" si="11"/>
-        <v>222.83799999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" s="54" t="s">
+        <v>244.2748</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>56</v>
+      <c r="B7" s="50" t="s">
+        <v>41</v>
       </c>
       <c r="C7" s="6">
         <v>30</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="64">
         <v>120</v>
       </c>
-      <c r="E7" s="100">
+      <c r="E7" s="99">
         <f t="shared" si="12"/>
-        <v>138</v>
-      </c>
-      <c r="F7" s="100"/>
-      <c r="G7" s="93">
+        <v>166.79999999999998</v>
+      </c>
+      <c r="F7" s="99"/>
+      <c r="G7" s="92">
         <v>162</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="76">
+      <c r="I7" s="75">
         <f t="shared" si="13"/>
-        <v>300</v>
-      </c>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55">
+        <v>328.79999999999995</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54">
         <f t="shared" si="1"/>
-        <v>21.000000000000004</v>
-      </c>
-      <c r="L7" s="55">
+        <v>23.015999999999998</v>
+      </c>
+      <c r="L7" s="54">
         <f t="shared" si="2"/>
-        <v>42.000000000000007</v>
-      </c>
-      <c r="M7" s="55">
+        <v>46.031999999999996</v>
+      </c>
+      <c r="M7" s="54">
         <f t="shared" si="3"/>
-        <v>63.000000000000007</v>
-      </c>
-      <c r="N7" s="55">
+        <v>69.048000000000002</v>
+      </c>
+      <c r="N7" s="54">
         <f t="shared" si="4"/>
-        <v>84.000000000000014</v>
-      </c>
-      <c r="O7" s="55">
+        <v>92.063999999999993</v>
+      </c>
+      <c r="O7" s="54">
         <f t="shared" si="5"/>
-        <v>105.00000000000001</v>
-      </c>
-      <c r="P7" s="55">
+        <v>115.08</v>
+      </c>
+      <c r="P7" s="54">
         <f t="shared" si="6"/>
-        <v>126.00000000000001</v>
-      </c>
-      <c r="Q7" s="55">
+        <v>138.096</v>
+      </c>
+      <c r="Q7" s="54">
         <f t="shared" si="7"/>
-        <v>147</v>
-      </c>
-      <c r="R7" s="55">
+        <v>161.11199999999999</v>
+      </c>
+      <c r="R7" s="54">
         <f t="shared" si="8"/>
-        <v>168.00000000000003</v>
-      </c>
-      <c r="S7" s="55">
+        <v>184.12799999999999</v>
+      </c>
+      <c r="S7" s="54">
         <f t="shared" si="9"/>
-        <v>189.00000000000003</v>
-      </c>
-      <c r="T7" s="55">
+        <v>207.14400000000001</v>
+      </c>
+      <c r="T7" s="54">
         <f t="shared" si="10"/>
-        <v>210.00000000000003</v>
-      </c>
-      <c r="U7" s="56">
+        <v>230.16</v>
+      </c>
+      <c r="U7" s="55">
         <f t="shared" si="11"/>
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A8" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>72</v>
+        <v>253.17599999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>57</v>
       </c>
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="64">
         <v>96</v>
       </c>
-      <c r="E8" s="100">
+      <c r="E8" s="99">
         <f t="shared" si="12"/>
-        <v>110.39999999999999</v>
-      </c>
-      <c r="F8" s="100"/>
-      <c r="G8" s="93">
+        <v>133.44</v>
+      </c>
+      <c r="F8" s="99"/>
+      <c r="G8" s="92">
         <v>100</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="75">
         <f t="shared" si="13"/>
-        <v>210.39999999999998</v>
-      </c>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55">
+        <v>233.44</v>
+      </c>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54">
         <f t="shared" si="1"/>
-        <v>14.728</v>
-      </c>
-      <c r="L8" s="55">
+        <v>16.340800000000002</v>
+      </c>
+      <c r="L8" s="54">
         <f t="shared" si="2"/>
-        <v>29.456</v>
-      </c>
-      <c r="M8" s="55">
+        <v>32.681600000000003</v>
+      </c>
+      <c r="M8" s="54">
         <f t="shared" si="3"/>
-        <v>44.183999999999997</v>
-      </c>
-      <c r="N8" s="55">
+        <v>49.022400000000005</v>
+      </c>
+      <c r="N8" s="54">
         <f t="shared" si="4"/>
-        <v>58.911999999999999</v>
-      </c>
-      <c r="O8" s="55">
+        <v>65.363200000000006</v>
+      </c>
+      <c r="O8" s="54">
         <f t="shared" si="5"/>
-        <v>73.64</v>
-      </c>
-      <c r="P8" s="55">
+        <v>81.704000000000008</v>
+      </c>
+      <c r="P8" s="54">
         <f t="shared" si="6"/>
-        <v>88.367999999999995</v>
-      </c>
-      <c r="Q8" s="55">
+        <v>98.044800000000009</v>
+      </c>
+      <c r="Q8" s="54">
         <f t="shared" si="7"/>
-        <v>103.096</v>
-      </c>
-      <c r="R8" s="55">
+        <v>114.38560000000001</v>
+      </c>
+      <c r="R8" s="54">
         <f t="shared" si="8"/>
-        <v>117.824</v>
-      </c>
-      <c r="S8" s="55">
+        <v>130.72640000000001</v>
+      </c>
+      <c r="S8" s="54">
         <f t="shared" si="9"/>
-        <v>132.55200000000002</v>
-      </c>
-      <c r="T8" s="55">
+        <v>147.06720000000001</v>
+      </c>
+      <c r="T8" s="54">
         <f t="shared" si="10"/>
-        <v>147.28</v>
-      </c>
-      <c r="U8" s="56">
+        <v>163.40800000000002</v>
+      </c>
+      <c r="U8" s="55">
         <f t="shared" si="11"/>
-        <v>162.00799999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="54" t="s">
+        <v>179.74879999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="90">
+      <c r="B9" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="89">
         <v>25</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="64">
         <v>99</v>
       </c>
-      <c r="E9" s="100">
+      <c r="E9" s="99">
         <f t="shared" si="12"/>
-        <v>113.85</v>
-      </c>
-      <c r="F9" s="100"/>
-      <c r="G9" s="93">
+        <v>137.60999999999999</v>
+      </c>
+      <c r="F9" s="99"/>
+      <c r="G9" s="92">
         <v>250</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="76">
+      <c r="I9" s="75">
         <f t="shared" si="13"/>
-        <v>363.85</v>
-      </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55">
+        <v>387.61</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54">
         <f t="shared" si="1"/>
-        <v>25.469500000000004</v>
-      </c>
-      <c r="L9" s="55">
+        <v>27.132700000000003</v>
+      </c>
+      <c r="L9" s="54">
         <f t="shared" si="2"/>
-        <v>50.939000000000007</v>
-      </c>
-      <c r="M9" s="55">
+        <v>54.265400000000007</v>
+      </c>
+      <c r="M9" s="54">
         <f t="shared" si="3"/>
-        <v>76.408500000000018</v>
-      </c>
-      <c r="N9" s="55">
+        <v>81.398100000000014</v>
+      </c>
+      <c r="N9" s="54">
         <f t="shared" si="4"/>
-        <v>101.87800000000001</v>
-      </c>
-      <c r="O9" s="55">
+        <v>108.53080000000001</v>
+      </c>
+      <c r="O9" s="54">
         <f t="shared" si="5"/>
-        <v>127.34750000000003</v>
-      </c>
-      <c r="P9" s="55">
+        <v>135.66350000000003</v>
+      </c>
+      <c r="P9" s="54">
         <f t="shared" si="6"/>
-        <v>152.81700000000004</v>
-      </c>
-      <c r="Q9" s="55">
+        <v>162.79620000000003</v>
+      </c>
+      <c r="Q9" s="54">
         <f t="shared" si="7"/>
-        <v>178.28650000000002</v>
-      </c>
-      <c r="R9" s="55">
+        <v>189.92890000000003</v>
+      </c>
+      <c r="R9" s="54">
         <f t="shared" si="8"/>
-        <v>203.75600000000003</v>
-      </c>
-      <c r="S9" s="55">
+        <v>217.06160000000003</v>
+      </c>
+      <c r="S9" s="54">
         <f t="shared" si="9"/>
-        <v>229.22550000000007</v>
-      </c>
-      <c r="T9" s="55">
+        <v>244.19430000000006</v>
+      </c>
+      <c r="T9" s="54">
         <f t="shared" si="10"/>
-        <v>254.69500000000005</v>
-      </c>
-      <c r="U9" s="56">
+        <v>271.32700000000006</v>
+      </c>
+      <c r="U9" s="55">
         <f t="shared" si="11"/>
-        <v>280.16450000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+        <v>298.4597</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>74</v>
+      <c r="B10" s="50" t="s">
+        <v>59</v>
       </c>
       <c r="C10" s="6">
         <v>30</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="64">
         <v>95</v>
       </c>
-      <c r="E10" s="100">
+      <c r="E10" s="99">
         <f t="shared" si="12"/>
-        <v>109.24999999999999</v>
-      </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="93">
+        <v>132.04999999999998</v>
+      </c>
+      <c r="F10" s="99"/>
+      <c r="G10" s="92">
         <v>126</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="76">
+      <c r="I10" s="75">
         <f t="shared" si="13"/>
-        <v>235.25</v>
-      </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55">
+        <v>258.04999999999995</v>
+      </c>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54">
         <f t="shared" si="1"/>
-        <v>16.467500000000001</v>
-      </c>
-      <c r="L10" s="55">
+        <v>18.063499999999998</v>
+      </c>
+      <c r="L10" s="54">
         <f t="shared" si="2"/>
-        <v>32.935000000000002</v>
-      </c>
-      <c r="M10" s="55">
+        <v>36.126999999999995</v>
+      </c>
+      <c r="M10" s="54">
         <f t="shared" si="3"/>
-        <v>49.402500000000003</v>
-      </c>
-      <c r="N10" s="55">
+        <v>54.190499999999993</v>
+      </c>
+      <c r="N10" s="54">
         <f t="shared" si="4"/>
-        <v>65.87</v>
-      </c>
-      <c r="O10" s="55">
+        <v>72.253999999999991</v>
+      </c>
+      <c r="O10" s="54">
         <f t="shared" si="5"/>
-        <v>82.337500000000006</v>
-      </c>
-      <c r="P10" s="55">
+        <v>90.317499999999995</v>
+      </c>
+      <c r="P10" s="54">
         <f t="shared" si="6"/>
-        <v>98.805000000000007</v>
-      </c>
-      <c r="Q10" s="55">
+        <v>108.38099999999999</v>
+      </c>
+      <c r="Q10" s="54">
         <f t="shared" si="7"/>
-        <v>115.27250000000001</v>
-      </c>
-      <c r="R10" s="55">
+        <v>126.44449999999999</v>
+      </c>
+      <c r="R10" s="54">
         <f t="shared" si="8"/>
-        <v>131.74</v>
-      </c>
-      <c r="S10" s="55">
+        <v>144.50799999999998</v>
+      </c>
+      <c r="S10" s="54">
         <f t="shared" si="9"/>
-        <v>148.20750000000004</v>
-      </c>
-      <c r="T10" s="55">
+        <v>162.57150000000001</v>
+      </c>
+      <c r="T10" s="54">
         <f t="shared" si="10"/>
-        <v>164.67500000000001</v>
-      </c>
-      <c r="U10" s="56">
+        <v>180.63499999999999</v>
+      </c>
+      <c r="U10" s="55">
         <f t="shared" si="11"/>
-        <v>181.14250000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="54" t="s">
+        <v>198.69849999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>61</v>
+      <c r="B11" s="50" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="6">
         <v>30</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="64">
         <v>106</v>
       </c>
-      <c r="E11" s="100">
+      <c r="E11" s="99">
         <f t="shared" si="12"/>
-        <v>121.89999999999999</v>
-      </c>
-      <c r="F11" s="100"/>
-      <c r="G11" s="93">
+        <v>147.34</v>
+      </c>
+      <c r="F11" s="99"/>
+      <c r="G11" s="92">
         <v>118</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="75">
         <f t="shared" si="13"/>
-        <v>239.89999999999998</v>
-      </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55">
+        <v>265.34000000000003</v>
+      </c>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54">
         <f t="shared" si="1"/>
-        <v>16.792999999999999</v>
-      </c>
-      <c r="L11" s="55">
+        <v>18.573800000000006</v>
+      </c>
+      <c r="L11" s="54">
         <f t="shared" si="2"/>
-        <v>33.585999999999999</v>
-      </c>
-      <c r="M11" s="55">
+        <v>37.147600000000011</v>
+      </c>
+      <c r="M11" s="54">
         <f t="shared" si="3"/>
-        <v>50.378999999999998</v>
-      </c>
-      <c r="N11" s="55">
+        <v>55.72140000000001</v>
+      </c>
+      <c r="N11" s="54">
         <f t="shared" si="4"/>
-        <v>67.171999999999997</v>
-      </c>
-      <c r="O11" s="55">
+        <v>74.295200000000023</v>
+      </c>
+      <c r="O11" s="54">
         <f t="shared" si="5"/>
-        <v>83.965000000000003</v>
-      </c>
-      <c r="P11" s="55">
+        <v>92.869000000000014</v>
+      </c>
+      <c r="P11" s="54">
         <f t="shared" si="6"/>
-        <v>100.758</v>
-      </c>
-      <c r="Q11" s="55">
+        <v>111.44280000000002</v>
+      </c>
+      <c r="Q11" s="54">
         <f t="shared" si="7"/>
-        <v>117.551</v>
-      </c>
-      <c r="R11" s="55">
+        <v>130.01660000000004</v>
+      </c>
+      <c r="R11" s="54">
         <f t="shared" si="8"/>
-        <v>134.34399999999999</v>
-      </c>
-      <c r="S11" s="55">
+        <v>148.59040000000005</v>
+      </c>
+      <c r="S11" s="54">
         <f t="shared" si="9"/>
-        <v>151.137</v>
-      </c>
-      <c r="T11" s="55">
+        <v>167.16420000000005</v>
+      </c>
+      <c r="T11" s="54">
         <f t="shared" si="10"/>
-        <v>167.93</v>
-      </c>
-      <c r="U11" s="56">
+        <v>185.73800000000003</v>
+      </c>
+      <c r="U11" s="55">
         <f t="shared" si="11"/>
-        <v>184.72299999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>60</v>
+        <v>204.31180000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>45</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="65">
+      <c r="D12" s="64">
         <v>111</v>
       </c>
-      <c r="E12" s="100">
+      <c r="E12" s="99">
         <f t="shared" si="12"/>
-        <v>127.64999999999999</v>
-      </c>
-      <c r="F12" s="100"/>
-      <c r="G12" s="93">
+        <v>154.29</v>
+      </c>
+      <c r="F12" s="99"/>
+      <c r="G12" s="92">
         <v>118</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="76">
+      <c r="I12" s="75">
         <f t="shared" si="13"/>
-        <v>245.64999999999998</v>
-      </c>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55">
+        <v>272.28999999999996</v>
+      </c>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54">
         <f t="shared" si="1"/>
-        <v>17.195499999999999</v>
-      </c>
-      <c r="L12" s="55">
+        <v>19.060299999999998</v>
+      </c>
+      <c r="L12" s="54">
         <f t="shared" si="2"/>
-        <v>34.390999999999998</v>
-      </c>
-      <c r="M12" s="55">
+        <v>38.120599999999996</v>
+      </c>
+      <c r="M12" s="54">
         <f t="shared" si="3"/>
-        <v>51.586500000000001</v>
-      </c>
-      <c r="N12" s="55">
+        <v>57.180900000000001</v>
+      </c>
+      <c r="N12" s="54">
         <f t="shared" si="4"/>
-        <v>68.781999999999996</v>
-      </c>
-      <c r="O12" s="55">
+        <v>76.241199999999992</v>
+      </c>
+      <c r="O12" s="54">
         <f t="shared" si="5"/>
-        <v>85.977500000000006</v>
-      </c>
-      <c r="P12" s="55">
+        <v>95.30149999999999</v>
+      </c>
+      <c r="P12" s="54">
         <f t="shared" si="6"/>
-        <v>103.173</v>
-      </c>
-      <c r="Q12" s="55">
+        <v>114.3618</v>
+      </c>
+      <c r="Q12" s="54">
         <f t="shared" si="7"/>
-        <v>120.3685</v>
-      </c>
-      <c r="R12" s="55">
+        <v>133.4221</v>
+      </c>
+      <c r="R12" s="54">
         <f t="shared" si="8"/>
-        <v>137.56399999999999</v>
-      </c>
-      <c r="S12" s="55">
+        <v>152.48239999999998</v>
+      </c>
+      <c r="S12" s="54">
         <f t="shared" si="9"/>
-        <v>154.7595</v>
-      </c>
-      <c r="T12" s="55">
+        <v>171.5427</v>
+      </c>
+      <c r="T12" s="54">
         <f t="shared" si="10"/>
-        <v>171.95500000000001</v>
-      </c>
-      <c r="U12" s="56">
+        <v>190.60299999999998</v>
+      </c>
+      <c r="U12" s="55">
         <f t="shared" si="11"/>
-        <v>189.15049999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="54" t="s">
+        <v>209.66329999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="51" t="s">
-        <v>63</v>
+      <c r="B13" s="50" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="6">
         <v>30</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="64">
         <v>111</v>
       </c>
-      <c r="E13" s="100">
+      <c r="E13" s="99">
         <f t="shared" si="12"/>
-        <v>127.64999999999999</v>
-      </c>
-      <c r="F13" s="100"/>
-      <c r="G13" s="93">
+        <v>154.29</v>
+      </c>
+      <c r="F13" s="99"/>
+      <c r="G13" s="92">
         <v>128</v>
       </c>
-      <c r="H13" s="66">
+      <c r="H13" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="76">
+      <c r="I13" s="75">
         <f t="shared" si="13"/>
-        <v>255.64999999999998</v>
-      </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55">
+        <v>282.28999999999996</v>
+      </c>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54">
         <f t="shared" si="1"/>
-        <v>17.895499999999998</v>
-      </c>
-      <c r="L13" s="55">
+        <v>19.760300000000001</v>
+      </c>
+      <c r="L13" s="54">
         <f t="shared" si="2"/>
-        <v>35.790999999999997</v>
-      </c>
-      <c r="M13" s="55">
+        <v>39.520600000000002</v>
+      </c>
+      <c r="M13" s="54">
         <f t="shared" si="3"/>
-        <v>53.686500000000002</v>
-      </c>
-      <c r="N13" s="55">
+        <v>59.280899999999995</v>
+      </c>
+      <c r="N13" s="54">
         <f t="shared" si="4"/>
-        <v>71.581999999999994</v>
-      </c>
-      <c r="O13" s="55">
+        <v>79.041200000000003</v>
+      </c>
+      <c r="O13" s="54">
         <f t="shared" si="5"/>
-        <v>89.477500000000006</v>
-      </c>
-      <c r="P13" s="55">
+        <v>98.80149999999999</v>
+      </c>
+      <c r="P13" s="54">
         <f t="shared" si="6"/>
-        <v>107.373</v>
-      </c>
-      <c r="Q13" s="55">
+        <v>118.56179999999999</v>
+      </c>
+      <c r="Q13" s="54">
         <f t="shared" si="7"/>
-        <v>125.2685</v>
-      </c>
-      <c r="R13" s="55">
+        <v>138.32210000000001</v>
+      </c>
+      <c r="R13" s="54">
         <f t="shared" si="8"/>
-        <v>143.16399999999999</v>
-      </c>
-      <c r="S13" s="55">
+        <v>158.08240000000001</v>
+      </c>
+      <c r="S13" s="54">
         <f t="shared" si="9"/>
-        <v>161.05950000000001</v>
-      </c>
-      <c r="T13" s="55">
+        <v>177.84270000000001</v>
+      </c>
+      <c r="T13" s="54">
         <f t="shared" si="10"/>
-        <v>178.95500000000001</v>
-      </c>
-      <c r="U13" s="56">
+        <v>197.60299999999998</v>
+      </c>
+      <c r="U13" s="55">
         <f t="shared" si="11"/>
-        <v>196.85049999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="54" t="s">
+        <v>217.36329999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="51" t="s">
-        <v>53</v>
+      <c r="B14" s="50" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="6">
         <v>30</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="64">
         <v>110</v>
       </c>
-      <c r="E14" s="100">
+      <c r="E14" s="99">
         <f t="shared" si="12"/>
-        <v>126.49999999999999</v>
-      </c>
-      <c r="F14" s="100"/>
-      <c r="G14" s="93">
+        <v>152.89999999999998</v>
+      </c>
+      <c r="F14" s="99"/>
+      <c r="G14" s="92">
         <v>131</v>
       </c>
-      <c r="H14" s="66">
+      <c r="H14" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="75">
         <f t="shared" si="13"/>
-        <v>257.5</v>
-      </c>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55">
+        <v>283.89999999999998</v>
+      </c>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54">
         <f t="shared" si="1"/>
-        <v>18.025000000000002</v>
-      </c>
-      <c r="L14" s="55">
+        <v>19.873000000000001</v>
+      </c>
+      <c r="L14" s="54">
         <f t="shared" si="2"/>
-        <v>36.050000000000004</v>
-      </c>
-      <c r="M14" s="55">
+        <v>39.746000000000002</v>
+      </c>
+      <c r="M14" s="54">
         <f t="shared" si="3"/>
-        <v>54.075000000000003</v>
-      </c>
-      <c r="N14" s="55">
+        <v>59.619</v>
+      </c>
+      <c r="N14" s="54">
         <f t="shared" si="4"/>
-        <v>72.100000000000009</v>
-      </c>
-      <c r="O14" s="55">
+        <v>79.492000000000004</v>
+      </c>
+      <c r="O14" s="54">
         <f t="shared" si="5"/>
-        <v>90.125000000000014</v>
-      </c>
-      <c r="P14" s="55">
+        <v>99.364999999999995</v>
+      </c>
+      <c r="P14" s="54">
         <f t="shared" si="6"/>
-        <v>108.15</v>
-      </c>
-      <c r="Q14" s="55">
+        <v>119.238</v>
+      </c>
+      <c r="Q14" s="54">
         <f t="shared" si="7"/>
-        <v>126.17500000000001</v>
-      </c>
-      <c r="R14" s="55">
+        <v>139.11099999999999</v>
+      </c>
+      <c r="R14" s="54">
         <f t="shared" si="8"/>
-        <v>144.20000000000002</v>
-      </c>
-      <c r="S14" s="55">
+        <v>158.98400000000001</v>
+      </c>
+      <c r="S14" s="54">
         <f t="shared" si="9"/>
-        <v>162.22500000000002</v>
-      </c>
-      <c r="T14" s="55">
+        <v>178.85700000000003</v>
+      </c>
+      <c r="T14" s="54">
         <f t="shared" si="10"/>
-        <v>180.25000000000003</v>
-      </c>
-      <c r="U14" s="56">
+        <v>198.73</v>
+      </c>
+      <c r="U14" s="55">
         <f t="shared" si="11"/>
-        <v>198.27500000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="54" t="s">
+        <v>218.60299999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="51" t="s">
-        <v>59</v>
+      <c r="B15" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="65">
+      <c r="D15" s="64">
         <v>99</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="99">
         <f t="shared" si="12"/>
-        <v>113.85</v>
-      </c>
-      <c r="F15" s="100"/>
-      <c r="G15" s="93">
+        <v>137.60999999999999</v>
+      </c>
+      <c r="F15" s="99"/>
+      <c r="G15" s="92">
         <v>100</v>
       </c>
-      <c r="H15" s="66">
+      <c r="H15" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="76">
+      <c r="I15" s="75">
         <f t="shared" si="13"/>
-        <v>213.85</v>
-      </c>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55">
+        <v>237.60999999999999</v>
+      </c>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54">
         <f t="shared" si="1"/>
-        <v>14.969500000000002</v>
-      </c>
-      <c r="L15" s="55">
+        <v>16.6327</v>
+      </c>
+      <c r="L15" s="54">
         <f t="shared" si="2"/>
-        <v>29.939000000000004</v>
-      </c>
-      <c r="M15" s="55">
+        <v>33.2654</v>
+      </c>
+      <c r="M15" s="54">
         <f t="shared" si="3"/>
-        <v>44.908500000000004</v>
-      </c>
-      <c r="N15" s="55">
+        <v>49.898099999999999</v>
+      </c>
+      <c r="N15" s="54">
         <f t="shared" si="4"/>
-        <v>59.878000000000007</v>
-      </c>
-      <c r="O15" s="55">
+        <v>66.530799999999999</v>
+      </c>
+      <c r="O15" s="54">
         <f t="shared" si="5"/>
-        <v>74.847500000000011</v>
-      </c>
-      <c r="P15" s="55">
+        <v>83.163499999999999</v>
+      </c>
+      <c r="P15" s="54">
         <f t="shared" si="6"/>
-        <v>89.817000000000007</v>
-      </c>
-      <c r="Q15" s="55">
+        <v>99.796199999999999</v>
+      </c>
+      <c r="Q15" s="54">
         <f t="shared" si="7"/>
-        <v>104.7865</v>
-      </c>
-      <c r="R15" s="55">
+        <v>116.4289</v>
+      </c>
+      <c r="R15" s="54">
         <f t="shared" si="8"/>
-        <v>119.75600000000001</v>
-      </c>
-      <c r="S15" s="55">
+        <v>133.0616</v>
+      </c>
+      <c r="S15" s="54">
         <f t="shared" si="9"/>
-        <v>134.72550000000001</v>
-      </c>
-      <c r="T15" s="55">
+        <v>149.69430000000003</v>
+      </c>
+      <c r="T15" s="54">
         <f t="shared" si="10"/>
-        <v>149.69500000000002</v>
-      </c>
-      <c r="U15" s="56">
+        <v>166.327</v>
+      </c>
+      <c r="U15" s="55">
         <f t="shared" si="11"/>
-        <v>164.6645</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" s="54" t="s">
+        <v>182.9597</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="90">
+      <c r="B16" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="89">
         <v>50</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="64">
         <v>108</v>
       </c>
-      <c r="E16" s="100">
+      <c r="E16" s="99">
         <f t="shared" si="12"/>
-        <v>124.19999999999999</v>
-      </c>
-      <c r="F16" s="100"/>
-      <c r="G16" s="93">
+        <v>150.11999999999998</v>
+      </c>
+      <c r="F16" s="99"/>
+      <c r="G16" s="92">
         <v>100</v>
       </c>
-      <c r="H16" s="66">
+      <c r="H16" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="76">
+      <c r="I16" s="75">
         <f t="shared" si="13"/>
-        <v>224.2</v>
-      </c>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55">
+        <v>250.11999999999998</v>
+      </c>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54">
         <f t="shared" si="1"/>
-        <v>15.694000000000001</v>
-      </c>
-      <c r="L16" s="55">
+        <v>17.508400000000002</v>
+      </c>
+      <c r="L16" s="54">
         <f t="shared" si="2"/>
-        <v>31.388000000000002</v>
-      </c>
-      <c r="M16" s="55">
+        <v>35.016800000000003</v>
+      </c>
+      <c r="M16" s="54">
         <f t="shared" si="3"/>
-        <v>47.082000000000001</v>
-      </c>
-      <c r="N16" s="55">
+        <v>52.525199999999998</v>
+      </c>
+      <c r="N16" s="54">
         <f t="shared" si="4"/>
-        <v>62.776000000000003</v>
-      </c>
-      <c r="O16" s="55">
+        <v>70.033600000000007</v>
+      </c>
+      <c r="O16" s="54">
         <f t="shared" si="5"/>
-        <v>78.47</v>
-      </c>
-      <c r="P16" s="55">
+        <v>87.542000000000002</v>
+      </c>
+      <c r="P16" s="54">
         <f t="shared" si="6"/>
-        <v>94.164000000000001</v>
-      </c>
-      <c r="Q16" s="55">
+        <v>105.0504</v>
+      </c>
+      <c r="Q16" s="54">
         <f t="shared" si="7"/>
-        <v>109.858</v>
-      </c>
-      <c r="R16" s="55">
+        <v>122.55880000000001</v>
+      </c>
+      <c r="R16" s="54">
         <f t="shared" si="8"/>
-        <v>125.55200000000001</v>
-      </c>
-      <c r="S16" s="55">
+        <v>140.06720000000001</v>
+      </c>
+      <c r="S16" s="54">
         <f t="shared" si="9"/>
-        <v>141.24600000000001</v>
-      </c>
-      <c r="T16" s="55">
+        <v>157.57560000000001</v>
+      </c>
+      <c r="T16" s="54">
         <f t="shared" si="10"/>
-        <v>156.94</v>
-      </c>
-      <c r="U16" s="56">
+        <v>175.084</v>
+      </c>
+      <c r="U16" s="55">
         <f t="shared" si="11"/>
-        <v>172.63399999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A17" s="54" t="s">
+        <v>192.5924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="90">
+      <c r="B17" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="89">
         <v>20</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="64">
         <v>105</v>
       </c>
-      <c r="E17" s="100">
+      <c r="E17" s="99">
         <f t="shared" si="12"/>
-        <v>120.74999999999999</v>
-      </c>
-      <c r="F17" s="100"/>
-      <c r="G17" s="93">
+        <v>145.94999999999999</v>
+      </c>
+      <c r="F17" s="99"/>
+      <c r="G17" s="92">
         <v>122</v>
       </c>
-      <c r="H17" s="66">
+      <c r="H17" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="75">
         <f t="shared" si="13"/>
-        <v>242.75</v>
-      </c>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55">
+        <v>267.95</v>
+      </c>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54">
         <f t="shared" si="1"/>
-        <v>16.992500000000003</v>
-      </c>
-      <c r="L17" s="55">
+        <v>18.756500000000003</v>
+      </c>
+      <c r="L17" s="54">
         <f t="shared" si="2"/>
-        <v>33.985000000000007</v>
-      </c>
-      <c r="M17" s="55">
+        <v>37.513000000000005</v>
+      </c>
+      <c r="M17" s="54">
         <f t="shared" si="3"/>
-        <v>50.977500000000006</v>
-      </c>
-      <c r="N17" s="55">
+        <v>56.269500000000001</v>
+      </c>
+      <c r="N17" s="54">
         <f t="shared" si="4"/>
-        <v>67.970000000000013</v>
-      </c>
-      <c r="O17" s="55">
+        <v>75.02600000000001</v>
+      </c>
+      <c r="O17" s="54">
         <f t="shared" si="5"/>
-        <v>84.962500000000006</v>
-      </c>
-      <c r="P17" s="55">
+        <v>93.782499999999999</v>
+      </c>
+      <c r="P17" s="54">
         <f t="shared" si="6"/>
-        <v>101.95500000000001</v>
-      </c>
-      <c r="Q17" s="55">
+        <v>112.539</v>
+      </c>
+      <c r="Q17" s="54">
         <f t="shared" si="7"/>
-        <v>118.94750000000001</v>
-      </c>
-      <c r="R17" s="55">
+        <v>131.2955</v>
+      </c>
+      <c r="R17" s="54">
         <f t="shared" si="8"/>
-        <v>135.94000000000003</v>
-      </c>
-      <c r="S17" s="55">
+        <v>150.05200000000002</v>
+      </c>
+      <c r="S17" s="54">
         <f t="shared" si="9"/>
-        <v>152.93250000000003</v>
-      </c>
-      <c r="T17" s="55">
+        <v>168.80850000000004</v>
+      </c>
+      <c r="T17" s="54">
         <f t="shared" si="10"/>
-        <v>169.92500000000001</v>
-      </c>
-      <c r="U17" s="56">
+        <v>187.565</v>
+      </c>
+      <c r="U17" s="55">
         <f t="shared" si="11"/>
-        <v>186.91750000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+        <v>206.32149999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="90">
+      <c r="B18" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="89">
         <v>20</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="64">
         <v>97</v>
       </c>
-      <c r="E18" s="100">
+      <c r="E18" s="99">
         <f t="shared" si="12"/>
-        <v>111.55</v>
-      </c>
-      <c r="F18" s="100"/>
-      <c r="G18" s="93">
+        <v>134.82999999999998</v>
+      </c>
+      <c r="F18" s="99"/>
+      <c r="G18" s="92">
         <v>88</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="76">
+      <c r="I18" s="75">
         <f t="shared" si="13"/>
-        <v>199.55</v>
-      </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55">
+        <v>222.82999999999998</v>
+      </c>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54">
         <f t="shared" si="1"/>
-        <v>13.968500000000002</v>
-      </c>
-      <c r="L18" s="55">
+        <v>15.598100000000001</v>
+      </c>
+      <c r="L18" s="54">
         <f t="shared" si="2"/>
-        <v>27.937000000000005</v>
-      </c>
-      <c r="M18" s="55">
+        <v>31.196200000000001</v>
+      </c>
+      <c r="M18" s="54">
         <f t="shared" si="3"/>
-        <v>41.905500000000004</v>
-      </c>
-      <c r="N18" s="55">
+        <v>46.7943</v>
+      </c>
+      <c r="N18" s="54">
         <f t="shared" si="4"/>
-        <v>55.874000000000009</v>
-      </c>
-      <c r="O18" s="55">
+        <v>62.392400000000002</v>
+      </c>
+      <c r="O18" s="54">
         <f t="shared" si="5"/>
-        <v>69.842500000000015</v>
-      </c>
-      <c r="P18" s="55">
+        <v>77.990499999999997</v>
+      </c>
+      <c r="P18" s="54">
         <f t="shared" si="6"/>
-        <v>83.811000000000007</v>
-      </c>
-      <c r="Q18" s="55">
+        <v>93.5886</v>
+      </c>
+      <c r="Q18" s="54">
         <f t="shared" si="7"/>
-        <v>97.779500000000013</v>
-      </c>
-      <c r="R18" s="55">
+        <v>109.1867</v>
+      </c>
+      <c r="R18" s="54">
         <f t="shared" si="8"/>
-        <v>111.74800000000002</v>
-      </c>
-      <c r="S18" s="55">
+        <v>124.7848</v>
+      </c>
+      <c r="S18" s="54">
         <f t="shared" si="9"/>
-        <v>125.71650000000002</v>
-      </c>
-      <c r="T18" s="55">
+        <v>140.38290000000001</v>
+      </c>
+      <c r="T18" s="54">
         <f t="shared" si="10"/>
-        <v>139.68500000000003</v>
-      </c>
-      <c r="U18" s="56">
+        <v>155.98099999999999</v>
+      </c>
+      <c r="U18" s="55">
         <f t="shared" si="11"/>
-        <v>153.65350000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="54" t="s">
+        <v>171.57909999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>50</v>
+      <c r="B19" s="50" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="6">
         <v>30</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="64">
         <v>106</v>
       </c>
-      <c r="E19" s="100">
+      <c r="E19" s="99">
         <f t="shared" si="12"/>
-        <v>121.89999999999999</v>
-      </c>
-      <c r="F19" s="100"/>
-      <c r="G19" s="93">
+        <v>147.34</v>
+      </c>
+      <c r="F19" s="99"/>
+      <c r="G19" s="92">
         <v>85</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="76">
+      <c r="I19" s="75">
         <f t="shared" si="13"/>
-        <v>206.89999999999998</v>
-      </c>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55">
+        <v>232.34</v>
+      </c>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54">
         <f t="shared" si="1"/>
-        <v>14.483000000000001</v>
-      </c>
-      <c r="L19" s="55">
+        <v>16.263800000000003</v>
+      </c>
+      <c r="L19" s="54">
         <f t="shared" si="2"/>
-        <v>28.966000000000001</v>
-      </c>
-      <c r="M19" s="55">
+        <v>32.527600000000007</v>
+      </c>
+      <c r="M19" s="54">
         <f t="shared" si="3"/>
-        <v>43.448999999999998</v>
-      </c>
-      <c r="N19" s="55">
+        <v>48.791400000000003</v>
+      </c>
+      <c r="N19" s="54">
         <f t="shared" si="4"/>
-        <v>57.932000000000002</v>
-      </c>
-      <c r="O19" s="55">
+        <v>65.055200000000013</v>
+      </c>
+      <c r="O19" s="54">
         <f t="shared" si="5"/>
-        <v>72.414999999999992</v>
-      </c>
-      <c r="P19" s="55">
+        <v>81.319000000000003</v>
+      </c>
+      <c r="P19" s="54">
         <f t="shared" si="6"/>
-        <v>86.897999999999996</v>
-      </c>
-      <c r="Q19" s="55">
+        <v>97.582800000000006</v>
+      </c>
+      <c r="Q19" s="54">
         <f t="shared" si="7"/>
-        <v>101.381</v>
-      </c>
-      <c r="R19" s="55">
+        <v>113.84660000000001</v>
+      </c>
+      <c r="R19" s="54">
         <f t="shared" si="8"/>
-        <v>115.864</v>
-      </c>
-      <c r="S19" s="55">
+        <v>130.11040000000003</v>
+      </c>
+      <c r="S19" s="54">
         <f t="shared" si="9"/>
-        <v>130.34700000000001</v>
-      </c>
-      <c r="T19" s="55">
+        <v>146.37420000000003</v>
+      </c>
+      <c r="T19" s="54">
         <f t="shared" si="10"/>
-        <v>144.82999999999998</v>
-      </c>
-      <c r="U19" s="56">
+        <v>162.63800000000001</v>
+      </c>
+      <c r="U19" s="55">
         <f t="shared" si="11"/>
-        <v>159.31299999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="51" t="s">
-        <v>58</v>
+        <v>178.90180000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>43</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="65">
+      <c r="D20" s="64">
         <v>98</v>
       </c>
-      <c r="E20" s="100">
+      <c r="E20" s="99">
         <f t="shared" si="12"/>
-        <v>112.69999999999999</v>
-      </c>
-      <c r="F20" s="100"/>
-      <c r="G20" s="93">
+        <v>136.22</v>
+      </c>
+      <c r="F20" s="99"/>
+      <c r="G20" s="92">
         <v>85</v>
       </c>
-      <c r="H20" s="66">
+      <c r="H20" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="76">
+      <c r="I20" s="75">
         <f t="shared" si="13"/>
-        <v>197.7</v>
-      </c>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55">
+        <v>221.22</v>
+      </c>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54">
         <f t="shared" si="1"/>
-        <v>13.839</v>
-      </c>
-      <c r="L20" s="55">
+        <v>15.485400000000002</v>
+      </c>
+      <c r="L20" s="54">
         <f t="shared" si="2"/>
-        <v>27.678000000000001</v>
-      </c>
-      <c r="M20" s="55">
+        <v>30.970800000000004</v>
+      </c>
+      <c r="M20" s="54">
         <f t="shared" si="3"/>
-        <v>41.517000000000003</v>
-      </c>
-      <c r="N20" s="55">
+        <v>46.456200000000003</v>
+      </c>
+      <c r="N20" s="54">
         <f t="shared" si="4"/>
-        <v>55.356000000000002</v>
-      </c>
-      <c r="O20" s="55">
+        <v>61.941600000000008</v>
+      </c>
+      <c r="O20" s="54">
         <f t="shared" si="5"/>
-        <v>69.195000000000007</v>
-      </c>
-      <c r="P20" s="55">
+        <v>77.427000000000007</v>
+      </c>
+      <c r="P20" s="54">
         <f t="shared" si="6"/>
-        <v>83.034000000000006</v>
-      </c>
-      <c r="Q20" s="55">
+        <v>92.912400000000005</v>
+      </c>
+      <c r="Q20" s="54">
         <f t="shared" si="7"/>
-        <v>96.873000000000005</v>
-      </c>
-      <c r="R20" s="55">
+        <v>108.3978</v>
+      </c>
+      <c r="R20" s="54">
         <f t="shared" si="8"/>
-        <v>110.712</v>
-      </c>
-      <c r="S20" s="55">
+        <v>123.88320000000002</v>
+      </c>
+      <c r="S20" s="54">
         <f t="shared" si="9"/>
-        <v>124.55100000000002</v>
-      </c>
-      <c r="T20" s="55">
+        <v>139.36860000000001</v>
+      </c>
+      <c r="T20" s="54">
         <f t="shared" si="10"/>
-        <v>138.39000000000001</v>
-      </c>
-      <c r="U20" s="56">
+        <v>154.85400000000001</v>
+      </c>
+      <c r="U20" s="55">
         <f t="shared" si="11"/>
-        <v>152.22899999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="77" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="80">
+        <v>170.33940000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="78"/>
+      <c r="D21" s="79">
         <v>87</v>
       </c>
-      <c r="E21" s="101">
+      <c r="E21" s="100">
         <f t="shared" si="12"/>
-        <v>100.05</v>
-      </c>
-      <c r="F21" s="101"/>
-      <c r="G21" s="94">
+        <v>120.92999999999999</v>
+      </c>
+      <c r="F21" s="100"/>
+      <c r="G21" s="93">
         <v>0</v>
       </c>
-      <c r="H21" s="81">
+      <c r="H21" s="80">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="82">
+      <c r="I21" s="81">
         <f t="shared" si="13"/>
-        <v>100.05</v>
-      </c>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57">
+        <v>120.92999999999999</v>
+      </c>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56">
         <f t="shared" si="1"/>
-        <v>7.0035000000000007</v>
-      </c>
-      <c r="L21" s="57">
+        <v>8.4650999999999996</v>
+      </c>
+      <c r="L21" s="56">
         <f t="shared" si="2"/>
-        <v>14.007000000000001</v>
-      </c>
-      <c r="M21" s="57">
+        <v>16.930199999999999</v>
+      </c>
+      <c r="M21" s="56">
         <f t="shared" si="3"/>
-        <v>21.0105</v>
-      </c>
-      <c r="N21" s="57">
+        <v>25.395300000000002</v>
+      </c>
+      <c r="N21" s="56">
         <f t="shared" si="4"/>
-        <v>28.014000000000003</v>
-      </c>
-      <c r="O21" s="57">
+        <v>33.860399999999998</v>
+      </c>
+      <c r="O21" s="56">
         <f t="shared" si="5"/>
-        <v>35.017500000000005</v>
-      </c>
-      <c r="P21" s="57">
+        <v>42.325499999999998</v>
+      </c>
+      <c r="P21" s="56">
         <f t="shared" si="6"/>
-        <v>42.021000000000001</v>
-      </c>
-      <c r="Q21" s="57">
+        <v>50.790600000000005</v>
+      </c>
+      <c r="Q21" s="56">
         <f t="shared" si="7"/>
-        <v>49.024500000000003</v>
-      </c>
-      <c r="R21" s="57">
+        <v>59.255700000000004</v>
+      </c>
+      <c r="R21" s="56">
         <f t="shared" si="8"/>
-        <v>56.028000000000006</v>
-      </c>
-      <c r="S21" s="57">
+        <v>67.720799999999997</v>
+      </c>
+      <c r="S21" s="56">
         <f t="shared" si="9"/>
-        <v>63.031500000000008</v>
-      </c>
-      <c r="T21" s="57">
+        <v>76.185900000000004</v>
+      </c>
+      <c r="T21" s="56">
         <f t="shared" si="10"/>
-        <v>70.035000000000011</v>
-      </c>
-      <c r="U21" s="58">
+        <v>84.650999999999996</v>
+      </c>
+      <c r="U21" s="57">
         <f t="shared" si="11"/>
-        <v>77.038499999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="1:21" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
+        <v>93.116100000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:21" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B24" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="47"/>
+        <v>29</v>
+      </c>
+      <c r="C24" s="46"/>
       <c r="D24" s="36"/>
       <c r="E24" s="36"/>
       <c r="F24" s="36"/>
       <c r="G24" s="37"/>
       <c r="H24" s="20"/>
       <c r="I24" s="30" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="16"/>
@@ -2743,7 +2690,7 @@
       <c r="T24" s="16"/>
       <c r="U24" s="17"/>
     </row>
-    <row r="25" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
         <v>14</v>
       </c>
@@ -2800,11 +2747,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="47"/>
       <c r="D26" s="14">
         <v>0.15</v>
       </c>
@@ -2822,52 +2769,52 @@
         <v>1429</v>
       </c>
       <c r="J26" s="25"/>
-      <c r="K26" s="96">
+      <c r="K26" s="95">
         <f>SUM($I26*(0.07*1))</f>
         <v>100.03000000000002</v>
       </c>
-      <c r="L26" s="59">
+      <c r="L26" s="58">
         <f>SUM($I26*(0.07*2))</f>
         <v>200.06000000000003</v>
       </c>
-      <c r="M26" s="59">
+      <c r="M26" s="58">
         <f>SUM($I26*(0.07*3))</f>
         <v>300.09000000000003</v>
       </c>
-      <c r="N26" s="59">
+      <c r="N26" s="58">
         <f>SUM($I26*(0.07*4))</f>
         <v>400.12000000000006</v>
       </c>
-      <c r="O26" s="59">
+      <c r="O26" s="58">
         <f>SUM($I26*(0.07*5))</f>
         <v>500.15000000000003</v>
       </c>
-      <c r="P26" s="59">
+      <c r="P26" s="58">
         <f>SUM($I26*(0.07*6))</f>
         <v>600.18000000000006</v>
       </c>
-      <c r="Q26" s="59">
+      <c r="Q26" s="58">
         <f>SUM($I26*(0.07*7))</f>
         <v>700.21</v>
       </c>
-      <c r="R26" s="59">
+      <c r="R26" s="58">
         <f>SUM($I26*(0.07*8))</f>
         <v>800.24000000000012</v>
       </c>
-      <c r="S26" s="59">
+      <c r="S26" s="58">
         <f>SUM($I26*(0.07*9))</f>
         <v>900.27000000000021</v>
       </c>
-      <c r="T26" s="59">
+      <c r="T26" s="58">
         <f>SUM($I26*(0.07*10))</f>
         <v>1000.3000000000001</v>
       </c>
-      <c r="U26" s="60">
+      <c r="U26" s="59">
         <f>SUM($I26*(0.07*11))</f>
         <v>1100.33</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="8"/>
@@ -2876,376 +2823,376 @@
         <v>715</v>
       </c>
       <c r="J27" s="25"/>
-      <c r="K27" s="59">
+      <c r="K27" s="58">
         <f t="shared" ref="K27:K53" si="14">SUM($I27*(0.07*1))</f>
         <v>50.050000000000004</v>
       </c>
-      <c r="L27" s="96">
+      <c r="L27" s="95">
         <f t="shared" ref="L27:L53" si="15">SUM($I27*(0.07*2))</f>
         <v>100.10000000000001</v>
       </c>
-      <c r="M27" s="59">
+      <c r="M27" s="58">
         <f t="shared" ref="M27:M53" si="16">SUM($I27*(0.07*3))</f>
         <v>150.15</v>
       </c>
-      <c r="N27" s="59">
+      <c r="N27" s="58">
         <f t="shared" ref="N27:N53" si="17">SUM($I27*(0.07*4))</f>
         <v>200.20000000000002</v>
       </c>
-      <c r="O27" s="59">
+      <c r="O27" s="58">
         <f t="shared" ref="O27:O53" si="18">SUM($I27*(0.07*5))</f>
         <v>250.25000000000003</v>
       </c>
-      <c r="P27" s="59">
+      <c r="P27" s="58">
         <f t="shared" ref="P27:P53" si="19">SUM($I27*(0.07*6))</f>
         <v>300.3</v>
       </c>
-      <c r="Q27" s="59">
+      <c r="Q27" s="58">
         <f t="shared" ref="Q27:Q53" si="20">SUM($I27*(0.07*7))</f>
         <v>350.35</v>
       </c>
-      <c r="R27" s="59">
+      <c r="R27" s="58">
         <f t="shared" ref="R27:R53" si="21">SUM($I27*(0.07*8))</f>
         <v>400.40000000000003</v>
       </c>
-      <c r="S27" s="59">
+      <c r="S27" s="58">
         <f t="shared" ref="S27:S53" si="22">SUM($I27*(0.07*9))</f>
         <v>450.4500000000001</v>
       </c>
-      <c r="T27" s="59">
+      <c r="T27" s="58">
         <f t="shared" ref="T27:T53" si="23">SUM($I27*(0.07*10))</f>
         <v>500.50000000000006</v>
       </c>
-      <c r="U27" s="60">
+      <c r="U27" s="59">
         <f t="shared" ref="U27:U53" si="24">SUM($I27*(0.07*11))</f>
         <v>550.55000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I28" s="24">
         <v>477</v>
       </c>
       <c r="J28" s="25"/>
-      <c r="K28" s="59">
+      <c r="K28" s="58">
         <f t="shared" si="14"/>
         <v>33.39</v>
       </c>
-      <c r="L28" s="59">
+      <c r="L28" s="58">
         <f t="shared" si="15"/>
         <v>66.78</v>
       </c>
-      <c r="M28" s="96">
+      <c r="M28" s="95">
         <f t="shared" si="16"/>
         <v>100.17000000000002</v>
       </c>
-      <c r="N28" s="59">
+      <c r="N28" s="58">
         <f t="shared" si="17"/>
         <v>133.56</v>
       </c>
-      <c r="O28" s="59">
+      <c r="O28" s="58">
         <f t="shared" si="18"/>
         <v>166.95000000000002</v>
       </c>
-      <c r="P28" s="59">
+      <c r="P28" s="58">
         <f t="shared" si="19"/>
         <v>200.34000000000003</v>
       </c>
-      <c r="Q28" s="59">
+      <c r="Q28" s="58">
         <f t="shared" si="20"/>
         <v>233.73000000000002</v>
       </c>
-      <c r="R28" s="59">
+      <c r="R28" s="58">
         <f t="shared" si="21"/>
         <v>267.12</v>
       </c>
-      <c r="S28" s="59">
+      <c r="S28" s="58">
         <f t="shared" si="22"/>
         <v>300.51000000000005</v>
       </c>
-      <c r="T28" s="59">
+      <c r="T28" s="58">
         <f t="shared" si="23"/>
         <v>333.90000000000003</v>
       </c>
-      <c r="U28" s="60">
+      <c r="U28" s="59">
         <f t="shared" si="24"/>
         <v>367.29</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:21" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="36"/>
       <c r="E29" s="37"/>
       <c r="I29" s="24">
         <v>358</v>
       </c>
       <c r="J29" s="25"/>
-      <c r="K29" s="59">
+      <c r="K29" s="58">
         <f t="shared" si="14"/>
         <v>25.060000000000002</v>
       </c>
-      <c r="L29" s="59">
+      <c r="L29" s="58">
         <f t="shared" si="15"/>
         <v>50.120000000000005</v>
       </c>
-      <c r="M29" s="59">
+      <c r="M29" s="58">
         <f t="shared" si="16"/>
         <v>75.180000000000007</v>
       </c>
-      <c r="N29" s="96">
+      <c r="N29" s="95">
         <f t="shared" si="17"/>
         <v>100.24000000000001</v>
       </c>
-      <c r="O29" s="59">
+      <c r="O29" s="58">
         <f t="shared" si="18"/>
         <v>125.30000000000001</v>
       </c>
-      <c r="P29" s="59">
+      <c r="P29" s="58">
         <f t="shared" si="19"/>
         <v>150.36000000000001</v>
       </c>
-      <c r="Q29" s="59">
+      <c r="Q29" s="58">
         <f t="shared" si="20"/>
         <v>175.42000000000002</v>
       </c>
-      <c r="R29" s="59">
+      <c r="R29" s="58">
         <f t="shared" si="21"/>
         <v>200.48000000000002</v>
       </c>
-      <c r="S29" s="59">
+      <c r="S29" s="58">
         <f t="shared" si="22"/>
         <v>225.54000000000005</v>
       </c>
-      <c r="T29" s="59">
+      <c r="T29" s="58">
         <f t="shared" si="23"/>
         <v>250.60000000000002</v>
       </c>
-      <c r="U29" s="60">
+      <c r="U29" s="59">
         <f t="shared" si="24"/>
         <v>275.66000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="49"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="32"/>
       <c r="E30" s="44"/>
       <c r="I30" s="24">
         <v>290</v>
       </c>
       <c r="J30" s="25"/>
-      <c r="K30" s="59">
+      <c r="K30" s="58">
         <f t="shared" si="14"/>
         <v>20.3</v>
       </c>
-      <c r="L30" s="59">
+      <c r="L30" s="58">
         <f t="shared" si="15"/>
         <v>40.6</v>
       </c>
-      <c r="M30" s="59">
+      <c r="M30" s="58">
         <f t="shared" si="16"/>
         <v>60.900000000000006</v>
       </c>
-      <c r="N30" s="59">
+      <c r="N30" s="58">
         <f t="shared" si="17"/>
         <v>81.2</v>
       </c>
-      <c r="O30" s="59">
+      <c r="O30" s="58">
         <f t="shared" si="18"/>
         <v>101.50000000000001</v>
       </c>
-      <c r="P30" s="59">
+      <c r="P30" s="58">
         <f t="shared" si="19"/>
         <v>121.80000000000001</v>
       </c>
-      <c r="Q30" s="59">
+      <c r="Q30" s="58">
         <f t="shared" si="20"/>
         <v>142.10000000000002</v>
       </c>
-      <c r="R30" s="59">
+      <c r="R30" s="58">
         <f t="shared" si="21"/>
         <v>162.4</v>
       </c>
-      <c r="S30" s="59">
+      <c r="S30" s="58">
         <f t="shared" si="22"/>
         <v>182.70000000000005</v>
       </c>
-      <c r="T30" s="59">
+      <c r="T30" s="58">
         <f t="shared" si="23"/>
         <v>203.00000000000003</v>
       </c>
-      <c r="U30" s="60">
+      <c r="U30" s="59">
         <f t="shared" si="24"/>
         <v>223.3</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="32"/>
       <c r="E31" s="44"/>
       <c r="I31" s="24">
         <v>286</v>
       </c>
       <c r="J31" s="25"/>
-      <c r="K31" s="59">
+      <c r="K31" s="58">
         <f t="shared" si="14"/>
         <v>20.020000000000003</v>
       </c>
-      <c r="L31" s="59">
+      <c r="L31" s="58">
         <f t="shared" si="15"/>
         <v>40.040000000000006</v>
       </c>
-      <c r="M31" s="59">
+      <c r="M31" s="58">
         <f t="shared" si="16"/>
         <v>60.06</v>
       </c>
-      <c r="N31" s="96">
+      <c r="N31" s="95">
         <f t="shared" si="17"/>
         <v>80.080000000000013</v>
       </c>
-      <c r="O31" s="96">
+      <c r="O31" s="95">
         <f t="shared" si="18"/>
         <v>100.10000000000001</v>
       </c>
-      <c r="P31" s="59">
+      <c r="P31" s="58">
         <f t="shared" si="19"/>
         <v>120.12</v>
       </c>
-      <c r="Q31" s="59">
+      <c r="Q31" s="58">
         <f t="shared" si="20"/>
         <v>140.14000000000001</v>
       </c>
-      <c r="R31" s="59">
+      <c r="R31" s="58">
         <f t="shared" si="21"/>
         <v>160.16000000000003</v>
       </c>
-      <c r="S31" s="59">
+      <c r="S31" s="58">
         <f t="shared" si="22"/>
         <v>180.18000000000004</v>
       </c>
-      <c r="T31" s="59">
+      <c r="T31" s="58">
         <f t="shared" si="23"/>
         <v>200.20000000000002</v>
       </c>
-      <c r="U31" s="60">
+      <c r="U31" s="59">
         <f t="shared" si="24"/>
         <v>220.22</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="50"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="41"/>
       <c r="E32" s="42"/>
       <c r="I32" s="24">
         <v>268</v>
       </c>
       <c r="J32" s="25"/>
-      <c r="K32" s="59">
+      <c r="K32" s="58">
         <f t="shared" si="14"/>
         <v>18.760000000000002</v>
       </c>
-      <c r="L32" s="59">
+      <c r="L32" s="58">
         <f t="shared" si="15"/>
         <v>37.520000000000003</v>
       </c>
-      <c r="M32" s="59">
+      <c r="M32" s="58">
         <f t="shared" si="16"/>
         <v>56.280000000000008</v>
       </c>
-      <c r="N32" s="96">
+      <c r="N32" s="95">
         <f t="shared" si="17"/>
         <v>75.040000000000006</v>
       </c>
-      <c r="O32" s="59">
+      <c r="O32" s="58">
         <f t="shared" si="18"/>
         <v>93.800000000000011</v>
       </c>
-      <c r="P32" s="59">
+      <c r="P32" s="58">
         <f t="shared" si="19"/>
         <v>112.56000000000002</v>
       </c>
-      <c r="Q32" s="59">
+      <c r="Q32" s="58">
         <f t="shared" si="20"/>
         <v>131.32000000000002</v>
       </c>
-      <c r="R32" s="59">
+      <c r="R32" s="58">
         <f t="shared" si="21"/>
         <v>150.08000000000001</v>
       </c>
-      <c r="S32" s="59">
+      <c r="S32" s="58">
         <f t="shared" si="22"/>
         <v>168.84000000000003</v>
       </c>
-      <c r="T32" s="59">
+      <c r="T32" s="58">
         <f t="shared" si="23"/>
         <v>187.60000000000002</v>
       </c>
-      <c r="U32" s="60">
+      <c r="U32" s="59">
         <f t="shared" si="24"/>
         <v>206.36</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I33" s="24">
         <v>260</v>
       </c>
       <c r="J33" s="25"/>
-      <c r="K33" s="59">
+      <c r="K33" s="58">
         <f t="shared" si="14"/>
         <v>18.200000000000003</v>
       </c>
-      <c r="L33" s="59">
+      <c r="L33" s="58">
         <f t="shared" si="15"/>
         <v>36.400000000000006</v>
       </c>
-      <c r="M33" s="59">
+      <c r="M33" s="58">
         <f t="shared" si="16"/>
         <v>54.600000000000009</v>
       </c>
-      <c r="N33" s="59">
+      <c r="N33" s="58">
         <f t="shared" si="17"/>
         <v>72.800000000000011</v>
       </c>
-      <c r="O33" s="59">
+      <c r="O33" s="58">
         <f t="shared" si="18"/>
         <v>91.000000000000014</v>
       </c>
-      <c r="P33" s="59">
+      <c r="P33" s="58">
         <f t="shared" si="19"/>
         <v>109.20000000000002</v>
       </c>
-      <c r="Q33" s="59">
+      <c r="Q33" s="58">
         <f t="shared" si="20"/>
         <v>127.4</v>
       </c>
-      <c r="R33" s="59">
+      <c r="R33" s="58">
         <f t="shared" si="21"/>
         <v>145.60000000000002</v>
       </c>
-      <c r="S33" s="59">
+      <c r="S33" s="58">
         <f t="shared" si="22"/>
         <v>163.80000000000004</v>
       </c>
-      <c r="T33" s="59">
+      <c r="T33" s="58">
         <f t="shared" si="23"/>
         <v>182.00000000000003</v>
       </c>
-      <c r="U33" s="60">
+      <c r="U33" s="59">
         <f t="shared" si="24"/>
         <v>200.20000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3258,1009 +3205,1009 @@
         <v>250</v>
       </c>
       <c r="J34" s="25"/>
-      <c r="K34" s="59">
+      <c r="K34" s="58">
         <f t="shared" si="14"/>
         <v>17.5</v>
       </c>
-      <c r="L34" s="59">
+      <c r="L34" s="58">
         <f t="shared" si="15"/>
         <v>35</v>
       </c>
-      <c r="M34" s="59">
+      <c r="M34" s="58">
         <f t="shared" si="16"/>
         <v>52.500000000000007</v>
       </c>
-      <c r="N34" s="96">
+      <c r="N34" s="95">
         <f t="shared" si="17"/>
         <v>70</v>
       </c>
-      <c r="O34" s="59">
+      <c r="O34" s="58">
         <f t="shared" si="18"/>
         <v>87.500000000000014</v>
       </c>
-      <c r="P34" s="59">
+      <c r="P34" s="58">
         <f t="shared" si="19"/>
         <v>105.00000000000001</v>
       </c>
-      <c r="Q34" s="59">
+      <c r="Q34" s="58">
         <f t="shared" si="20"/>
         <v>122.50000000000001</v>
       </c>
-      <c r="R34" s="59">
+      <c r="R34" s="58">
         <f t="shared" si="21"/>
         <v>140</v>
       </c>
-      <c r="S34" s="59">
+      <c r="S34" s="58">
         <f t="shared" si="22"/>
         <v>157.50000000000003</v>
       </c>
-      <c r="T34" s="59">
+      <c r="T34" s="58">
         <f t="shared" si="23"/>
         <v>175.00000000000003</v>
       </c>
-      <c r="U34" s="60">
+      <c r="U34" s="59">
         <f t="shared" si="24"/>
         <v>192.5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="I35" s="24">
         <v>239</v>
       </c>
       <c r="J35" s="25"/>
-      <c r="K35" s="59">
+      <c r="K35" s="58">
         <f t="shared" si="14"/>
         <v>16.73</v>
       </c>
-      <c r="L35" s="59">
+      <c r="L35" s="58">
         <f t="shared" si="15"/>
         <v>33.46</v>
       </c>
-      <c r="M35" s="59">
+      <c r="M35" s="58">
         <f t="shared" si="16"/>
         <v>50.190000000000005</v>
       </c>
-      <c r="N35" s="59">
+      <c r="N35" s="58">
         <f t="shared" si="17"/>
         <v>66.92</v>
       </c>
-      <c r="O35" s="59">
+      <c r="O35" s="58">
         <f t="shared" si="18"/>
         <v>83.65</v>
       </c>
-      <c r="P35" s="96">
+      <c r="P35" s="95">
         <f t="shared" si="19"/>
         <v>100.38000000000001</v>
       </c>
-      <c r="Q35" s="59">
+      <c r="Q35" s="58">
         <f t="shared" si="20"/>
         <v>117.11000000000001</v>
       </c>
-      <c r="R35" s="59">
+      <c r="R35" s="58">
         <f t="shared" si="21"/>
         <v>133.84</v>
       </c>
-      <c r="S35" s="59">
+      <c r="S35" s="58">
         <f t="shared" si="22"/>
         <v>150.57000000000002</v>
       </c>
-      <c r="T35" s="59">
+      <c r="T35" s="58">
         <f t="shared" si="23"/>
         <v>167.3</v>
       </c>
-      <c r="U35" s="60">
+      <c r="U35" s="59">
         <f t="shared" si="24"/>
         <v>184.03</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I36" s="24">
         <v>229</v>
       </c>
       <c r="J36" s="25"/>
-      <c r="K36" s="59">
+      <c r="K36" s="58">
         <f t="shared" si="14"/>
         <v>16.03</v>
       </c>
-      <c r="L36" s="59">
+      <c r="L36" s="58">
         <f t="shared" si="15"/>
         <v>32.06</v>
       </c>
-      <c r="M36" s="59">
+      <c r="M36" s="58">
         <f t="shared" si="16"/>
         <v>48.09</v>
       </c>
-      <c r="N36" s="59">
+      <c r="N36" s="58">
         <f t="shared" si="17"/>
         <v>64.12</v>
       </c>
-      <c r="O36" s="96">
+      <c r="O36" s="95">
         <f t="shared" si="18"/>
         <v>80.150000000000006</v>
       </c>
-      <c r="P36" s="59">
+      <c r="P36" s="58">
         <f t="shared" si="19"/>
         <v>96.18</v>
       </c>
-      <c r="Q36" s="59">
+      <c r="Q36" s="58">
         <f t="shared" si="20"/>
         <v>112.21000000000001</v>
       </c>
-      <c r="R36" s="59">
+      <c r="R36" s="58">
         <f t="shared" si="21"/>
         <v>128.24</v>
       </c>
-      <c r="S36" s="59">
+      <c r="S36" s="58">
         <f t="shared" si="22"/>
         <v>144.27000000000004</v>
       </c>
-      <c r="T36" s="59">
+      <c r="T36" s="58">
         <f t="shared" si="23"/>
         <v>160.30000000000001</v>
       </c>
-      <c r="U36" s="60">
+      <c r="U36" s="59">
         <f t="shared" si="24"/>
         <v>176.33</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I37" s="24">
         <v>220</v>
       </c>
       <c r="J37" s="25"/>
-      <c r="K37" s="59">
+      <c r="K37" s="58">
         <f t="shared" si="14"/>
         <v>15.400000000000002</v>
       </c>
-      <c r="L37" s="59">
+      <c r="L37" s="58">
         <f t="shared" si="15"/>
         <v>30.800000000000004</v>
       </c>
-      <c r="M37" s="59">
+      <c r="M37" s="58">
         <f t="shared" si="16"/>
         <v>46.2</v>
       </c>
-      <c r="N37" s="59">
+      <c r="N37" s="58">
         <f t="shared" si="17"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="O37" s="59">
+      <c r="O37" s="58">
         <f t="shared" si="18"/>
         <v>77.000000000000014</v>
       </c>
-      <c r="P37" s="59">
+      <c r="P37" s="58">
         <f t="shared" si="19"/>
         <v>92.4</v>
       </c>
-      <c r="Q37" s="59">
+      <c r="Q37" s="58">
         <f t="shared" si="20"/>
         <v>107.80000000000001</v>
       </c>
-      <c r="R37" s="59">
+      <c r="R37" s="58">
         <f t="shared" si="21"/>
         <v>123.20000000000002</v>
       </c>
-      <c r="S37" s="59">
+      <c r="S37" s="58">
         <f t="shared" si="22"/>
         <v>138.60000000000002</v>
       </c>
-      <c r="T37" s="59">
+      <c r="T37" s="58">
         <f t="shared" si="23"/>
         <v>154.00000000000003</v>
       </c>
-      <c r="U37" s="60">
+      <c r="U37" s="59">
         <f t="shared" si="24"/>
         <v>169.4</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I38" s="24">
         <v>215</v>
       </c>
       <c r="J38" s="25"/>
-      <c r="K38" s="59">
+      <c r="K38" s="58">
         <f t="shared" si="14"/>
         <v>15.05</v>
       </c>
-      <c r="L38" s="59">
+      <c r="L38" s="58">
         <f t="shared" si="15"/>
         <v>30.1</v>
       </c>
-      <c r="M38" s="59">
+      <c r="M38" s="58">
         <f t="shared" si="16"/>
         <v>45.150000000000006</v>
       </c>
-      <c r="N38" s="59">
+      <c r="N38" s="58">
         <f t="shared" si="17"/>
         <v>60.2</v>
       </c>
-      <c r="O38" s="96">
+      <c r="O38" s="95">
         <f t="shared" si="18"/>
         <v>75.250000000000014</v>
       </c>
-      <c r="P38" s="59">
+      <c r="P38" s="58">
         <f t="shared" si="19"/>
         <v>90.300000000000011</v>
       </c>
-      <c r="Q38" s="59">
+      <c r="Q38" s="58">
         <f t="shared" si="20"/>
         <v>105.35000000000001</v>
       </c>
-      <c r="R38" s="59">
+      <c r="R38" s="58">
         <f t="shared" si="21"/>
         <v>120.4</v>
       </c>
-      <c r="S38" s="59">
+      <c r="S38" s="58">
         <f t="shared" si="22"/>
         <v>135.45000000000002</v>
       </c>
-      <c r="T38" s="59">
+      <c r="T38" s="58">
         <f t="shared" si="23"/>
         <v>150.50000000000003</v>
       </c>
-      <c r="U38" s="60">
+      <c r="U38" s="59">
         <f t="shared" si="24"/>
         <v>165.55</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="I39" s="95">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I39" s="94">
         <v>205</v>
       </c>
       <c r="J39" s="25"/>
-      <c r="K39" s="59">
+      <c r="K39" s="58">
         <f t="shared" si="14"/>
         <v>14.350000000000001</v>
       </c>
-      <c r="L39" s="59">
+      <c r="L39" s="58">
         <f t="shared" si="15"/>
         <v>28.700000000000003</v>
       </c>
-      <c r="M39" s="59">
+      <c r="M39" s="58">
         <f t="shared" si="16"/>
         <v>43.050000000000004</v>
       </c>
-      <c r="N39" s="59">
+      <c r="N39" s="58">
         <f t="shared" si="17"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="O39" s="59">
+      <c r="O39" s="58">
         <f t="shared" si="18"/>
         <v>71.75</v>
       </c>
-      <c r="P39" s="59">
+      <c r="P39" s="58">
         <f t="shared" si="19"/>
         <v>86.100000000000009</v>
       </c>
-      <c r="Q39" s="96">
+      <c r="Q39" s="95">
         <f t="shared" si="20"/>
         <v>100.45</v>
       </c>
-      <c r="R39" s="59">
+      <c r="R39" s="58">
         <f t="shared" si="21"/>
         <v>114.80000000000001</v>
       </c>
-      <c r="S39" s="59">
+      <c r="S39" s="58">
         <f t="shared" si="22"/>
         <v>129.15000000000003</v>
       </c>
-      <c r="T39" s="59">
+      <c r="T39" s="58">
         <f t="shared" si="23"/>
         <v>143.5</v>
       </c>
-      <c r="U39" s="60">
+      <c r="U39" s="59">
         <f t="shared" si="24"/>
         <v>157.85</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="I40" s="95">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I40" s="94">
         <v>200</v>
       </c>
       <c r="J40" s="25"/>
-      <c r="K40" s="59">
+      <c r="K40" s="58">
         <f t="shared" si="14"/>
         <v>14.000000000000002</v>
       </c>
-      <c r="L40" s="59">
+      <c r="L40" s="58">
         <f t="shared" si="15"/>
         <v>28.000000000000004</v>
       </c>
-      <c r="M40" s="59">
+      <c r="M40" s="58">
         <f t="shared" si="16"/>
         <v>42.000000000000007</v>
       </c>
-      <c r="N40" s="59">
+      <c r="N40" s="58">
         <f t="shared" si="17"/>
         <v>56.000000000000007</v>
       </c>
-      <c r="O40" s="96">
+      <c r="O40" s="95">
         <f t="shared" si="18"/>
         <v>70</v>
       </c>
-      <c r="P40" s="59">
+      <c r="P40" s="58">
         <f t="shared" si="19"/>
         <v>84.000000000000014</v>
       </c>
-      <c r="Q40" s="59">
+      <c r="Q40" s="58">
         <f t="shared" si="20"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="R40" s="59">
+      <c r="R40" s="58">
         <f t="shared" si="21"/>
         <v>112.00000000000001</v>
       </c>
-      <c r="S40" s="59">
+      <c r="S40" s="58">
         <f t="shared" si="22"/>
         <v>126.00000000000003</v>
       </c>
-      <c r="T40" s="59">
+      <c r="T40" s="58">
         <f t="shared" si="23"/>
         <v>140</v>
       </c>
-      <c r="U40" s="60">
+      <c r="U40" s="59">
         <f t="shared" si="24"/>
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I41" s="24">
         <v>191</v>
       </c>
       <c r="J41" s="25"/>
-      <c r="K41" s="59">
+      <c r="K41" s="58">
         <f t="shared" si="14"/>
         <v>13.370000000000001</v>
       </c>
-      <c r="L41" s="59">
+      <c r="L41" s="58">
         <f t="shared" si="15"/>
         <v>26.740000000000002</v>
       </c>
-      <c r="M41" s="59">
+      <c r="M41" s="58">
         <f t="shared" si="16"/>
         <v>40.110000000000007</v>
       </c>
-      <c r="N41" s="59">
+      <c r="N41" s="58">
         <f t="shared" si="17"/>
         <v>53.480000000000004</v>
       </c>
-      <c r="O41" s="59">
+      <c r="O41" s="58">
         <f t="shared" si="18"/>
         <v>66.850000000000009</v>
       </c>
-      <c r="P41" s="96">
+      <c r="P41" s="95">
         <f t="shared" si="19"/>
         <v>80.220000000000013</v>
       </c>
-      <c r="Q41" s="59">
+      <c r="Q41" s="58">
         <f t="shared" si="20"/>
         <v>93.59</v>
       </c>
-      <c r="R41" s="59">
+      <c r="R41" s="58">
         <f t="shared" si="21"/>
         <v>106.96000000000001</v>
       </c>
-      <c r="S41" s="59">
+      <c r="S41" s="58">
         <f t="shared" si="22"/>
         <v>120.33000000000003</v>
       </c>
-      <c r="T41" s="59">
+      <c r="T41" s="58">
         <f t="shared" si="23"/>
         <v>133.70000000000002</v>
       </c>
-      <c r="U41" s="60">
+      <c r="U41" s="59">
         <f t="shared" si="24"/>
         <v>147.07</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I42" s="24">
         <v>180</v>
       </c>
       <c r="J42" s="25"/>
-      <c r="K42" s="59">
+      <c r="K42" s="58">
         <f t="shared" si="14"/>
         <v>12.600000000000001</v>
       </c>
-      <c r="L42" s="59">
+      <c r="L42" s="58">
         <f t="shared" si="15"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="M42" s="59">
+      <c r="M42" s="58">
         <f t="shared" si="16"/>
         <v>37.800000000000004</v>
       </c>
-      <c r="N42" s="59">
+      <c r="N42" s="58">
         <f t="shared" si="17"/>
         <v>50.400000000000006</v>
       </c>
-      <c r="O42" s="59">
+      <c r="O42" s="58">
         <f t="shared" si="18"/>
         <v>63.000000000000007</v>
       </c>
-      <c r="P42" s="59">
+      <c r="P42" s="58">
         <f t="shared" si="19"/>
         <v>75.600000000000009</v>
       </c>
-      <c r="Q42" s="59">
+      <c r="Q42" s="58">
         <f t="shared" si="20"/>
         <v>88.2</v>
       </c>
-      <c r="R42" s="59">
+      <c r="R42" s="58">
         <f t="shared" si="21"/>
         <v>100.80000000000001</v>
       </c>
-      <c r="S42" s="59">
+      <c r="S42" s="58">
         <f t="shared" si="22"/>
         <v>113.40000000000002</v>
       </c>
-      <c r="T42" s="59">
+      <c r="T42" s="58">
         <f t="shared" si="23"/>
         <v>126.00000000000001</v>
       </c>
-      <c r="U42" s="60">
+      <c r="U42" s="59">
         <f t="shared" si="24"/>
         <v>138.6</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I43" s="24">
         <v>179</v>
       </c>
       <c r="J43" s="25"/>
-      <c r="K43" s="59">
+      <c r="K43" s="58">
         <f t="shared" si="14"/>
         <v>12.530000000000001</v>
       </c>
-      <c r="L43" s="59">
+      <c r="L43" s="58">
         <f t="shared" si="15"/>
         <v>25.060000000000002</v>
       </c>
-      <c r="M43" s="59">
+      <c r="M43" s="58">
         <f t="shared" si="16"/>
         <v>37.590000000000003</v>
       </c>
-      <c r="N43" s="96">
+      <c r="N43" s="95">
         <f t="shared" si="17"/>
         <v>50.120000000000005</v>
       </c>
-      <c r="O43" s="59">
+      <c r="O43" s="58">
         <f t="shared" si="18"/>
         <v>62.650000000000006</v>
       </c>
-      <c r="P43" s="96">
+      <c r="P43" s="95">
         <f t="shared" si="19"/>
         <v>75.180000000000007</v>
       </c>
-      <c r="Q43" s="59">
+      <c r="Q43" s="58">
         <f t="shared" si="20"/>
         <v>87.710000000000008</v>
       </c>
-      <c r="R43" s="96">
+      <c r="R43" s="95">
         <f t="shared" si="21"/>
         <v>100.24000000000001</v>
       </c>
-      <c r="S43" s="59">
+      <c r="S43" s="58">
         <f t="shared" si="22"/>
         <v>112.77000000000002</v>
       </c>
-      <c r="T43" s="59">
+      <c r="T43" s="58">
         <f t="shared" si="23"/>
         <v>125.30000000000001</v>
       </c>
-      <c r="U43" s="60">
+      <c r="U43" s="59">
         <f t="shared" si="24"/>
         <v>137.83000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I44" s="24">
         <v>170</v>
       </c>
       <c r="J44" s="25"/>
-      <c r="K44" s="59">
+      <c r="K44" s="58">
         <f t="shared" si="14"/>
         <v>11.9</v>
       </c>
-      <c r="L44" s="59">
+      <c r="L44" s="58">
         <f t="shared" si="15"/>
         <v>23.8</v>
       </c>
-      <c r="M44" s="59">
+      <c r="M44" s="58">
         <f t="shared" si="16"/>
         <v>35.700000000000003</v>
       </c>
-      <c r="N44" s="59">
+      <c r="N44" s="58">
         <f t="shared" si="17"/>
         <v>47.6</v>
       </c>
-      <c r="O44" s="59">
+      <c r="O44" s="58">
         <f t="shared" si="18"/>
         <v>59.500000000000007</v>
       </c>
-      <c r="P44" s="59">
+      <c r="P44" s="58">
         <f t="shared" si="19"/>
         <v>71.400000000000006</v>
       </c>
-      <c r="Q44" s="59">
+      <c r="Q44" s="58">
         <f t="shared" si="20"/>
         <v>83.300000000000011</v>
       </c>
-      <c r="R44" s="59">
+      <c r="R44" s="58">
         <f t="shared" si="21"/>
         <v>95.2</v>
       </c>
-      <c r="S44" s="59">
+      <c r="S44" s="58">
         <f t="shared" si="22"/>
         <v>107.10000000000002</v>
       </c>
-      <c r="T44" s="59">
+      <c r="T44" s="58">
         <f t="shared" si="23"/>
         <v>119.00000000000001</v>
       </c>
-      <c r="U44" s="60">
+      <c r="U44" s="59">
         <f t="shared" si="24"/>
         <v>130.9</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I45" s="24">
         <v>168</v>
       </c>
       <c r="J45" s="25"/>
-      <c r="K45" s="59">
+      <c r="K45" s="58">
         <f t="shared" si="14"/>
         <v>11.760000000000002</v>
       </c>
-      <c r="L45" s="59">
+      <c r="L45" s="58">
         <f t="shared" si="15"/>
         <v>23.520000000000003</v>
       </c>
-      <c r="M45" s="59">
+      <c r="M45" s="58">
         <f t="shared" si="16"/>
         <v>35.28</v>
       </c>
-      <c r="N45" s="59">
+      <c r="N45" s="58">
         <f t="shared" si="17"/>
         <v>47.040000000000006</v>
       </c>
-      <c r="O45" s="59">
+      <c r="O45" s="58">
         <f t="shared" si="18"/>
         <v>58.800000000000004</v>
       </c>
-      <c r="P45" s="96">
+      <c r="P45" s="95">
         <f t="shared" si="19"/>
         <v>70.56</v>
       </c>
-      <c r="Q45" s="59">
+      <c r="Q45" s="58">
         <f t="shared" si="20"/>
         <v>82.320000000000007</v>
       </c>
-      <c r="R45" s="59">
+      <c r="R45" s="58">
         <f t="shared" si="21"/>
         <v>94.080000000000013</v>
       </c>
-      <c r="S45" s="59">
+      <c r="S45" s="58">
         <f t="shared" si="22"/>
         <v>105.84000000000002</v>
       </c>
-      <c r="T45" s="59">
+      <c r="T45" s="58">
         <f t="shared" si="23"/>
         <v>117.60000000000001</v>
       </c>
-      <c r="U45" s="60">
+      <c r="U45" s="59">
         <f t="shared" si="24"/>
         <v>129.36000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I46" s="24">
         <v>164</v>
       </c>
       <c r="J46" s="25"/>
-      <c r="K46" s="59">
+      <c r="K46" s="58">
         <f t="shared" si="14"/>
         <v>11.48</v>
       </c>
-      <c r="L46" s="59">
+      <c r="L46" s="58">
         <f t="shared" si="15"/>
         <v>22.96</v>
       </c>
-      <c r="M46" s="59">
+      <c r="M46" s="58">
         <f t="shared" si="16"/>
         <v>34.440000000000005</v>
       </c>
-      <c r="N46" s="59">
+      <c r="N46" s="58">
         <f t="shared" si="17"/>
         <v>45.92</v>
       </c>
-      <c r="O46" s="59">
+      <c r="O46" s="58">
         <f t="shared" si="18"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="P46" s="59">
+      <c r="P46" s="58">
         <f t="shared" si="19"/>
         <v>68.88000000000001</v>
       </c>
-      <c r="Q46" s="96">
+      <c r="Q46" s="95">
         <f t="shared" si="20"/>
         <v>80.360000000000014</v>
       </c>
-      <c r="R46" s="59">
+      <c r="R46" s="58">
         <f t="shared" si="21"/>
         <v>91.84</v>
       </c>
-      <c r="S46" s="59">
+      <c r="S46" s="58">
         <f t="shared" si="22"/>
         <v>103.32000000000002</v>
       </c>
-      <c r="T46" s="59">
+      <c r="T46" s="58">
         <f t="shared" si="23"/>
         <v>114.80000000000001</v>
       </c>
-      <c r="U46" s="98">
+      <c r="U46" s="97">
         <f t="shared" si="24"/>
         <v>126.28</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I47" s="24">
         <v>159</v>
       </c>
       <c r="J47" s="25"/>
-      <c r="K47" s="59">
+      <c r="K47" s="58">
         <f t="shared" si="14"/>
         <v>11.13</v>
       </c>
-      <c r="L47" s="59">
+      <c r="L47" s="58">
         <f t="shared" si="15"/>
         <v>22.26</v>
       </c>
-      <c r="M47" s="59">
+      <c r="M47" s="58">
         <f t="shared" si="16"/>
         <v>33.39</v>
       </c>
-      <c r="N47" s="59">
+      <c r="N47" s="58">
         <f t="shared" si="17"/>
         <v>44.52</v>
       </c>
-      <c r="O47" s="59">
+      <c r="O47" s="58">
         <f t="shared" si="18"/>
         <v>55.650000000000006</v>
       </c>
-      <c r="P47" s="59">
+      <c r="P47" s="58">
         <f t="shared" si="19"/>
         <v>66.78</v>
       </c>
-      <c r="Q47" s="59">
+      <c r="Q47" s="58">
         <f t="shared" si="20"/>
         <v>77.910000000000011</v>
       </c>
-      <c r="R47" s="59">
+      <c r="R47" s="58">
         <f t="shared" si="21"/>
         <v>89.04</v>
       </c>
-      <c r="S47" s="96">
+      <c r="S47" s="95">
         <f t="shared" si="22"/>
         <v>100.17000000000002</v>
       </c>
-      <c r="T47" s="59">
+      <c r="T47" s="58">
         <f t="shared" si="23"/>
         <v>111.30000000000001</v>
       </c>
-      <c r="U47" s="60">
+      <c r="U47" s="59">
         <f t="shared" si="24"/>
         <v>122.43</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I48" s="24">
         <v>154</v>
       </c>
       <c r="J48" s="25"/>
-      <c r="K48" s="59">
+      <c r="K48" s="58">
         <f t="shared" si="14"/>
         <v>10.780000000000001</v>
       </c>
-      <c r="L48" s="59">
+      <c r="L48" s="58">
         <f t="shared" si="15"/>
         <v>21.560000000000002</v>
       </c>
-      <c r="M48" s="59">
+      <c r="M48" s="58">
         <f t="shared" si="16"/>
         <v>32.340000000000003</v>
       </c>
-      <c r="N48" s="59">
+      <c r="N48" s="58">
         <f t="shared" si="17"/>
         <v>43.120000000000005</v>
       </c>
-      <c r="O48" s="59">
+      <c r="O48" s="58">
         <f t="shared" si="18"/>
         <v>53.900000000000006</v>
       </c>
-      <c r="P48" s="59">
+      <c r="P48" s="58">
         <f t="shared" si="19"/>
         <v>64.680000000000007</v>
       </c>
-      <c r="Q48" s="96">
+      <c r="Q48" s="95">
         <f t="shared" si="20"/>
         <v>75.460000000000008</v>
       </c>
-      <c r="R48" s="59">
+      <c r="R48" s="58">
         <f t="shared" si="21"/>
         <v>86.240000000000009</v>
       </c>
-      <c r="S48" s="59">
+      <c r="S48" s="58">
         <f t="shared" si="22"/>
         <v>97.020000000000024</v>
       </c>
-      <c r="T48" s="59">
+      <c r="T48" s="58">
         <f t="shared" si="23"/>
         <v>107.80000000000001</v>
       </c>
-      <c r="U48" s="60">
+      <c r="U48" s="59">
         <f t="shared" si="24"/>
         <v>118.58</v>
       </c>
     </row>
-    <row r="49" spans="9:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I49" s="24">
         <v>143</v>
       </c>
       <c r="J49" s="25"/>
-      <c r="K49" s="59">
+      <c r="K49" s="58">
         <f t="shared" si="14"/>
         <v>10.010000000000002</v>
       </c>
-      <c r="L49" s="59">
+      <c r="L49" s="58">
         <f t="shared" si="15"/>
         <v>20.020000000000003</v>
       </c>
-      <c r="M49" s="59">
+      <c r="M49" s="58">
         <f t="shared" si="16"/>
         <v>30.03</v>
       </c>
-      <c r="N49" s="59">
+      <c r="N49" s="58">
         <f t="shared" si="17"/>
         <v>40.040000000000006</v>
       </c>
-      <c r="O49" s="96">
+      <c r="O49" s="95">
         <f t="shared" si="18"/>
         <v>50.050000000000004</v>
       </c>
-      <c r="P49" s="59">
+      <c r="P49" s="58">
         <f t="shared" si="19"/>
         <v>60.06</v>
       </c>
-      <c r="Q49" s="96">
+      <c r="Q49" s="95">
         <f t="shared" si="20"/>
         <v>70.070000000000007</v>
       </c>
-      <c r="R49" s="59">
+      <c r="R49" s="58">
         <f t="shared" si="21"/>
         <v>80.080000000000013</v>
       </c>
-      <c r="S49" s="59">
+      <c r="S49" s="58">
         <f t="shared" si="22"/>
         <v>90.090000000000018</v>
       </c>
-      <c r="T49" s="96">
+      <c r="T49" s="95">
         <f t="shared" si="23"/>
         <v>100.10000000000001</v>
       </c>
-      <c r="U49" s="60">
+      <c r="U49" s="59">
         <f t="shared" si="24"/>
         <v>110.11</v>
       </c>
     </row>
-    <row r="50" spans="9:21" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I50" s="24">
         <v>178</v>
       </c>
       <c r="J50" s="25"/>
-      <c r="K50" s="59">
+      <c r="K50" s="58">
         <f t="shared" si="14"/>
         <v>12.46</v>
       </c>
-      <c r="L50" s="59">
+      <c r="L50" s="58">
         <f t="shared" si="15"/>
         <v>24.92</v>
       </c>
-      <c r="M50" s="59">
+      <c r="M50" s="58">
         <f t="shared" si="16"/>
         <v>37.380000000000003</v>
       </c>
-      <c r="N50" s="59">
+      <c r="N50" s="58">
         <f t="shared" si="17"/>
         <v>49.84</v>
       </c>
-      <c r="O50" s="59">
+      <c r="O50" s="58">
         <f t="shared" si="18"/>
         <v>62.300000000000004</v>
       </c>
-      <c r="P50" s="59">
+      <c r="P50" s="58">
         <f t="shared" si="19"/>
         <v>74.760000000000005</v>
       </c>
-      <c r="Q50" s="59">
+      <c r="Q50" s="58">
         <f t="shared" si="20"/>
         <v>87.220000000000013</v>
       </c>
-      <c r="R50" s="59">
+      <c r="R50" s="58">
         <f t="shared" si="21"/>
         <v>99.68</v>
       </c>
-      <c r="S50" s="59">
+      <c r="S50" s="58">
         <f t="shared" si="22"/>
         <v>112.14000000000001</v>
       </c>
-      <c r="T50" s="59">
+      <c r="T50" s="58">
         <f t="shared" si="23"/>
         <v>124.60000000000001</v>
       </c>
-      <c r="U50" s="60">
+      <c r="U50" s="59">
         <f t="shared" si="24"/>
         <v>137.06</v>
       </c>
     </row>
-    <row r="51" spans="9:21" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I51" s="24">
         <v>130</v>
       </c>
       <c r="J51" s="25"/>
-      <c r="K51" s="59">
+      <c r="K51" s="58">
         <f t="shared" si="14"/>
         <v>9.1000000000000014</v>
       </c>
-      <c r="L51" s="59">
+      <c r="L51" s="58">
         <f t="shared" si="15"/>
         <v>18.200000000000003</v>
       </c>
-      <c r="M51" s="59">
+      <c r="M51" s="58">
         <f t="shared" si="16"/>
         <v>27.300000000000004</v>
       </c>
-      <c r="N51" s="59">
+      <c r="N51" s="58">
         <f t="shared" si="17"/>
         <v>36.400000000000006</v>
       </c>
-      <c r="O51" s="59">
+      <c r="O51" s="58">
         <f t="shared" si="18"/>
         <v>45.500000000000007</v>
       </c>
-      <c r="P51" s="59">
+      <c r="P51" s="58">
         <f t="shared" si="19"/>
         <v>54.600000000000009</v>
       </c>
-      <c r="Q51" s="59">
+      <c r="Q51" s="58">
         <f t="shared" si="20"/>
         <v>63.7</v>
       </c>
-      <c r="R51" s="59">
+      <c r="R51" s="58">
         <f t="shared" si="21"/>
         <v>72.800000000000011</v>
       </c>
-      <c r="S51" s="59">
+      <c r="S51" s="58">
         <f t="shared" si="22"/>
         <v>81.90000000000002</v>
       </c>
-      <c r="T51" s="59">
+      <c r="T51" s="58">
         <f t="shared" si="23"/>
         <v>91.000000000000014</v>
       </c>
-      <c r="U51" s="98">
+      <c r="U51" s="97">
         <f t="shared" si="24"/>
         <v>100.10000000000001</v>
       </c>
     </row>
-    <row r="52" spans="9:21" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I52" s="24">
         <v>120</v>
       </c>
       <c r="J52" s="25"/>
-      <c r="K52" s="59">
+      <c r="K52" s="58">
         <f t="shared" si="14"/>
         <v>8.4</v>
       </c>
-      <c r="L52" s="59">
+      <c r="L52" s="58">
         <f t="shared" si="15"/>
         <v>16.8</v>
       </c>
-      <c r="M52" s="59">
+      <c r="M52" s="58">
         <f t="shared" si="16"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="N52" s="59">
+      <c r="N52" s="58">
         <f t="shared" si="17"/>
         <v>33.6</v>
       </c>
-      <c r="O52" s="59">
+      <c r="O52" s="58">
         <f t="shared" si="18"/>
         <v>42.000000000000007</v>
       </c>
-      <c r="P52" s="96">
+      <c r="P52" s="95">
         <f t="shared" si="19"/>
         <v>50.400000000000006</v>
       </c>
-      <c r="Q52" s="59">
+      <c r="Q52" s="58">
         <f t="shared" si="20"/>
         <v>58.800000000000004</v>
       </c>
-      <c r="R52" s="59">
+      <c r="R52" s="58">
         <f t="shared" si="21"/>
         <v>67.2</v>
       </c>
-      <c r="S52" s="59">
+      <c r="S52" s="58">
         <f t="shared" si="22"/>
         <v>75.600000000000009</v>
       </c>
-      <c r="T52" s="59">
+      <c r="T52" s="58">
         <f t="shared" si="23"/>
         <v>84.000000000000014</v>
       </c>
-      <c r="U52" s="60">
+      <c r="U52" s="59">
         <f t="shared" si="24"/>
         <v>92.4</v>
       </c>
     </row>
-    <row r="53" spans="9:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="9:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I53" s="26">
         <v>103</v>
       </c>
       <c r="J53" s="27"/>
-      <c r="K53" s="61">
+      <c r="K53" s="60">
         <f t="shared" si="14"/>
         <v>7.2100000000000009</v>
       </c>
-      <c r="L53" s="61">
+      <c r="L53" s="60">
         <f t="shared" si="15"/>
         <v>14.420000000000002</v>
       </c>
-      <c r="M53" s="61">
+      <c r="M53" s="60">
         <f t="shared" si="16"/>
         <v>21.630000000000003</v>
       </c>
-      <c r="N53" s="61">
+      <c r="N53" s="60">
         <f t="shared" si="17"/>
         <v>28.840000000000003</v>
       </c>
-      <c r="O53" s="61">
+      <c r="O53" s="60">
         <f t="shared" si="18"/>
         <v>36.050000000000004</v>
       </c>
-      <c r="P53" s="61">
+      <c r="P53" s="60">
         <f t="shared" si="19"/>
         <v>43.260000000000005</v>
       </c>
-      <c r="Q53" s="97">
+      <c r="Q53" s="96">
         <f t="shared" si="20"/>
         <v>50.470000000000006</v>
       </c>
-      <c r="R53" s="61">
+      <c r="R53" s="60">
         <f t="shared" si="21"/>
         <v>57.680000000000007</v>
       </c>
-      <c r="S53" s="61">
+      <c r="S53" s="60">
         <f t="shared" si="22"/>
         <v>64.890000000000015</v>
       </c>
-      <c r="T53" s="61">
+      <c r="T53" s="60">
         <f t="shared" si="23"/>
         <v>72.100000000000009</v>
       </c>
-      <c r="U53" s="62">
+      <c r="U53" s="61">
         <f t="shared" si="24"/>
         <v>79.31</v>
       </c>
     </row>
-    <row r="54" spans="9:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="9:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="O54" s="5"/>
       <c r="Q54" s="5"/>
       <c r="U54" s="5"/>
     </row>
-    <row r="55" spans="9:21" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:21" x14ac:dyDescent="0.25">
       <c r="O55" s="5"/>
       <c r="Q55" s="5"/>
       <c r="U55" s="5"/>
@@ -4313,139 +4260,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17">
-        <v>205</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
spd buff changed to .33
</commit_message>
<xml_diff>
--- a/summoners_war_0_1_0/output/xlsx_reports/speed_charts.xlsx
+++ b/summoners_war_0_1_0/output/xlsx_reports/speed_charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="7005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18230" windowHeight="7010"/>
   </bookViews>
   <sheets>
     <sheet name="Speed Calculators" sheetId="1" r:id="rId1"/>
@@ -697,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -734,7 +734,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -801,9 +800,6 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -826,9 +822,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -867,16 +860,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,6 +878,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1179,118 +1185,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" style="107" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.81640625" customWidth="1"/>
+    <col min="11" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="32.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="51" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="50" t="s">
         <v>27</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
       <c r="U1" s="11"/>
       <c r="V1" s="4"/>
     </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="102"/>
-      <c r="G2" s="63" t="s">
+      <c r="F2" s="97"/>
+      <c r="G2" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H2" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="73" t="s">
+      <c r="I2" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="103" t="s">
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="104"/>
-      <c r="P2" s="104"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="91"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="88"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="86">
-        <v>0.24</v>
-      </c>
-      <c r="F3" s="87">
+      <c r="D3" s="82"/>
+      <c r="E3" s="83">
+        <v>0</v>
+      </c>
+      <c r="F3" s="84">
         <v>0.15</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="87">
-        <v>0</v>
-      </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="52" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="83">
+        <v>0.33</v>
+      </c>
+      <c r="I3" s="85"/>
+      <c r="J3" s="51" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="9">
@@ -1302,16 +1308,16 @@
       <c r="M3" s="9">
         <v>3</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="20">
         <v>4</v>
       </c>
-      <c r="O3" s="22">
+      <c r="O3" s="21">
         <v>5</v>
       </c>
-      <c r="P3" s="22">
+      <c r="P3" s="21">
         <v>6</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="22">
         <v>7</v>
       </c>
       <c r="R3" s="9">
@@ -1328,1353 +1334,1353 @@
       </c>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="98">
-        <v>104</v>
-      </c>
-      <c r="E4" s="99">
+      <c r="D4" s="95">
+        <v>102</v>
+      </c>
+      <c r="E4" s="98">
         <f>SUM($D4*(1+$E$3+$F$3))</f>
-        <v>144.56</v>
-      </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="92">
-        <v>89</v>
-      </c>
-      <c r="H4" s="65">
+        <v>117.3</v>
+      </c>
+      <c r="F4" s="98"/>
+      <c r="G4" s="89">
+        <v>38</v>
+      </c>
+      <c r="H4" s="105">
         <f>SUM($H$3)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I4" s="73">
         <f>SUM(($E4+$G4)*(1+$H4))</f>
-        <v>233.56</v>
-      </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54">
+        <v>206.54900000000004</v>
+      </c>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53">
         <f>SUM($I4*(0.07*1))</f>
-        <v>16.349200000000003</v>
-      </c>
-      <c r="L4" s="54">
+        <v>14.458430000000003</v>
+      </c>
+      <c r="L4" s="53">
         <f>SUM($I4*(0.07*2))</f>
-        <v>32.698400000000007</v>
-      </c>
-      <c r="M4" s="54">
+        <v>28.916860000000007</v>
+      </c>
+      <c r="M4" s="53">
         <f>SUM($I4*(0.07*3))</f>
-        <v>49.047600000000003</v>
-      </c>
-      <c r="N4" s="54">
+        <v>43.375290000000014</v>
+      </c>
+      <c r="N4" s="53">
         <f>SUM($I4*(0.07*4))</f>
-        <v>65.396800000000013</v>
-      </c>
-      <c r="O4" s="54">
+        <v>57.833720000000014</v>
+      </c>
+      <c r="O4" s="53">
         <f>SUM($I4*(0.07*5))</f>
-        <v>81.746000000000009</v>
-      </c>
-      <c r="P4" s="54">
+        <v>72.292150000000021</v>
+      </c>
+      <c r="P4" s="53">
         <f>SUM($I4*(0.07*6))</f>
-        <v>98.095200000000006</v>
-      </c>
-      <c r="Q4" s="54">
+        <v>86.750580000000028</v>
+      </c>
+      <c r="Q4" s="53">
         <f>SUM($I4*(0.07*7))</f>
-        <v>114.44440000000002</v>
-      </c>
-      <c r="R4" s="54">
+        <v>101.20901000000002</v>
+      </c>
+      <c r="R4" s="53">
         <f>SUM($I4*(0.07*8))</f>
-        <v>130.79360000000003</v>
-      </c>
-      <c r="S4" s="54">
+        <v>115.66744000000003</v>
+      </c>
+      <c r="S4" s="53">
         <f>SUM($I4*(0.07*9))</f>
-        <v>147.14280000000002</v>
-      </c>
-      <c r="T4" s="54">
+        <v>130.12587000000005</v>
+      </c>
+      <c r="T4" s="53">
         <f>SUM($I4*(0.07*10))</f>
-        <v>163.49200000000002</v>
-      </c>
-      <c r="U4" s="55">
+        <v>144.58430000000004</v>
+      </c>
+      <c r="U4" s="54">
         <f>SUM($I4*(0.07*11))</f>
-        <v>179.84120000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+        <v>159.04273000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="66">
-        <v>126</v>
-      </c>
-      <c r="E5" s="99">
+      <c r="D5" s="64">
+        <v>116</v>
+      </c>
+      <c r="E5" s="98">
         <f>SUM($D5*(1+$E$3+$F$3))</f>
-        <v>175.14</v>
-      </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="92">
-        <v>190</v>
-      </c>
-      <c r="H5" s="65">
+        <v>133.39999999999998</v>
+      </c>
+      <c r="F5" s="98"/>
+      <c r="G5" s="89">
+        <v>20</v>
+      </c>
+      <c r="H5" s="105">
         <f t="shared" ref="H5:H21" si="0">SUM($H$3)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I5" s="73">
         <f>SUM(($E5+$G5)*(1+$H5))</f>
-        <v>365.14</v>
-      </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54">
+        <v>204.02199999999999</v>
+      </c>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53">
         <f t="shared" ref="K5:K21" si="1">SUM($I5*(0.07*1))</f>
-        <v>25.559800000000003</v>
-      </c>
-      <c r="L5" s="54">
+        <v>14.281540000000001</v>
+      </c>
+      <c r="L5" s="53">
         <f t="shared" ref="L5:L21" si="2">SUM($I5*(0.07*2))</f>
-        <v>51.119600000000005</v>
-      </c>
-      <c r="M5" s="54">
+        <v>28.563080000000003</v>
+      </c>
+      <c r="M5" s="53">
         <f t="shared" ref="M5:M21" si="3">SUM($I5*(0.07*3))</f>
-        <v>76.679400000000001</v>
-      </c>
-      <c r="N5" s="54">
+        <v>42.844619999999999</v>
+      </c>
+      <c r="N5" s="53">
         <f t="shared" ref="N5:N21" si="4">SUM($I5*(0.07*4))</f>
-        <v>102.23920000000001</v>
-      </c>
-      <c r="O5" s="54">
+        <v>57.126160000000006</v>
+      </c>
+      <c r="O5" s="53">
         <f t="shared" ref="O5:O21" si="5">SUM($I5*(0.07*5))</f>
-        <v>127.79900000000001</v>
-      </c>
-      <c r="P5" s="54">
+        <v>71.407700000000006</v>
+      </c>
+      <c r="P5" s="53">
         <f t="shared" ref="P5:P21" si="6">SUM($I5*(0.07*6))</f>
-        <v>153.3588</v>
-      </c>
-      <c r="Q5" s="54">
+        <v>85.689239999999998</v>
+      </c>
+      <c r="Q5" s="53">
         <f t="shared" ref="Q5:Q21" si="7">SUM($I5*(0.07*7))</f>
-        <v>178.9186</v>
-      </c>
-      <c r="R5" s="54">
+        <v>99.970780000000005</v>
+      </c>
+      <c r="R5" s="53">
         <f t="shared" ref="R5:R21" si="8">SUM($I5*(0.07*8))</f>
-        <v>204.47840000000002</v>
-      </c>
-      <c r="S5" s="54">
+        <v>114.25232000000001</v>
+      </c>
+      <c r="S5" s="53">
         <f t="shared" ref="S5:S21" si="9">SUM($I5*(0.07*9))</f>
-        <v>230.03820000000005</v>
-      </c>
-      <c r="T5" s="54">
+        <v>128.53386</v>
+      </c>
+      <c r="T5" s="53">
         <f t="shared" ref="T5:T21" si="10">SUM($I5*(0.07*10))</f>
-        <v>255.59800000000001</v>
-      </c>
-      <c r="U5" s="55">
+        <v>142.81540000000001</v>
+      </c>
+      <c r="U5" s="54">
         <f t="shared" ref="U5:U21" si="11">SUM($I5*(0.07*11))</f>
-        <v>281.15780000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+        <v>157.09693999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="64">
+      <c r="D6" s="63">
         <v>116</v>
       </c>
-      <c r="E6" s="99">
+      <c r="E6" s="98">
         <f t="shared" ref="E6:E21" si="12">SUM($D6*(1+$E$3+$F$3))</f>
-        <v>161.23999999999998</v>
-      </c>
-      <c r="F6" s="99"/>
-      <c r="G6" s="92">
+        <v>133.39999999999998</v>
+      </c>
+      <c r="F6" s="98"/>
+      <c r="G6" s="89">
         <v>156</v>
       </c>
-      <c r="H6" s="65">
+      <c r="H6" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I6" s="73">
         <f t="shared" ref="I6:I21" si="13">SUM(($E6+$G6)*(1+$H6))</f>
-        <v>317.24</v>
-      </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54">
+        <v>384.90199999999999</v>
+      </c>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53">
         <f t="shared" si="1"/>
-        <v>22.206800000000001</v>
-      </c>
-      <c r="L6" s="54">
+        <v>26.943140000000003</v>
+      </c>
+      <c r="L6" s="53">
         <f t="shared" si="2"/>
-        <v>44.413600000000002</v>
-      </c>
-      <c r="M6" s="54">
+        <v>53.886280000000006</v>
+      </c>
+      <c r="M6" s="53">
         <f t="shared" si="3"/>
-        <v>66.620400000000004</v>
-      </c>
-      <c r="N6" s="54">
+        <v>80.829419999999999</v>
+      </c>
+      <c r="N6" s="53">
         <f t="shared" si="4"/>
-        <v>88.827200000000005</v>
-      </c>
-      <c r="O6" s="54">
+        <v>107.77256000000001</v>
+      </c>
+      <c r="O6" s="53">
         <f t="shared" si="5"/>
-        <v>111.03400000000002</v>
-      </c>
-      <c r="P6" s="54">
+        <v>134.7157</v>
+      </c>
+      <c r="P6" s="53">
         <f t="shared" si="6"/>
-        <v>133.24080000000001</v>
-      </c>
-      <c r="Q6" s="54">
+        <v>161.65884</v>
+      </c>
+      <c r="Q6" s="53">
         <f t="shared" si="7"/>
-        <v>155.44760000000002</v>
-      </c>
-      <c r="R6" s="54">
+        <v>188.60198</v>
+      </c>
+      <c r="R6" s="53">
         <f t="shared" si="8"/>
-        <v>177.65440000000001</v>
-      </c>
-      <c r="S6" s="54">
+        <v>215.54512000000003</v>
+      </c>
+      <c r="S6" s="53">
         <f t="shared" si="9"/>
-        <v>199.86120000000005</v>
-      </c>
-      <c r="T6" s="54">
+        <v>242.48826000000003</v>
+      </c>
+      <c r="T6" s="53">
         <f t="shared" si="10"/>
-        <v>222.06800000000004</v>
-      </c>
-      <c r="U6" s="55">
+        <v>269.4314</v>
+      </c>
+      <c r="U6" s="54">
         <f t="shared" si="11"/>
-        <v>244.2748</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+        <v>296.37454000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="6">
         <v>30</v>
       </c>
-      <c r="D7" s="64">
+      <c r="D7" s="63">
         <v>120</v>
       </c>
-      <c r="E7" s="99">
+      <c r="E7" s="98">
         <f t="shared" si="12"/>
-        <v>166.79999999999998</v>
-      </c>
-      <c r="F7" s="99"/>
-      <c r="G7" s="92">
+        <v>138</v>
+      </c>
+      <c r="F7" s="98"/>
+      <c r="G7" s="89">
         <v>162</v>
       </c>
-      <c r="H7" s="65">
+      <c r="H7" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I7" s="73">
         <f t="shared" si="13"/>
-        <v>328.79999999999995</v>
-      </c>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54">
+        <v>399</v>
+      </c>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53">
         <f t="shared" si="1"/>
-        <v>23.015999999999998</v>
-      </c>
-      <c r="L7" s="54">
+        <v>27.930000000000003</v>
+      </c>
+      <c r="L7" s="53">
         <f t="shared" si="2"/>
-        <v>46.031999999999996</v>
-      </c>
-      <c r="M7" s="54">
+        <v>55.860000000000007</v>
+      </c>
+      <c r="M7" s="53">
         <f t="shared" si="3"/>
-        <v>69.048000000000002</v>
-      </c>
-      <c r="N7" s="54">
+        <v>83.79</v>
+      </c>
+      <c r="N7" s="53">
         <f t="shared" si="4"/>
-        <v>92.063999999999993</v>
-      </c>
-      <c r="O7" s="54">
+        <v>111.72000000000001</v>
+      </c>
+      <c r="O7" s="53">
         <f t="shared" si="5"/>
-        <v>115.08</v>
-      </c>
-      <c r="P7" s="54">
+        <v>139.65</v>
+      </c>
+      <c r="P7" s="53">
         <f t="shared" si="6"/>
-        <v>138.096</v>
-      </c>
-      <c r="Q7" s="54">
+        <v>167.58</v>
+      </c>
+      <c r="Q7" s="53">
         <f t="shared" si="7"/>
-        <v>161.11199999999999</v>
-      </c>
-      <c r="R7" s="54">
+        <v>195.51000000000002</v>
+      </c>
+      <c r="R7" s="53">
         <f t="shared" si="8"/>
-        <v>184.12799999999999</v>
-      </c>
-      <c r="S7" s="54">
+        <v>223.44000000000003</v>
+      </c>
+      <c r="S7" s="53">
         <f t="shared" si="9"/>
-        <v>207.14400000000001</v>
-      </c>
-      <c r="T7" s="54">
+        <v>251.37000000000003</v>
+      </c>
+      <c r="T7" s="53">
         <f t="shared" si="10"/>
-        <v>230.16</v>
-      </c>
-      <c r="U7" s="55">
+        <v>279.3</v>
+      </c>
+      <c r="U7" s="54">
         <f t="shared" si="11"/>
-        <v>253.17599999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+        <v>307.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="D8" s="64">
+      <c r="D8" s="63">
         <v>96</v>
       </c>
-      <c r="E8" s="99">
+      <c r="E8" s="98">
         <f t="shared" si="12"/>
-        <v>133.44</v>
-      </c>
-      <c r="F8" s="99"/>
-      <c r="G8" s="92">
+        <v>110.39999999999999</v>
+      </c>
+      <c r="F8" s="98"/>
+      <c r="G8" s="89">
         <v>100</v>
       </c>
-      <c r="H8" s="65">
+      <c r="H8" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I8" s="73">
         <f t="shared" si="13"/>
-        <v>233.44</v>
-      </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54">
+        <v>279.83199999999999</v>
+      </c>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53">
         <f t="shared" si="1"/>
-        <v>16.340800000000002</v>
-      </c>
-      <c r="L8" s="54">
+        <v>19.588240000000003</v>
+      </c>
+      <c r="L8" s="53">
         <f t="shared" si="2"/>
-        <v>32.681600000000003</v>
-      </c>
-      <c r="M8" s="54">
+        <v>39.176480000000005</v>
+      </c>
+      <c r="M8" s="53">
         <f t="shared" si="3"/>
-        <v>49.022400000000005</v>
-      </c>
-      <c r="N8" s="54">
+        <v>58.764720000000004</v>
+      </c>
+      <c r="N8" s="53">
         <f t="shared" si="4"/>
-        <v>65.363200000000006</v>
-      </c>
-      <c r="O8" s="54">
+        <v>78.35296000000001</v>
+      </c>
+      <c r="O8" s="53">
         <f t="shared" si="5"/>
-        <v>81.704000000000008</v>
-      </c>
-      <c r="P8" s="54">
+        <v>97.941200000000009</v>
+      </c>
+      <c r="P8" s="53">
         <f t="shared" si="6"/>
-        <v>98.044800000000009</v>
-      </c>
-      <c r="Q8" s="54">
+        <v>117.52944000000001</v>
+      </c>
+      <c r="Q8" s="53">
         <f t="shared" si="7"/>
-        <v>114.38560000000001</v>
-      </c>
-      <c r="R8" s="54">
+        <v>137.11768000000001</v>
+      </c>
+      <c r="R8" s="53">
         <f t="shared" si="8"/>
-        <v>130.72640000000001</v>
-      </c>
-      <c r="S8" s="54">
+        <v>156.70592000000002</v>
+      </c>
+      <c r="S8" s="53">
         <f t="shared" si="9"/>
-        <v>147.06720000000001</v>
-      </c>
-      <c r="T8" s="54">
+        <v>176.29416000000003</v>
+      </c>
+      <c r="T8" s="53">
         <f t="shared" si="10"/>
-        <v>163.40800000000002</v>
-      </c>
-      <c r="U8" s="55">
+        <v>195.88240000000002</v>
+      </c>
+      <c r="U8" s="54">
         <f t="shared" si="11"/>
-        <v>179.74879999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+        <v>215.47064</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="89">
+      <c r="C9" s="86">
         <v>25</v>
       </c>
-      <c r="D9" s="64">
+      <c r="D9" s="63">
         <v>99</v>
       </c>
-      <c r="E9" s="99">
+      <c r="E9" s="98">
         <f t="shared" si="12"/>
-        <v>137.60999999999999</v>
-      </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="92">
+        <v>113.85</v>
+      </c>
+      <c r="F9" s="98"/>
+      <c r="G9" s="89">
         <v>250</v>
       </c>
-      <c r="H9" s="65">
+      <c r="H9" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I9" s="73">
         <f t="shared" si="13"/>
-        <v>387.61</v>
-      </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54">
+        <v>483.92050000000006</v>
+      </c>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53">
         <f t="shared" si="1"/>
-        <v>27.132700000000003</v>
-      </c>
-      <c r="L9" s="54">
+        <v>33.874435000000005</v>
+      </c>
+      <c r="L9" s="53">
         <f t="shared" si="2"/>
-        <v>54.265400000000007</v>
-      </c>
-      <c r="M9" s="54">
+        <v>67.748870000000011</v>
+      </c>
+      <c r="M9" s="53">
         <f t="shared" si="3"/>
-        <v>81.398100000000014</v>
-      </c>
-      <c r="N9" s="54">
+        <v>101.62330500000002</v>
+      </c>
+      <c r="N9" s="53">
         <f t="shared" si="4"/>
-        <v>108.53080000000001</v>
-      </c>
-      <c r="O9" s="54">
+        <v>135.49774000000002</v>
+      </c>
+      <c r="O9" s="53">
         <f t="shared" si="5"/>
-        <v>135.66350000000003</v>
-      </c>
-      <c r="P9" s="54">
+        <v>169.37217500000003</v>
+      </c>
+      <c r="P9" s="53">
         <f t="shared" si="6"/>
-        <v>162.79620000000003</v>
-      </c>
-      <c r="Q9" s="54">
+        <v>203.24661000000003</v>
+      </c>
+      <c r="Q9" s="53">
         <f t="shared" si="7"/>
-        <v>189.92890000000003</v>
-      </c>
-      <c r="R9" s="54">
+        <v>237.12104500000007</v>
+      </c>
+      <c r="R9" s="53">
         <f t="shared" si="8"/>
-        <v>217.06160000000003</v>
-      </c>
-      <c r="S9" s="54">
+        <v>270.99548000000004</v>
+      </c>
+      <c r="S9" s="53">
         <f t="shared" si="9"/>
-        <v>244.19430000000006</v>
-      </c>
-      <c r="T9" s="54">
+        <v>304.86991500000011</v>
+      </c>
+      <c r="T9" s="53">
         <f t="shared" si="10"/>
-        <v>271.32700000000006</v>
-      </c>
-      <c r="U9" s="55">
+        <v>338.74435000000005</v>
+      </c>
+      <c r="U9" s="54">
         <f t="shared" si="11"/>
-        <v>298.4597</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+        <v>372.61878500000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="6">
         <v>30</v>
       </c>
-      <c r="D10" s="64">
+      <c r="D10" s="63">
         <v>95</v>
       </c>
-      <c r="E10" s="99">
+      <c r="E10" s="98">
         <f t="shared" si="12"/>
-        <v>132.04999999999998</v>
-      </c>
-      <c r="F10" s="99"/>
-      <c r="G10" s="92">
+        <v>109.24999999999999</v>
+      </c>
+      <c r="F10" s="98"/>
+      <c r="G10" s="89">
         <v>126</v>
       </c>
-      <c r="H10" s="65">
+      <c r="H10" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I10" s="73">
         <f t="shared" si="13"/>
-        <v>258.04999999999995</v>
-      </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54">
+        <v>312.88249999999999</v>
+      </c>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53">
         <f t="shared" si="1"/>
-        <v>18.063499999999998</v>
-      </c>
-      <c r="L10" s="54">
+        <v>21.901775000000001</v>
+      </c>
+      <c r="L10" s="53">
         <f t="shared" si="2"/>
-        <v>36.126999999999995</v>
-      </c>
-      <c r="M10" s="54">
+        <v>43.803550000000001</v>
+      </c>
+      <c r="M10" s="53">
         <f t="shared" si="3"/>
-        <v>54.190499999999993</v>
-      </c>
-      <c r="N10" s="54">
+        <v>65.705325000000002</v>
+      </c>
+      <c r="N10" s="53">
         <f t="shared" si="4"/>
-        <v>72.253999999999991</v>
-      </c>
-      <c r="O10" s="54">
+        <v>87.607100000000003</v>
+      </c>
+      <c r="O10" s="53">
         <f t="shared" si="5"/>
-        <v>90.317499999999995</v>
-      </c>
-      <c r="P10" s="54">
+        <v>109.508875</v>
+      </c>
+      <c r="P10" s="53">
         <f t="shared" si="6"/>
-        <v>108.38099999999999</v>
-      </c>
-      <c r="Q10" s="54">
+        <v>131.41065</v>
+      </c>
+      <c r="Q10" s="53">
         <f t="shared" si="7"/>
-        <v>126.44449999999999</v>
-      </c>
-      <c r="R10" s="54">
+        <v>153.31242500000002</v>
+      </c>
+      <c r="R10" s="53">
         <f t="shared" si="8"/>
-        <v>144.50799999999998</v>
-      </c>
-      <c r="S10" s="54">
+        <v>175.21420000000001</v>
+      </c>
+      <c r="S10" s="53">
         <f t="shared" si="9"/>
-        <v>162.57150000000001</v>
-      </c>
-      <c r="T10" s="54">
+        <v>197.11597500000002</v>
+      </c>
+      <c r="T10" s="53">
         <f t="shared" si="10"/>
-        <v>180.63499999999999</v>
-      </c>
-      <c r="U10" s="55">
+        <v>219.01775000000001</v>
+      </c>
+      <c r="U10" s="54">
         <f t="shared" si="11"/>
-        <v>198.69849999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+        <v>240.91952499999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="6">
         <v>30</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="63">
         <v>106</v>
       </c>
-      <c r="E11" s="99">
+      <c r="E11" s="98">
         <f t="shared" si="12"/>
-        <v>147.34</v>
-      </c>
-      <c r="F11" s="99"/>
-      <c r="G11" s="92">
+        <v>121.89999999999999</v>
+      </c>
+      <c r="F11" s="98"/>
+      <c r="G11" s="89">
         <v>118</v>
       </c>
-      <c r="H11" s="65">
+      <c r="H11" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I11" s="73">
         <f t="shared" si="13"/>
-        <v>265.34000000000003</v>
-      </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54">
+        <v>319.06700000000001</v>
+      </c>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53">
         <f t="shared" si="1"/>
-        <v>18.573800000000006</v>
-      </c>
-      <c r="L11" s="54">
+        <v>22.334690000000002</v>
+      </c>
+      <c r="L11" s="53">
         <f t="shared" si="2"/>
-        <v>37.147600000000011</v>
-      </c>
-      <c r="M11" s="54">
+        <v>44.669380000000004</v>
+      </c>
+      <c r="M11" s="53">
         <f t="shared" si="3"/>
-        <v>55.72140000000001</v>
-      </c>
-      <c r="N11" s="54">
+        <v>67.004070000000013</v>
+      </c>
+      <c r="N11" s="53">
         <f t="shared" si="4"/>
-        <v>74.295200000000023</v>
-      </c>
-      <c r="O11" s="54">
+        <v>89.338760000000008</v>
+      </c>
+      <c r="O11" s="53">
         <f t="shared" si="5"/>
-        <v>92.869000000000014</v>
-      </c>
-      <c r="P11" s="54">
+        <v>111.67345000000002</v>
+      </c>
+      <c r="P11" s="53">
         <f t="shared" si="6"/>
-        <v>111.44280000000002</v>
-      </c>
-      <c r="Q11" s="54">
+        <v>134.00814000000003</v>
+      </c>
+      <c r="Q11" s="53">
         <f t="shared" si="7"/>
-        <v>130.01660000000004</v>
-      </c>
-      <c r="R11" s="54">
+        <v>156.34283000000002</v>
+      </c>
+      <c r="R11" s="53">
         <f t="shared" si="8"/>
-        <v>148.59040000000005</v>
-      </c>
-      <c r="S11" s="54">
+        <v>178.67752000000002</v>
+      </c>
+      <c r="S11" s="53">
         <f t="shared" si="9"/>
-        <v>167.16420000000005</v>
-      </c>
-      <c r="T11" s="54">
+        <v>201.01221000000004</v>
+      </c>
+      <c r="T11" s="53">
         <f t="shared" si="10"/>
-        <v>185.73800000000003</v>
-      </c>
-      <c r="U11" s="55">
+        <v>223.34690000000003</v>
+      </c>
+      <c r="U11" s="54">
         <f t="shared" si="11"/>
-        <v>204.31180000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+        <v>245.68159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="64">
+      <c r="D12" s="63">
         <v>111</v>
       </c>
-      <c r="E12" s="99">
+      <c r="E12" s="98">
         <f t="shared" si="12"/>
-        <v>154.29</v>
-      </c>
-      <c r="F12" s="99"/>
-      <c r="G12" s="92">
+        <v>127.64999999999999</v>
+      </c>
+      <c r="F12" s="98"/>
+      <c r="G12" s="89">
         <v>118</v>
       </c>
-      <c r="H12" s="65">
+      <c r="H12" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I12" s="73">
         <f t="shared" si="13"/>
-        <v>272.28999999999996</v>
-      </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54">
+        <v>326.71449999999999</v>
+      </c>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53">
         <f t="shared" si="1"/>
-        <v>19.060299999999998</v>
-      </c>
-      <c r="L12" s="54">
+        <v>22.870015000000002</v>
+      </c>
+      <c r="L12" s="53">
         <f t="shared" si="2"/>
-        <v>38.120599999999996</v>
-      </c>
-      <c r="M12" s="54">
+        <v>45.740030000000004</v>
+      </c>
+      <c r="M12" s="53">
         <f t="shared" si="3"/>
-        <v>57.180900000000001</v>
-      </c>
-      <c r="N12" s="54">
+        <v>68.610045</v>
+      </c>
+      <c r="N12" s="53">
         <f t="shared" si="4"/>
-        <v>76.241199999999992</v>
-      </c>
-      <c r="O12" s="54">
+        <v>91.480060000000009</v>
+      </c>
+      <c r="O12" s="53">
         <f t="shared" si="5"/>
-        <v>95.30149999999999</v>
-      </c>
-      <c r="P12" s="54">
+        <v>114.350075</v>
+      </c>
+      <c r="P12" s="53">
         <f t="shared" si="6"/>
-        <v>114.3618</v>
-      </c>
-      <c r="Q12" s="54">
+        <v>137.22009</v>
+      </c>
+      <c r="Q12" s="53">
         <f t="shared" si="7"/>
-        <v>133.4221</v>
-      </c>
-      <c r="R12" s="54">
+        <v>160.09010500000002</v>
+      </c>
+      <c r="R12" s="53">
         <f t="shared" si="8"/>
-        <v>152.48239999999998</v>
-      </c>
-      <c r="S12" s="54">
+        <v>182.96012000000002</v>
+      </c>
+      <c r="S12" s="53">
         <f t="shared" si="9"/>
-        <v>171.5427</v>
-      </c>
-      <c r="T12" s="54">
+        <v>205.83013500000004</v>
+      </c>
+      <c r="T12" s="53">
         <f t="shared" si="10"/>
-        <v>190.60299999999998</v>
-      </c>
-      <c r="U12" s="55">
+        <v>228.70015000000001</v>
+      </c>
+      <c r="U12" s="54">
         <f t="shared" si="11"/>
-        <v>209.66329999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+        <v>251.570165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="6">
         <v>30</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="63">
         <v>111</v>
       </c>
-      <c r="E13" s="99">
+      <c r="E13" s="98">
         <f t="shared" si="12"/>
-        <v>154.29</v>
-      </c>
-      <c r="F13" s="99"/>
-      <c r="G13" s="92">
+        <v>127.64999999999999</v>
+      </c>
+      <c r="F13" s="98"/>
+      <c r="G13" s="89">
         <v>128</v>
       </c>
-      <c r="H13" s="65">
+      <c r="H13" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I13" s="73">
         <f t="shared" si="13"/>
-        <v>282.28999999999996</v>
-      </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54">
+        <v>340.0145</v>
+      </c>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53">
         <f t="shared" si="1"/>
-        <v>19.760300000000001</v>
-      </c>
-      <c r="L13" s="54">
+        <v>23.801015000000003</v>
+      </c>
+      <c r="L13" s="53">
         <f t="shared" si="2"/>
-        <v>39.520600000000002</v>
-      </c>
-      <c r="M13" s="54">
+        <v>47.602030000000006</v>
+      </c>
+      <c r="M13" s="53">
         <f t="shared" si="3"/>
-        <v>59.280899999999995</v>
-      </c>
-      <c r="N13" s="54">
+        <v>71.403045000000006</v>
+      </c>
+      <c r="N13" s="53">
         <f t="shared" si="4"/>
-        <v>79.041200000000003</v>
-      </c>
-      <c r="O13" s="54">
+        <v>95.204060000000013</v>
+      </c>
+      <c r="O13" s="53">
         <f t="shared" si="5"/>
-        <v>98.80149999999999</v>
-      </c>
-      <c r="P13" s="54">
+        <v>119.00507500000001</v>
+      </c>
+      <c r="P13" s="53">
         <f t="shared" si="6"/>
-        <v>118.56179999999999</v>
-      </c>
-      <c r="Q13" s="54">
+        <v>142.80609000000001</v>
+      </c>
+      <c r="Q13" s="53">
         <f t="shared" si="7"/>
-        <v>138.32210000000001</v>
-      </c>
-      <c r="R13" s="54">
+        <v>166.60710500000002</v>
+      </c>
+      <c r="R13" s="53">
         <f t="shared" si="8"/>
-        <v>158.08240000000001</v>
-      </c>
-      <c r="S13" s="54">
+        <v>190.40812000000003</v>
+      </c>
+      <c r="S13" s="53">
         <f t="shared" si="9"/>
-        <v>177.84270000000001</v>
-      </c>
-      <c r="T13" s="54">
+        <v>214.20913500000003</v>
+      </c>
+      <c r="T13" s="53">
         <f t="shared" si="10"/>
-        <v>197.60299999999998</v>
-      </c>
-      <c r="U13" s="55">
+        <v>238.01015000000001</v>
+      </c>
+      <c r="U13" s="54">
         <f t="shared" si="11"/>
-        <v>217.36329999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+        <v>261.81116500000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A14" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="49" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="6">
         <v>30</v>
       </c>
-      <c r="D14" s="64">
+      <c r="D14" s="63">
         <v>110</v>
       </c>
-      <c r="E14" s="99">
+      <c r="E14" s="98">
         <f t="shared" si="12"/>
-        <v>152.89999999999998</v>
-      </c>
-      <c r="F14" s="99"/>
-      <c r="G14" s="92">
+        <v>126.49999999999999</v>
+      </c>
+      <c r="F14" s="98"/>
+      <c r="G14" s="89">
         <v>131</v>
       </c>
-      <c r="H14" s="65">
+      <c r="H14" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I14" s="73">
         <f t="shared" si="13"/>
-        <v>283.89999999999998</v>
-      </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54">
+        <v>342.47500000000002</v>
+      </c>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53">
         <f t="shared" si="1"/>
-        <v>19.873000000000001</v>
-      </c>
-      <c r="L14" s="54">
+        <v>23.973250000000004</v>
+      </c>
+      <c r="L14" s="53">
         <f t="shared" si="2"/>
-        <v>39.746000000000002</v>
-      </c>
-      <c r="M14" s="54">
+        <v>47.946500000000007</v>
+      </c>
+      <c r="M14" s="53">
         <f t="shared" si="3"/>
-        <v>59.619</v>
-      </c>
-      <c r="N14" s="54">
+        <v>71.919750000000008</v>
+      </c>
+      <c r="N14" s="53">
         <f t="shared" si="4"/>
-        <v>79.492000000000004</v>
-      </c>
-      <c r="O14" s="54">
+        <v>95.893000000000015</v>
+      </c>
+      <c r="O14" s="53">
         <f t="shared" si="5"/>
-        <v>99.364999999999995</v>
-      </c>
-      <c r="P14" s="54">
+        <v>119.86625000000002</v>
+      </c>
+      <c r="P14" s="53">
         <f t="shared" si="6"/>
-        <v>119.238</v>
-      </c>
-      <c r="Q14" s="54">
+        <v>143.83950000000002</v>
+      </c>
+      <c r="Q14" s="53">
         <f t="shared" si="7"/>
-        <v>139.11099999999999</v>
-      </c>
-      <c r="R14" s="54">
+        <v>167.81275000000002</v>
+      </c>
+      <c r="R14" s="53">
         <f t="shared" si="8"/>
-        <v>158.98400000000001</v>
-      </c>
-      <c r="S14" s="54">
+        <v>191.78600000000003</v>
+      </c>
+      <c r="S14" s="53">
         <f t="shared" si="9"/>
-        <v>178.85700000000003</v>
-      </c>
-      <c r="T14" s="54">
+        <v>215.75925000000007</v>
+      </c>
+      <c r="T14" s="53">
         <f t="shared" si="10"/>
-        <v>198.73</v>
-      </c>
-      <c r="U14" s="55">
+        <v>239.73250000000004</v>
+      </c>
+      <c r="U14" s="54">
         <f t="shared" si="11"/>
-        <v>218.60299999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+        <v>263.70575000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="49" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="64">
+      <c r="D15" s="63">
         <v>99</v>
       </c>
-      <c r="E15" s="99">
+      <c r="E15" s="98">
         <f t="shared" si="12"/>
-        <v>137.60999999999999</v>
-      </c>
-      <c r="F15" s="99"/>
-      <c r="G15" s="92">
+        <v>113.85</v>
+      </c>
+      <c r="F15" s="98"/>
+      <c r="G15" s="89">
         <v>100</v>
       </c>
-      <c r="H15" s="65">
+      <c r="H15" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I15" s="73">
         <f t="shared" si="13"/>
-        <v>237.60999999999999</v>
-      </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54">
+        <v>284.4205</v>
+      </c>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53">
         <f t="shared" si="1"/>
-        <v>16.6327</v>
-      </c>
-      <c r="L15" s="54">
+        <v>19.909435000000002</v>
+      </c>
+      <c r="L15" s="53">
         <f t="shared" si="2"/>
-        <v>33.2654</v>
-      </c>
-      <c r="M15" s="54">
+        <v>39.818870000000004</v>
+      </c>
+      <c r="M15" s="53">
         <f t="shared" si="3"/>
-        <v>49.898099999999999</v>
-      </c>
-      <c r="N15" s="54">
+        <v>59.728305000000006</v>
+      </c>
+      <c r="N15" s="53">
         <f t="shared" si="4"/>
-        <v>66.530799999999999</v>
-      </c>
-      <c r="O15" s="54">
+        <v>79.637740000000008</v>
+      </c>
+      <c r="O15" s="53">
         <f t="shared" si="5"/>
-        <v>83.163499999999999</v>
-      </c>
-      <c r="P15" s="54">
+        <v>99.54717500000001</v>
+      </c>
+      <c r="P15" s="53">
         <f t="shared" si="6"/>
-        <v>99.796199999999999</v>
-      </c>
-      <c r="Q15" s="54">
+        <v>119.45661000000001</v>
+      </c>
+      <c r="Q15" s="53">
         <f t="shared" si="7"/>
-        <v>116.4289</v>
-      </c>
-      <c r="R15" s="54">
+        <v>139.36604500000001</v>
+      </c>
+      <c r="R15" s="53">
         <f t="shared" si="8"/>
-        <v>133.0616</v>
-      </c>
-      <c r="S15" s="54">
+        <v>159.27548000000002</v>
+      </c>
+      <c r="S15" s="53">
         <f t="shared" si="9"/>
-        <v>149.69430000000003</v>
-      </c>
-      <c r="T15" s="54">
+        <v>179.18491500000005</v>
+      </c>
+      <c r="T15" s="53">
         <f t="shared" si="10"/>
-        <v>166.327</v>
-      </c>
-      <c r="U15" s="55">
+        <v>199.09435000000002</v>
+      </c>
+      <c r="U15" s="54">
         <f t="shared" si="11"/>
-        <v>182.9597</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+        <v>219.00378500000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A16" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="89">
+      <c r="C16" s="86">
         <v>50</v>
       </c>
-      <c r="D16" s="64">
+      <c r="D16" s="63">
         <v>108</v>
       </c>
-      <c r="E16" s="99">
+      <c r="E16" s="98">
         <f t="shared" si="12"/>
-        <v>150.11999999999998</v>
-      </c>
-      <c r="F16" s="99"/>
-      <c r="G16" s="92">
+        <v>124.19999999999999</v>
+      </c>
+      <c r="F16" s="98"/>
+      <c r="G16" s="89">
         <v>100</v>
       </c>
-      <c r="H16" s="65">
+      <c r="H16" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I16" s="73">
         <f t="shared" si="13"/>
-        <v>250.11999999999998</v>
-      </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54">
+        <v>298.18599999999998</v>
+      </c>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53">
         <f t="shared" si="1"/>
-        <v>17.508400000000002</v>
-      </c>
-      <c r="L16" s="54">
+        <v>20.87302</v>
+      </c>
+      <c r="L16" s="53">
         <f t="shared" si="2"/>
-        <v>35.016800000000003</v>
-      </c>
-      <c r="M16" s="54">
+        <v>41.746040000000001</v>
+      </c>
+      <c r="M16" s="53">
         <f t="shared" si="3"/>
-        <v>52.525199999999998</v>
-      </c>
-      <c r="N16" s="54">
+        <v>62.619060000000005</v>
+      </c>
+      <c r="N16" s="53">
         <f t="shared" si="4"/>
-        <v>70.033600000000007</v>
-      </c>
-      <c r="O16" s="54">
+        <v>83.492080000000001</v>
+      </c>
+      <c r="O16" s="53">
         <f t="shared" si="5"/>
-        <v>87.542000000000002</v>
-      </c>
-      <c r="P16" s="54">
+        <v>104.3651</v>
+      </c>
+      <c r="P16" s="53">
         <f t="shared" si="6"/>
-        <v>105.0504</v>
-      </c>
-      <c r="Q16" s="54">
+        <v>125.23812000000001</v>
+      </c>
+      <c r="Q16" s="53">
         <f t="shared" si="7"/>
-        <v>122.55880000000001</v>
-      </c>
-      <c r="R16" s="54">
+        <v>146.11114000000001</v>
+      </c>
+      <c r="R16" s="53">
         <f t="shared" si="8"/>
-        <v>140.06720000000001</v>
-      </c>
-      <c r="S16" s="54">
+        <v>166.98416</v>
+      </c>
+      <c r="S16" s="53">
         <f t="shared" si="9"/>
-        <v>157.57560000000001</v>
-      </c>
-      <c r="T16" s="54">
+        <v>187.85718000000003</v>
+      </c>
+      <c r="T16" s="53">
         <f t="shared" si="10"/>
-        <v>175.084</v>
-      </c>
-      <c r="U16" s="55">
+        <v>208.7302</v>
+      </c>
+      <c r="U16" s="54">
         <f t="shared" si="11"/>
-        <v>192.5924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+        <v>229.60321999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A17" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="89">
+      <c r="C17" s="86">
         <v>20</v>
       </c>
-      <c r="D17" s="64">
+      <c r="D17" s="63">
         <v>105</v>
       </c>
-      <c r="E17" s="99">
+      <c r="E17" s="98">
         <f t="shared" si="12"/>
-        <v>145.94999999999999</v>
-      </c>
-      <c r="F17" s="99"/>
-      <c r="G17" s="92">
+        <v>120.74999999999999</v>
+      </c>
+      <c r="F17" s="98"/>
+      <c r="G17" s="89">
         <v>122</v>
       </c>
-      <c r="H17" s="65">
+      <c r="H17" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I17" s="73">
         <f t="shared" si="13"/>
-        <v>267.95</v>
-      </c>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54">
+        <v>322.85750000000002</v>
+      </c>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53">
         <f t="shared" si="1"/>
-        <v>18.756500000000003</v>
-      </c>
-      <c r="L17" s="54">
+        <v>22.600025000000002</v>
+      </c>
+      <c r="L17" s="53">
         <f t="shared" si="2"/>
-        <v>37.513000000000005</v>
-      </c>
-      <c r="M17" s="54">
+        <v>45.200050000000005</v>
+      </c>
+      <c r="M17" s="53">
         <f t="shared" si="3"/>
-        <v>56.269500000000001</v>
-      </c>
-      <c r="N17" s="54">
+        <v>67.800075000000007</v>
+      </c>
+      <c r="N17" s="53">
         <f t="shared" si="4"/>
-        <v>75.02600000000001</v>
-      </c>
-      <c r="O17" s="54">
+        <v>90.400100000000009</v>
+      </c>
+      <c r="O17" s="53">
         <f t="shared" si="5"/>
-        <v>93.782499999999999</v>
-      </c>
-      <c r="P17" s="54">
+        <v>113.00012500000001</v>
+      </c>
+      <c r="P17" s="53">
         <f t="shared" si="6"/>
-        <v>112.539</v>
-      </c>
-      <c r="Q17" s="54">
+        <v>135.60015000000001</v>
+      </c>
+      <c r="Q17" s="53">
         <f t="shared" si="7"/>
-        <v>131.2955</v>
-      </c>
-      <c r="R17" s="54">
+        <v>158.20017500000003</v>
+      </c>
+      <c r="R17" s="53">
         <f t="shared" si="8"/>
-        <v>150.05200000000002</v>
-      </c>
-      <c r="S17" s="54">
+        <v>180.80020000000002</v>
+      </c>
+      <c r="S17" s="53">
         <f t="shared" si="9"/>
-        <v>168.80850000000004</v>
-      </c>
-      <c r="T17" s="54">
+        <v>203.40022500000003</v>
+      </c>
+      <c r="T17" s="53">
         <f t="shared" si="10"/>
-        <v>187.565</v>
-      </c>
-      <c r="U17" s="55">
+        <v>226.00025000000002</v>
+      </c>
+      <c r="U17" s="54">
         <f t="shared" si="11"/>
-        <v>206.32149999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="53" t="s">
+        <v>248.60027500000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A18" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="89">
+      <c r="C18" s="86">
         <v>20</v>
       </c>
-      <c r="D18" s="64">
+      <c r="D18" s="63">
         <v>97</v>
       </c>
-      <c r="E18" s="99">
+      <c r="E18" s="98">
         <f t="shared" si="12"/>
-        <v>134.82999999999998</v>
-      </c>
-      <c r="F18" s="99"/>
-      <c r="G18" s="92">
+        <v>111.55</v>
+      </c>
+      <c r="F18" s="98"/>
+      <c r="G18" s="89">
         <v>88</v>
       </c>
-      <c r="H18" s="65">
+      <c r="H18" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="75">
+        <v>0.33</v>
+      </c>
+      <c r="I18" s="73">
         <f t="shared" si="13"/>
-        <v>222.82999999999998</v>
-      </c>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54">
+        <v>265.40150000000006</v>
+      </c>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53">
         <f t="shared" si="1"/>
-        <v>15.598100000000001</v>
-      </c>
-      <c r="L18" s="54">
+        <v>18.578105000000004</v>
+      </c>
+      <c r="L18" s="53">
         <f t="shared" si="2"/>
-        <v>31.196200000000001</v>
-      </c>
-      <c r="M18" s="54">
+        <v>37.156210000000009</v>
+      </c>
+      <c r="M18" s="53">
         <f t="shared" si="3"/>
-        <v>46.7943</v>
-      </c>
-      <c r="N18" s="54">
+        <v>55.734315000000016</v>
+      </c>
+      <c r="N18" s="53">
         <f t="shared" si="4"/>
-        <v>62.392400000000002</v>
-      </c>
-      <c r="O18" s="54">
+        <v>74.312420000000017</v>
+      </c>
+      <c r="O18" s="53">
         <f t="shared" si="5"/>
-        <v>77.990499999999997</v>
-      </c>
-      <c r="P18" s="54">
+        <v>92.890525000000025</v>
+      </c>
+      <c r="P18" s="53">
         <f t="shared" si="6"/>
-        <v>93.5886</v>
-      </c>
-      <c r="Q18" s="54">
+        <v>111.46863000000003</v>
+      </c>
+      <c r="Q18" s="53">
         <f t="shared" si="7"/>
-        <v>109.1867</v>
-      </c>
-      <c r="R18" s="54">
+        <v>130.04673500000004</v>
+      </c>
+      <c r="R18" s="53">
         <f t="shared" si="8"/>
-        <v>124.7848</v>
-      </c>
-      <c r="S18" s="54">
+        <v>148.62484000000003</v>
+      </c>
+      <c r="S18" s="53">
         <f t="shared" si="9"/>
-        <v>140.38290000000001</v>
-      </c>
-      <c r="T18" s="54">
+        <v>167.20294500000006</v>
+      </c>
+      <c r="T18" s="53">
         <f t="shared" si="10"/>
-        <v>155.98099999999999</v>
-      </c>
-      <c r="U18" s="55">
+        <v>185.78105000000005</v>
+      </c>
+      <c r="U18" s="54">
         <f t="shared" si="11"/>
-        <v>171.57909999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+        <v>204.35915500000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="6">
         <v>30</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="63">
         <v>106</v>
       </c>
-      <c r="E19" s="99">
+      <c r="E19" s="98">
         <f t="shared" si="12"/>
-        <v>147.34</v>
-      </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="92">
+        <v>121.89999999999999</v>
+      </c>
+      <c r="F19" s="98"/>
+      <c r="G19" s="89">
         <v>85</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="105">
         <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="I19" s="73">
+        <f t="shared" si="13"/>
+        <v>275.17699999999996</v>
+      </c>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53">
+        <f t="shared" si="1"/>
+        <v>19.26239</v>
+      </c>
+      <c r="L19" s="53">
+        <f t="shared" si="2"/>
+        <v>38.52478</v>
+      </c>
+      <c r="M19" s="53">
+        <f t="shared" si="3"/>
+        <v>57.787169999999996</v>
+      </c>
+      <c r="N19" s="53">
+        <f t="shared" si="4"/>
+        <v>77.04956</v>
+      </c>
+      <c r="O19" s="53">
+        <f t="shared" si="5"/>
+        <v>96.311949999999996</v>
+      </c>
+      <c r="P19" s="53">
+        <f t="shared" si="6"/>
+        <v>115.57433999999999</v>
+      </c>
+      <c r="Q19" s="53">
+        <f t="shared" si="7"/>
+        <v>134.83672999999999</v>
+      </c>
+      <c r="R19" s="53">
+        <f t="shared" si="8"/>
+        <v>154.09912</v>
+      </c>
+      <c r="S19" s="53">
+        <f t="shared" si="9"/>
+        <v>173.36151000000001</v>
+      </c>
+      <c r="T19" s="53">
+        <f t="shared" si="10"/>
+        <v>192.62389999999999</v>
+      </c>
+      <c r="U19" s="54">
+        <f t="shared" si="11"/>
+        <v>211.88628999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="63">
+        <v>98</v>
+      </c>
+      <c r="E20" s="98">
+        <f t="shared" si="12"/>
+        <v>112.69999999999999</v>
+      </c>
+      <c r="F20" s="98"/>
+      <c r="G20" s="89">
+        <v>85</v>
+      </c>
+      <c r="H20" s="105">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="I20" s="73">
+        <f t="shared" si="13"/>
+        <v>262.94099999999997</v>
+      </c>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53">
+        <f t="shared" si="1"/>
+        <v>18.40587</v>
+      </c>
+      <c r="L20" s="53">
+        <f t="shared" si="2"/>
+        <v>36.81174</v>
+      </c>
+      <c r="M20" s="53">
+        <f t="shared" si="3"/>
+        <v>55.217610000000001</v>
+      </c>
+      <c r="N20" s="53">
+        <f t="shared" si="4"/>
+        <v>73.623480000000001</v>
+      </c>
+      <c r="O20" s="53">
+        <f t="shared" si="5"/>
+        <v>92.029349999999994</v>
+      </c>
+      <c r="P20" s="53">
+        <f t="shared" si="6"/>
+        <v>110.43522</v>
+      </c>
+      <c r="Q20" s="53">
+        <f t="shared" si="7"/>
+        <v>128.84109000000001</v>
+      </c>
+      <c r="R20" s="53">
+        <f t="shared" si="8"/>
+        <v>147.24696</v>
+      </c>
+      <c r="S20" s="53">
+        <f t="shared" si="9"/>
+        <v>165.65283000000002</v>
+      </c>
+      <c r="T20" s="53">
+        <f t="shared" si="10"/>
+        <v>184.05869999999999</v>
+      </c>
+      <c r="U20" s="54">
+        <f t="shared" si="11"/>
+        <v>202.46456999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="76"/>
+      <c r="D21" s="77">
+        <v>87</v>
+      </c>
+      <c r="E21" s="102">
+        <f t="shared" si="12"/>
+        <v>100.05</v>
+      </c>
+      <c r="F21" s="102"/>
+      <c r="G21" s="90">
         <v>0</v>
       </c>
-      <c r="I19" s="75">
+      <c r="H21" s="106">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="I21" s="78">
         <f t="shared" si="13"/>
-        <v>232.34</v>
-      </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54">
+        <v>133.06649999999999</v>
+      </c>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55">
         <f t="shared" si="1"/>
-        <v>16.263800000000003</v>
-      </c>
-      <c r="L19" s="54">
+        <v>9.3146550000000001</v>
+      </c>
+      <c r="L21" s="55">
         <f t="shared" si="2"/>
-        <v>32.527600000000007</v>
-      </c>
-      <c r="M19" s="54">
+        <v>18.62931</v>
+      </c>
+      <c r="M21" s="55">
         <f t="shared" si="3"/>
-        <v>48.791400000000003</v>
-      </c>
-      <c r="N19" s="54">
+        <v>27.943965000000002</v>
+      </c>
+      <c r="N21" s="55">
         <f t="shared" si="4"/>
-        <v>65.055200000000013</v>
-      </c>
-      <c r="O19" s="54">
+        <v>37.258620000000001</v>
+      </c>
+      <c r="O21" s="55">
         <f t="shared" si="5"/>
-        <v>81.319000000000003</v>
-      </c>
-      <c r="P19" s="54">
+        <v>46.573275000000002</v>
+      </c>
+      <c r="P21" s="55">
         <f t="shared" si="6"/>
-        <v>97.582800000000006</v>
-      </c>
-      <c r="Q19" s="54">
+        <v>55.887930000000004</v>
+      </c>
+      <c r="Q21" s="55">
         <f t="shared" si="7"/>
-        <v>113.84660000000001</v>
-      </c>
-      <c r="R19" s="54">
+        <v>65.202584999999999</v>
+      </c>
+      <c r="R21" s="55">
         <f t="shared" si="8"/>
-        <v>130.11040000000003</v>
-      </c>
-      <c r="S19" s="54">
+        <v>74.517240000000001</v>
+      </c>
+      <c r="S21" s="55">
         <f t="shared" si="9"/>
-        <v>146.37420000000003</v>
-      </c>
-      <c r="T19" s="54">
+        <v>83.831895000000003</v>
+      </c>
+      <c r="T21" s="55">
         <f t="shared" si="10"/>
-        <v>162.63800000000001</v>
-      </c>
-      <c r="U19" s="55">
+        <v>93.146550000000005</v>
+      </c>
+      <c r="U21" s="56">
         <f t="shared" si="11"/>
-        <v>178.90180000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="64">
-        <v>98</v>
-      </c>
-      <c r="E20" s="99">
-        <f t="shared" si="12"/>
-        <v>136.22</v>
-      </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="92">
-        <v>85</v>
-      </c>
-      <c r="H20" s="65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="75">
-        <f t="shared" si="13"/>
-        <v>221.22</v>
-      </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54">
-        <f t="shared" si="1"/>
-        <v>15.485400000000002</v>
-      </c>
-      <c r="L20" s="54">
-        <f t="shared" si="2"/>
-        <v>30.970800000000004</v>
-      </c>
-      <c r="M20" s="54">
-        <f t="shared" si="3"/>
-        <v>46.456200000000003</v>
-      </c>
-      <c r="N20" s="54">
-        <f t="shared" si="4"/>
-        <v>61.941600000000008</v>
-      </c>
-      <c r="O20" s="54">
-        <f t="shared" si="5"/>
-        <v>77.427000000000007</v>
-      </c>
-      <c r="P20" s="54">
-        <f t="shared" si="6"/>
-        <v>92.912400000000005</v>
-      </c>
-      <c r="Q20" s="54">
-        <f t="shared" si="7"/>
-        <v>108.3978</v>
-      </c>
-      <c r="R20" s="54">
-        <f t="shared" si="8"/>
-        <v>123.88320000000002</v>
-      </c>
-      <c r="S20" s="54">
-        <f t="shared" si="9"/>
-        <v>139.36860000000001</v>
-      </c>
-      <c r="T20" s="54">
-        <f t="shared" si="10"/>
-        <v>154.85400000000001</v>
-      </c>
-      <c r="U20" s="55">
-        <f t="shared" si="11"/>
-        <v>170.33940000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="76" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="77" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="79">
-        <v>87</v>
-      </c>
-      <c r="E21" s="100">
-        <f t="shared" si="12"/>
-        <v>120.92999999999999</v>
-      </c>
-      <c r="F21" s="100"/>
-      <c r="G21" s="93">
-        <v>0</v>
-      </c>
-      <c r="H21" s="80">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="81">
-        <f t="shared" si="13"/>
-        <v>120.92999999999999</v>
-      </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56">
-        <f t="shared" si="1"/>
-        <v>8.4650999999999996</v>
-      </c>
-      <c r="L21" s="56">
-        <f t="shared" si="2"/>
-        <v>16.930199999999999</v>
-      </c>
-      <c r="M21" s="56">
-        <f t="shared" si="3"/>
-        <v>25.395300000000002</v>
-      </c>
-      <c r="N21" s="56">
-        <f t="shared" si="4"/>
-        <v>33.860399999999998</v>
-      </c>
-      <c r="O21" s="56">
-        <f t="shared" si="5"/>
-        <v>42.325499999999998</v>
-      </c>
-      <c r="P21" s="56">
-        <f t="shared" si="6"/>
-        <v>50.790600000000005</v>
-      </c>
-      <c r="Q21" s="56">
-        <f t="shared" si="7"/>
-        <v>59.255700000000004</v>
-      </c>
-      <c r="R21" s="56">
-        <f t="shared" si="8"/>
-        <v>67.720799999999997</v>
-      </c>
-      <c r="S21" s="56">
-        <f t="shared" si="9"/>
-        <v>76.185900000000004</v>
-      </c>
-      <c r="T21" s="56">
-        <f t="shared" si="10"/>
-        <v>84.650999999999996</v>
-      </c>
-      <c r="U21" s="57">
-        <f t="shared" si="11"/>
-        <v>93.116100000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:21" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="35" t="s">
+        <v>102.46120499999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="1:21" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="46"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="30" t="s">
+      <c r="C24" s="45"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="29" t="s">
         <v>26</v>
       </c>
       <c r="J24" s="15"/>
@@ -2690,27 +2696,27 @@
       <c r="T24" s="16"/>
       <c r="U24" s="17"/>
     </row>
-    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="38" t="s">
+    <row r="25" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="31">
+      <c r="C25" s="32"/>
+      <c r="D25" s="30">
         <v>0</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="38" t="s">
         <v>21</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="28" t="s">
+      <c r="J25" s="27" t="s">
         <v>15</v>
       </c>
       <c r="K25" s="13">
@@ -2747,11 +2753,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="40" t="s">
+    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="47"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="14">
         <v>0.15</v>
       </c>
@@ -2761,438 +2767,438 @@
       <c r="F26" s="14">
         <v>205</v>
       </c>
-      <c r="G26" s="42">
+      <c r="G26" s="41">
         <f>SUM(F26-(E26*(1+D25+D26)))</f>
         <v>85.4</v>
       </c>
-      <c r="I26" s="24">
+      <c r="I26" s="23">
         <v>1429</v>
       </c>
-      <c r="J26" s="25"/>
-      <c r="K26" s="95">
+      <c r="J26" s="24"/>
+      <c r="K26" s="92">
         <f>SUM($I26*(0.07*1))</f>
         <v>100.03000000000002</v>
       </c>
-      <c r="L26" s="58">
+      <c r="L26" s="57">
         <f>SUM($I26*(0.07*2))</f>
         <v>200.06000000000003</v>
       </c>
-      <c r="M26" s="58">
+      <c r="M26" s="57">
         <f>SUM($I26*(0.07*3))</f>
         <v>300.09000000000003</v>
       </c>
-      <c r="N26" s="58">
+      <c r="N26" s="57">
         <f>SUM($I26*(0.07*4))</f>
         <v>400.12000000000006</v>
       </c>
-      <c r="O26" s="58">
+      <c r="O26" s="57">
         <f>SUM($I26*(0.07*5))</f>
         <v>500.15000000000003</v>
       </c>
-      <c r="P26" s="58">
+      <c r="P26" s="57">
         <f>SUM($I26*(0.07*6))</f>
         <v>600.18000000000006</v>
       </c>
-      <c r="Q26" s="58">
+      <c r="Q26" s="57">
         <f>SUM($I26*(0.07*7))</f>
         <v>700.21</v>
       </c>
-      <c r="R26" s="58">
+      <c r="R26" s="57">
         <f>SUM($I26*(0.07*8))</f>
         <v>800.24000000000012</v>
       </c>
-      <c r="S26" s="58">
+      <c r="S26" s="57">
         <f>SUM($I26*(0.07*9))</f>
         <v>900.27000000000021</v>
       </c>
-      <c r="T26" s="58">
+      <c r="T26" s="57">
         <f>SUM($I26*(0.07*10))</f>
         <v>1000.3000000000001</v>
       </c>
-      <c r="U26" s="59">
+      <c r="U26" s="58">
         <f>SUM($I26*(0.07*11))</f>
         <v>1100.33</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
+    <row r="27" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="I27" s="24">
+      <c r="I27" s="23">
         <v>715</v>
       </c>
-      <c r="J27" s="25"/>
-      <c r="K27" s="58">
+      <c r="J27" s="24"/>
+      <c r="K27" s="57">
         <f t="shared" ref="K27:K53" si="14">SUM($I27*(0.07*1))</f>
         <v>50.050000000000004</v>
       </c>
-      <c r="L27" s="95">
+      <c r="L27" s="92">
         <f t="shared" ref="L27:L53" si="15">SUM($I27*(0.07*2))</f>
         <v>100.10000000000001</v>
       </c>
-      <c r="M27" s="58">
+      <c r="M27" s="57">
         <f t="shared" ref="M27:M53" si="16">SUM($I27*(0.07*3))</f>
         <v>150.15</v>
       </c>
-      <c r="N27" s="58">
+      <c r="N27" s="57">
         <f t="shared" ref="N27:N53" si="17">SUM($I27*(0.07*4))</f>
         <v>200.20000000000002</v>
       </c>
-      <c r="O27" s="58">
+      <c r="O27" s="57">
         <f t="shared" ref="O27:O53" si="18">SUM($I27*(0.07*5))</f>
         <v>250.25000000000003</v>
       </c>
-      <c r="P27" s="58">
+      <c r="P27" s="57">
         <f t="shared" ref="P27:P53" si="19">SUM($I27*(0.07*6))</f>
         <v>300.3</v>
       </c>
-      <c r="Q27" s="58">
+      <c r="Q27" s="57">
         <f t="shared" ref="Q27:Q53" si="20">SUM($I27*(0.07*7))</f>
         <v>350.35</v>
       </c>
-      <c r="R27" s="58">
+      <c r="R27" s="57">
         <f t="shared" ref="R27:R53" si="21">SUM($I27*(0.07*8))</f>
         <v>400.40000000000003</v>
       </c>
-      <c r="S27" s="58">
+      <c r="S27" s="57">
         <f t="shared" ref="S27:S53" si="22">SUM($I27*(0.07*9))</f>
         <v>450.4500000000001</v>
       </c>
-      <c r="T27" s="58">
+      <c r="T27" s="57">
         <f t="shared" ref="T27:T53" si="23">SUM($I27*(0.07*10))</f>
         <v>500.50000000000006</v>
       </c>
-      <c r="U27" s="59">
+      <c r="U27" s="58">
         <f t="shared" ref="U27:U53" si="24">SUM($I27*(0.07*11))</f>
         <v>550.55000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="24">
+    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="23">
         <v>477</v>
       </c>
-      <c r="J28" s="25"/>
-      <c r="K28" s="58">
+      <c r="J28" s="24"/>
+      <c r="K28" s="57">
         <f t="shared" si="14"/>
         <v>33.39</v>
       </c>
-      <c r="L28" s="58">
+      <c r="L28" s="57">
         <f t="shared" si="15"/>
         <v>66.78</v>
       </c>
-      <c r="M28" s="95">
+      <c r="M28" s="92">
         <f t="shared" si="16"/>
         <v>100.17000000000002</v>
       </c>
-      <c r="N28" s="58">
+      <c r="N28" s="57">
         <f t="shared" si="17"/>
         <v>133.56</v>
       </c>
-      <c r="O28" s="58">
+      <c r="O28" s="57">
         <f t="shared" si="18"/>
         <v>166.95000000000002</v>
       </c>
-      <c r="P28" s="58">
+      <c r="P28" s="57">
         <f t="shared" si="19"/>
         <v>200.34000000000003</v>
       </c>
-      <c r="Q28" s="58">
+      <c r="Q28" s="57">
         <f t="shared" si="20"/>
         <v>233.73000000000002</v>
       </c>
-      <c r="R28" s="58">
+      <c r="R28" s="57">
         <f t="shared" si="21"/>
         <v>267.12</v>
       </c>
-      <c r="S28" s="58">
+      <c r="S28" s="57">
         <f t="shared" si="22"/>
         <v>300.51000000000005</v>
       </c>
-      <c r="T28" s="58">
+      <c r="T28" s="57">
         <f t="shared" si="23"/>
         <v>333.90000000000003</v>
       </c>
-      <c r="U28" s="59">
+      <c r="U28" s="58">
         <f t="shared" si="24"/>
         <v>367.29</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="35" t="s">
+    <row r="29" spans="1:21" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="I29" s="24">
+      <c r="C29" s="45"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="36"/>
+      <c r="I29" s="23">
         <v>358</v>
       </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="58">
+      <c r="J29" s="24"/>
+      <c r="K29" s="57">
         <f t="shared" si="14"/>
         <v>25.060000000000002</v>
       </c>
-      <c r="L29" s="58">
+      <c r="L29" s="57">
         <f t="shared" si="15"/>
         <v>50.120000000000005</v>
       </c>
-      <c r="M29" s="58">
+      <c r="M29" s="57">
         <f t="shared" si="16"/>
         <v>75.180000000000007</v>
       </c>
-      <c r="N29" s="95">
+      <c r="N29" s="92">
         <f t="shared" si="17"/>
         <v>100.24000000000001</v>
       </c>
-      <c r="O29" s="58">
+      <c r="O29" s="57">
         <f t="shared" si="18"/>
         <v>125.30000000000001</v>
       </c>
-      <c r="P29" s="58">
+      <c r="P29" s="57">
         <f t="shared" si="19"/>
         <v>150.36000000000001</v>
       </c>
-      <c r="Q29" s="58">
+      <c r="Q29" s="57">
         <f t="shared" si="20"/>
         <v>175.42000000000002</v>
       </c>
-      <c r="R29" s="58">
+      <c r="R29" s="57">
         <f t="shared" si="21"/>
         <v>200.48000000000002</v>
       </c>
-      <c r="S29" s="58">
+      <c r="S29" s="57">
         <f t="shared" si="22"/>
         <v>225.54000000000005</v>
       </c>
-      <c r="T29" s="58">
+      <c r="T29" s="57">
         <f t="shared" si="23"/>
         <v>250.60000000000002</v>
       </c>
-      <c r="U29" s="59">
+      <c r="U29" s="58">
         <f t="shared" si="24"/>
         <v>275.66000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B30" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="44"/>
-      <c r="I30" s="24">
+      <c r="C30" s="47"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="43"/>
+      <c r="I30" s="23">
         <v>290</v>
       </c>
-      <c r="J30" s="25"/>
-      <c r="K30" s="58">
+      <c r="J30" s="24"/>
+      <c r="K30" s="57">
         <f t="shared" si="14"/>
         <v>20.3</v>
       </c>
-      <c r="L30" s="58">
+      <c r="L30" s="57">
         <f t="shared" si="15"/>
         <v>40.6</v>
       </c>
-      <c r="M30" s="58">
+      <c r="M30" s="57">
         <f t="shared" si="16"/>
         <v>60.900000000000006</v>
       </c>
-      <c r="N30" s="58">
+      <c r="N30" s="57">
         <f t="shared" si="17"/>
         <v>81.2</v>
       </c>
-      <c r="O30" s="58">
+      <c r="O30" s="57">
         <f t="shared" si="18"/>
         <v>101.50000000000001</v>
       </c>
-      <c r="P30" s="58">
+      <c r="P30" s="57">
         <f t="shared" si="19"/>
         <v>121.80000000000001</v>
       </c>
-      <c r="Q30" s="58">
+      <c r="Q30" s="57">
         <f t="shared" si="20"/>
         <v>142.10000000000002</v>
       </c>
-      <c r="R30" s="58">
+      <c r="R30" s="57">
         <f t="shared" si="21"/>
         <v>162.4</v>
       </c>
-      <c r="S30" s="58">
+      <c r="S30" s="57">
         <f t="shared" si="22"/>
         <v>182.70000000000005</v>
       </c>
-      <c r="T30" s="58">
+      <c r="T30" s="57">
         <f t="shared" si="23"/>
         <v>203.00000000000003</v>
       </c>
-      <c r="U30" s="59">
+      <c r="U30" s="58">
         <f t="shared" si="24"/>
         <v>223.3</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B31" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="44"/>
-      <c r="I31" s="24">
+      <c r="C31" s="47"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="43"/>
+      <c r="I31" s="23">
         <v>286</v>
       </c>
-      <c r="J31" s="25"/>
-      <c r="K31" s="58">
+      <c r="J31" s="24"/>
+      <c r="K31" s="57">
         <f t="shared" si="14"/>
         <v>20.020000000000003</v>
       </c>
-      <c r="L31" s="58">
+      <c r="L31" s="57">
         <f t="shared" si="15"/>
         <v>40.040000000000006</v>
       </c>
-      <c r="M31" s="58">
+      <c r="M31" s="57">
         <f t="shared" si="16"/>
         <v>60.06</v>
       </c>
-      <c r="N31" s="95">
+      <c r="N31" s="92">
         <f t="shared" si="17"/>
         <v>80.080000000000013</v>
       </c>
-      <c r="O31" s="95">
+      <c r="O31" s="92">
         <f t="shared" si="18"/>
         <v>100.10000000000001</v>
       </c>
-      <c r="P31" s="58">
+      <c r="P31" s="57">
         <f t="shared" si="19"/>
         <v>120.12</v>
       </c>
-      <c r="Q31" s="58">
+      <c r="Q31" s="57">
         <f t="shared" si="20"/>
         <v>140.14000000000001</v>
       </c>
-      <c r="R31" s="58">
+      <c r="R31" s="57">
         <f t="shared" si="21"/>
         <v>160.16000000000003</v>
       </c>
-      <c r="S31" s="58">
+      <c r="S31" s="57">
         <f t="shared" si="22"/>
         <v>180.18000000000004</v>
       </c>
-      <c r="T31" s="58">
+      <c r="T31" s="57">
         <f t="shared" si="23"/>
         <v>200.20000000000002</v>
       </c>
-      <c r="U31" s="59">
+      <c r="U31" s="58">
         <f t="shared" si="24"/>
         <v>220.22</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="45" t="s">
+    <row r="32" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
-      <c r="I32" s="24">
+      <c r="C32" s="48"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="I32" s="23">
         <v>268</v>
       </c>
-      <c r="J32" s="25"/>
-      <c r="K32" s="58">
+      <c r="J32" s="24"/>
+      <c r="K32" s="57">
         <f t="shared" si="14"/>
         <v>18.760000000000002</v>
       </c>
-      <c r="L32" s="58">
+      <c r="L32" s="57">
         <f t="shared" si="15"/>
         <v>37.520000000000003</v>
       </c>
-      <c r="M32" s="58">
+      <c r="M32" s="57">
         <f t="shared" si="16"/>
         <v>56.280000000000008</v>
       </c>
-      <c r="N32" s="95">
+      <c r="N32" s="92">
         <f t="shared" si="17"/>
         <v>75.040000000000006</v>
       </c>
-      <c r="O32" s="58">
+      <c r="O32" s="57">
         <f t="shared" si="18"/>
         <v>93.800000000000011</v>
       </c>
-      <c r="P32" s="58">
+      <c r="P32" s="57">
         <f t="shared" si="19"/>
         <v>112.56000000000002</v>
       </c>
-      <c r="Q32" s="58">
+      <c r="Q32" s="57">
         <f t="shared" si="20"/>
         <v>131.32000000000002</v>
       </c>
-      <c r="R32" s="58">
+      <c r="R32" s="57">
         <f t="shared" si="21"/>
         <v>150.08000000000001</v>
       </c>
-      <c r="S32" s="58">
+      <c r="S32" s="57">
         <f t="shared" si="22"/>
         <v>168.84000000000003</v>
       </c>
-      <c r="T32" s="58">
+      <c r="T32" s="57">
         <f t="shared" si="23"/>
         <v>187.60000000000002</v>
       </c>
-      <c r="U32" s="59">
+      <c r="U32" s="58">
         <f t="shared" si="24"/>
         <v>206.36</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I33" s="24">
+    <row r="33" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="I33" s="23">
         <v>260</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="58">
+      <c r="J33" s="24"/>
+      <c r="K33" s="57">
         <f t="shared" si="14"/>
         <v>18.200000000000003</v>
       </c>
-      <c r="L33" s="58">
+      <c r="L33" s="57">
         <f t="shared" si="15"/>
         <v>36.400000000000006</v>
       </c>
-      <c r="M33" s="58">
+      <c r="M33" s="57">
         <f t="shared" si="16"/>
         <v>54.600000000000009</v>
       </c>
-      <c r="N33" s="58">
+      <c r="N33" s="57">
         <f t="shared" si="17"/>
         <v>72.800000000000011</v>
       </c>
-      <c r="O33" s="58">
+      <c r="O33" s="57">
         <f t="shared" si="18"/>
         <v>91.000000000000014</v>
       </c>
-      <c r="P33" s="58">
+      <c r="P33" s="57">
         <f t="shared" si="19"/>
         <v>109.20000000000002</v>
       </c>
-      <c r="Q33" s="58">
+      <c r="Q33" s="57">
         <f t="shared" si="20"/>
         <v>127.4</v>
       </c>
-      <c r="R33" s="58">
+      <c r="R33" s="57">
         <f t="shared" si="21"/>
         <v>145.60000000000002</v>
       </c>
-      <c r="S33" s="58">
+      <c r="S33" s="57">
         <f t="shared" si="22"/>
         <v>163.80000000000004</v>
       </c>
-      <c r="T33" s="58">
+      <c r="T33" s="57">
         <f t="shared" si="23"/>
         <v>182.00000000000003</v>
       </c>
-      <c r="U33" s="59">
+      <c r="U33" s="58">
         <f t="shared" si="24"/>
         <v>200.20000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3200,1025 +3206,1020 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="24">
+      <c r="H34" s="109"/>
+      <c r="I34" s="23">
         <v>250</v>
       </c>
-      <c r="J34" s="25"/>
-      <c r="K34" s="58">
+      <c r="J34" s="24"/>
+      <c r="K34" s="57">
         <f t="shared" si="14"/>
         <v>17.5</v>
       </c>
-      <c r="L34" s="58">
+      <c r="L34" s="57">
         <f t="shared" si="15"/>
         <v>35</v>
       </c>
-      <c r="M34" s="58">
+      <c r="M34" s="57">
         <f t="shared" si="16"/>
         <v>52.500000000000007</v>
       </c>
-      <c r="N34" s="95">
+      <c r="N34" s="92">
         <f t="shared" si="17"/>
         <v>70</v>
       </c>
-      <c r="O34" s="58">
+      <c r="O34" s="57">
         <f t="shared" si="18"/>
         <v>87.500000000000014</v>
       </c>
-      <c r="P34" s="58">
+      <c r="P34" s="57">
         <f t="shared" si="19"/>
         <v>105.00000000000001</v>
       </c>
-      <c r="Q34" s="58">
+      <c r="Q34" s="57">
         <f t="shared" si="20"/>
         <v>122.50000000000001</v>
       </c>
-      <c r="R34" s="58">
+      <c r="R34" s="57">
         <f t="shared" si="21"/>
         <v>140</v>
       </c>
-      <c r="S34" s="58">
+      <c r="S34" s="57">
         <f t="shared" si="22"/>
         <v>157.50000000000003</v>
       </c>
-      <c r="T34" s="58">
+      <c r="T34" s="57">
         <f t="shared" si="23"/>
         <v>175.00000000000003</v>
       </c>
-      <c r="U34" s="59">
+      <c r="U34" s="58">
         <f t="shared" si="24"/>
         <v>192.5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="I35" s="24">
+      <c r="I35" s="23">
         <v>239</v>
       </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="58">
+      <c r="J35" s="24"/>
+      <c r="K35" s="57">
         <f t="shared" si="14"/>
         <v>16.73</v>
       </c>
-      <c r="L35" s="58">
+      <c r="L35" s="57">
         <f t="shared" si="15"/>
         <v>33.46</v>
       </c>
-      <c r="M35" s="58">
+      <c r="M35" s="57">
         <f t="shared" si="16"/>
         <v>50.190000000000005</v>
       </c>
-      <c r="N35" s="58">
+      <c r="N35" s="57">
         <f t="shared" si="17"/>
         <v>66.92</v>
       </c>
-      <c r="O35" s="58">
+      <c r="O35" s="57">
         <f t="shared" si="18"/>
         <v>83.65</v>
       </c>
-      <c r="P35" s="95">
+      <c r="P35" s="92">
         <f t="shared" si="19"/>
         <v>100.38000000000001</v>
       </c>
-      <c r="Q35" s="58">
+      <c r="Q35" s="57">
         <f t="shared" si="20"/>
         <v>117.11000000000001</v>
       </c>
-      <c r="R35" s="58">
+      <c r="R35" s="57">
         <f t="shared" si="21"/>
         <v>133.84</v>
       </c>
-      <c r="S35" s="58">
+      <c r="S35" s="57">
         <f t="shared" si="22"/>
         <v>150.57000000000002</v>
       </c>
-      <c r="T35" s="58">
+      <c r="T35" s="57">
         <f t="shared" si="23"/>
         <v>167.3</v>
       </c>
-      <c r="U35" s="59">
+      <c r="U35" s="58">
         <f t="shared" si="24"/>
         <v>184.03</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I36" s="24">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I36" s="23">
         <v>229</v>
       </c>
-      <c r="J36" s="25"/>
-      <c r="K36" s="58">
+      <c r="J36" s="24"/>
+      <c r="K36" s="57">
         <f t="shared" si="14"/>
         <v>16.03</v>
       </c>
-      <c r="L36" s="58">
+      <c r="L36" s="57">
         <f t="shared" si="15"/>
         <v>32.06</v>
       </c>
-      <c r="M36" s="58">
+      <c r="M36" s="57">
         <f t="shared" si="16"/>
         <v>48.09</v>
       </c>
-      <c r="N36" s="58">
+      <c r="N36" s="57">
         <f t="shared" si="17"/>
         <v>64.12</v>
       </c>
-      <c r="O36" s="95">
+      <c r="O36" s="92">
         <f t="shared" si="18"/>
         <v>80.150000000000006</v>
       </c>
-      <c r="P36" s="58">
+      <c r="P36" s="57">
         <f t="shared" si="19"/>
         <v>96.18</v>
       </c>
-      <c r="Q36" s="58">
+      <c r="Q36" s="57">
         <f t="shared" si="20"/>
         <v>112.21000000000001</v>
       </c>
-      <c r="R36" s="58">
+      <c r="R36" s="57">
         <f t="shared" si="21"/>
         <v>128.24</v>
       </c>
-      <c r="S36" s="58">
+      <c r="S36" s="57">
         <f t="shared" si="22"/>
         <v>144.27000000000004</v>
       </c>
-      <c r="T36" s="58">
+      <c r="T36" s="57">
         <f t="shared" si="23"/>
         <v>160.30000000000001</v>
       </c>
-      <c r="U36" s="59">
+      <c r="U36" s="58">
         <f t="shared" si="24"/>
         <v>176.33</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I37" s="24">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I37" s="23">
         <v>220</v>
       </c>
-      <c r="J37" s="25"/>
-      <c r="K37" s="58">
+      <c r="J37" s="24"/>
+      <c r="K37" s="57">
         <f t="shared" si="14"/>
         <v>15.400000000000002</v>
       </c>
-      <c r="L37" s="58">
+      <c r="L37" s="57">
         <f t="shared" si="15"/>
         <v>30.800000000000004</v>
       </c>
-      <c r="M37" s="58">
+      <c r="M37" s="57">
         <f t="shared" si="16"/>
         <v>46.2</v>
       </c>
-      <c r="N37" s="58">
+      <c r="N37" s="57">
         <f t="shared" si="17"/>
         <v>61.600000000000009</v>
       </c>
-      <c r="O37" s="58">
+      <c r="O37" s="57">
         <f t="shared" si="18"/>
         <v>77.000000000000014</v>
       </c>
-      <c r="P37" s="58">
+      <c r="P37" s="57">
         <f t="shared" si="19"/>
         <v>92.4</v>
       </c>
-      <c r="Q37" s="58">
+      <c r="Q37" s="57">
         <f t="shared" si="20"/>
         <v>107.80000000000001</v>
       </c>
-      <c r="R37" s="58">
+      <c r="R37" s="57">
         <f t="shared" si="21"/>
         <v>123.20000000000002</v>
       </c>
-      <c r="S37" s="58">
+      <c r="S37" s="57">
         <f t="shared" si="22"/>
         <v>138.60000000000002</v>
       </c>
-      <c r="T37" s="58">
+      <c r="T37" s="57">
         <f t="shared" si="23"/>
         <v>154.00000000000003</v>
       </c>
-      <c r="U37" s="59">
+      <c r="U37" s="58">
         <f t="shared" si="24"/>
         <v>169.4</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I38" s="24">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I38" s="23">
         <v>215</v>
       </c>
-      <c r="J38" s="25"/>
-      <c r="K38" s="58">
+      <c r="J38" s="24"/>
+      <c r="K38" s="57">
         <f t="shared" si="14"/>
         <v>15.05</v>
       </c>
-      <c r="L38" s="58">
+      <c r="L38" s="57">
         <f t="shared" si="15"/>
         <v>30.1</v>
       </c>
-      <c r="M38" s="58">
+      <c r="M38" s="57">
         <f t="shared" si="16"/>
         <v>45.150000000000006</v>
       </c>
-      <c r="N38" s="58">
+      <c r="N38" s="57">
         <f t="shared" si="17"/>
         <v>60.2</v>
       </c>
-      <c r="O38" s="95">
+      <c r="O38" s="92">
         <f t="shared" si="18"/>
         <v>75.250000000000014</v>
       </c>
-      <c r="P38" s="58">
+      <c r="P38" s="57">
         <f t="shared" si="19"/>
         <v>90.300000000000011</v>
       </c>
-      <c r="Q38" s="58">
+      <c r="Q38" s="57">
         <f t="shared" si="20"/>
         <v>105.35000000000001</v>
       </c>
-      <c r="R38" s="58">
+      <c r="R38" s="57">
         <f t="shared" si="21"/>
         <v>120.4</v>
       </c>
-      <c r="S38" s="58">
+      <c r="S38" s="57">
         <f t="shared" si="22"/>
         <v>135.45000000000002</v>
       </c>
-      <c r="T38" s="58">
+      <c r="T38" s="57">
         <f t="shared" si="23"/>
         <v>150.50000000000003</v>
       </c>
-      <c r="U38" s="59">
+      <c r="U38" s="58">
         <f t="shared" si="24"/>
         <v>165.55</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I39" s="94">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I39" s="91">
         <v>205</v>
       </c>
-      <c r="J39" s="25"/>
-      <c r="K39" s="58">
+      <c r="J39" s="24"/>
+      <c r="K39" s="57">
         <f t="shared" si="14"/>
         <v>14.350000000000001</v>
       </c>
-      <c r="L39" s="58">
+      <c r="L39" s="57">
         <f t="shared" si="15"/>
         <v>28.700000000000003</v>
       </c>
-      <c r="M39" s="58">
+      <c r="M39" s="57">
         <f t="shared" si="16"/>
         <v>43.050000000000004</v>
       </c>
-      <c r="N39" s="58">
+      <c r="N39" s="57">
         <f t="shared" si="17"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="O39" s="58">
+      <c r="O39" s="57">
         <f t="shared" si="18"/>
         <v>71.75</v>
       </c>
-      <c r="P39" s="58">
+      <c r="P39" s="57">
         <f t="shared" si="19"/>
         <v>86.100000000000009</v>
       </c>
-      <c r="Q39" s="95">
+      <c r="Q39" s="92">
         <f t="shared" si="20"/>
         <v>100.45</v>
       </c>
-      <c r="R39" s="58">
+      <c r="R39" s="57">
         <f t="shared" si="21"/>
         <v>114.80000000000001</v>
       </c>
-      <c r="S39" s="58">
+      <c r="S39" s="57">
         <f t="shared" si="22"/>
         <v>129.15000000000003</v>
       </c>
-      <c r="T39" s="58">
+      <c r="T39" s="57">
         <f t="shared" si="23"/>
         <v>143.5</v>
       </c>
-      <c r="U39" s="59">
+      <c r="U39" s="58">
         <f t="shared" si="24"/>
         <v>157.85</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I40" s="94">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I40" s="91">
         <v>200</v>
       </c>
-      <c r="J40" s="25"/>
-      <c r="K40" s="58">
+      <c r="J40" s="24"/>
+      <c r="K40" s="57">
         <f t="shared" si="14"/>
         <v>14.000000000000002</v>
       </c>
-      <c r="L40" s="58">
+      <c r="L40" s="57">
         <f t="shared" si="15"/>
         <v>28.000000000000004</v>
       </c>
-      <c r="M40" s="58">
+      <c r="M40" s="57">
         <f t="shared" si="16"/>
         <v>42.000000000000007</v>
       </c>
-      <c r="N40" s="58">
+      <c r="N40" s="57">
         <f t="shared" si="17"/>
         <v>56.000000000000007</v>
       </c>
-      <c r="O40" s="95">
+      <c r="O40" s="92">
         <f t="shared" si="18"/>
         <v>70</v>
       </c>
-      <c r="P40" s="58">
+      <c r="P40" s="57">
         <f t="shared" si="19"/>
         <v>84.000000000000014</v>
       </c>
-      <c r="Q40" s="58">
+      <c r="Q40" s="57">
         <f t="shared" si="20"/>
         <v>98.000000000000014</v>
       </c>
-      <c r="R40" s="58">
+      <c r="R40" s="57">
         <f t="shared" si="21"/>
         <v>112.00000000000001</v>
       </c>
-      <c r="S40" s="58">
+      <c r="S40" s="57">
         <f t="shared" si="22"/>
         <v>126.00000000000003</v>
       </c>
-      <c r="T40" s="58">
+      <c r="T40" s="57">
         <f t="shared" si="23"/>
         <v>140</v>
       </c>
-      <c r="U40" s="59">
+      <c r="U40" s="58">
         <f t="shared" si="24"/>
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I41" s="24">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I41" s="23">
         <v>191</v>
       </c>
-      <c r="J41" s="25"/>
-      <c r="K41" s="58">
+      <c r="J41" s="24"/>
+      <c r="K41" s="57">
         <f t="shared" si="14"/>
         <v>13.370000000000001</v>
       </c>
-      <c r="L41" s="58">
+      <c r="L41" s="57">
         <f t="shared" si="15"/>
         <v>26.740000000000002</v>
       </c>
-      <c r="M41" s="58">
+      <c r="M41" s="57">
         <f t="shared" si="16"/>
         <v>40.110000000000007</v>
       </c>
-      <c r="N41" s="58">
+      <c r="N41" s="57">
         <f t="shared" si="17"/>
         <v>53.480000000000004</v>
       </c>
-      <c r="O41" s="58">
+      <c r="O41" s="57">
         <f t="shared" si="18"/>
         <v>66.850000000000009</v>
       </c>
-      <c r="P41" s="95">
+      <c r="P41" s="92">
         <f t="shared" si="19"/>
         <v>80.220000000000013</v>
       </c>
-      <c r="Q41" s="58">
+      <c r="Q41" s="57">
         <f t="shared" si="20"/>
         <v>93.59</v>
       </c>
-      <c r="R41" s="58">
+      <c r="R41" s="57">
         <f t="shared" si="21"/>
         <v>106.96000000000001</v>
       </c>
-      <c r="S41" s="58">
+      <c r="S41" s="57">
         <f t="shared" si="22"/>
         <v>120.33000000000003</v>
       </c>
-      <c r="T41" s="58">
+      <c r="T41" s="57">
         <f t="shared" si="23"/>
         <v>133.70000000000002</v>
       </c>
-      <c r="U41" s="59">
+      <c r="U41" s="58">
         <f t="shared" si="24"/>
         <v>147.07</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I42" s="24">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I42" s="23">
         <v>180</v>
       </c>
-      <c r="J42" s="25"/>
-      <c r="K42" s="58">
+      <c r="J42" s="24"/>
+      <c r="K42" s="57">
         <f t="shared" si="14"/>
         <v>12.600000000000001</v>
       </c>
-      <c r="L42" s="58">
+      <c r="L42" s="57">
         <f t="shared" si="15"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="M42" s="58">
+      <c r="M42" s="57">
         <f t="shared" si="16"/>
         <v>37.800000000000004</v>
       </c>
-      <c r="N42" s="58">
+      <c r="N42" s="57">
         <f t="shared" si="17"/>
         <v>50.400000000000006</v>
       </c>
-      <c r="O42" s="58">
+      <c r="O42" s="57">
         <f t="shared" si="18"/>
         <v>63.000000000000007</v>
       </c>
-      <c r="P42" s="58">
+      <c r="P42" s="57">
         <f t="shared" si="19"/>
         <v>75.600000000000009</v>
       </c>
-      <c r="Q42" s="58">
+      <c r="Q42" s="57">
         <f t="shared" si="20"/>
         <v>88.2</v>
       </c>
-      <c r="R42" s="58">
+      <c r="R42" s="57">
         <f t="shared" si="21"/>
         <v>100.80000000000001</v>
       </c>
-      <c r="S42" s="58">
+      <c r="S42" s="57">
         <f t="shared" si="22"/>
         <v>113.40000000000002</v>
       </c>
-      <c r="T42" s="58">
+      <c r="T42" s="57">
         <f t="shared" si="23"/>
         <v>126.00000000000001</v>
       </c>
-      <c r="U42" s="59">
+      <c r="U42" s="58">
         <f t="shared" si="24"/>
         <v>138.6</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I43" s="24">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I43" s="23">
         <v>179</v>
       </c>
-      <c r="J43" s="25"/>
-      <c r="K43" s="58">
+      <c r="J43" s="24"/>
+      <c r="K43" s="57">
         <f t="shared" si="14"/>
         <v>12.530000000000001</v>
       </c>
-      <c r="L43" s="58">
+      <c r="L43" s="57">
         <f t="shared" si="15"/>
         <v>25.060000000000002</v>
       </c>
-      <c r="M43" s="58">
+      <c r="M43" s="57">
         <f t="shared" si="16"/>
         <v>37.590000000000003</v>
       </c>
-      <c r="N43" s="95">
+      <c r="N43" s="92">
         <f t="shared" si="17"/>
         <v>50.120000000000005</v>
       </c>
-      <c r="O43" s="58">
+      <c r="O43" s="57">
         <f t="shared" si="18"/>
         <v>62.650000000000006</v>
       </c>
-      <c r="P43" s="95">
+      <c r="P43" s="92">
         <f t="shared" si="19"/>
         <v>75.180000000000007</v>
       </c>
-      <c r="Q43" s="58">
+      <c r="Q43" s="57">
         <f t="shared" si="20"/>
         <v>87.710000000000008</v>
       </c>
-      <c r="R43" s="95">
+      <c r="R43" s="92">
         <f t="shared" si="21"/>
         <v>100.24000000000001</v>
       </c>
-      <c r="S43" s="58">
+      <c r="S43" s="57">
         <f t="shared" si="22"/>
         <v>112.77000000000002</v>
       </c>
-      <c r="T43" s="58">
+      <c r="T43" s="57">
         <f t="shared" si="23"/>
         <v>125.30000000000001</v>
       </c>
-      <c r="U43" s="59">
+      <c r="U43" s="58">
         <f t="shared" si="24"/>
         <v>137.83000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I44" s="24">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I44" s="23">
         <v>170</v>
       </c>
-      <c r="J44" s="25"/>
-      <c r="K44" s="58">
+      <c r="J44" s="24"/>
+      <c r="K44" s="57">
         <f t="shared" si="14"/>
         <v>11.9</v>
       </c>
-      <c r="L44" s="58">
+      <c r="L44" s="57">
         <f t="shared" si="15"/>
         <v>23.8</v>
       </c>
-      <c r="M44" s="58">
+      <c r="M44" s="57">
         <f t="shared" si="16"/>
         <v>35.700000000000003</v>
       </c>
-      <c r="N44" s="58">
+      <c r="N44" s="57">
         <f t="shared" si="17"/>
         <v>47.6</v>
       </c>
-      <c r="O44" s="58">
+      <c r="O44" s="57">
         <f t="shared" si="18"/>
         <v>59.500000000000007</v>
       </c>
-      <c r="P44" s="58">
+      <c r="P44" s="57">
         <f t="shared" si="19"/>
         <v>71.400000000000006</v>
       </c>
-      <c r="Q44" s="58">
+      <c r="Q44" s="57">
         <f t="shared" si="20"/>
         <v>83.300000000000011</v>
       </c>
-      <c r="R44" s="58">
+      <c r="R44" s="57">
         <f t="shared" si="21"/>
         <v>95.2</v>
       </c>
-      <c r="S44" s="58">
+      <c r="S44" s="57">
         <f t="shared" si="22"/>
         <v>107.10000000000002</v>
       </c>
-      <c r="T44" s="58">
+      <c r="T44" s="57">
         <f t="shared" si="23"/>
         <v>119.00000000000001</v>
       </c>
-      <c r="U44" s="59">
+      <c r="U44" s="58">
         <f t="shared" si="24"/>
         <v>130.9</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I45" s="24">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I45" s="23">
         <v>168</v>
       </c>
-      <c r="J45" s="25"/>
-      <c r="K45" s="58">
+      <c r="J45" s="24"/>
+      <c r="K45" s="57">
         <f t="shared" si="14"/>
         <v>11.760000000000002</v>
       </c>
-      <c r="L45" s="58">
+      <c r="L45" s="57">
         <f t="shared" si="15"/>
         <v>23.520000000000003</v>
       </c>
-      <c r="M45" s="58">
+      <c r="M45" s="57">
         <f t="shared" si="16"/>
         <v>35.28</v>
       </c>
-      <c r="N45" s="58">
+      <c r="N45" s="57">
         <f t="shared" si="17"/>
         <v>47.040000000000006</v>
       </c>
-      <c r="O45" s="58">
+      <c r="O45" s="57">
         <f t="shared" si="18"/>
         <v>58.800000000000004</v>
       </c>
-      <c r="P45" s="95">
+      <c r="P45" s="92">
         <f t="shared" si="19"/>
         <v>70.56</v>
       </c>
-      <c r="Q45" s="58">
+      <c r="Q45" s="57">
         <f t="shared" si="20"/>
         <v>82.320000000000007</v>
       </c>
-      <c r="R45" s="58">
+      <c r="R45" s="57">
         <f t="shared" si="21"/>
         <v>94.080000000000013</v>
       </c>
-      <c r="S45" s="58">
+      <c r="S45" s="57">
         <f t="shared" si="22"/>
         <v>105.84000000000002</v>
       </c>
-      <c r="T45" s="58">
+      <c r="T45" s="57">
         <f t="shared" si="23"/>
         <v>117.60000000000001</v>
       </c>
-      <c r="U45" s="59">
+      <c r="U45" s="58">
         <f t="shared" si="24"/>
         <v>129.36000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I46" s="24">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I46" s="23">
         <v>164</v>
       </c>
-      <c r="J46" s="25"/>
-      <c r="K46" s="58">
+      <c r="J46" s="24"/>
+      <c r="K46" s="57">
         <f t="shared" si="14"/>
         <v>11.48</v>
       </c>
-      <c r="L46" s="58">
+      <c r="L46" s="57">
         <f t="shared" si="15"/>
         <v>22.96</v>
       </c>
-      <c r="M46" s="58">
+      <c r="M46" s="57">
         <f t="shared" si="16"/>
         <v>34.440000000000005</v>
       </c>
-      <c r="N46" s="58">
+      <c r="N46" s="57">
         <f t="shared" si="17"/>
         <v>45.92</v>
       </c>
-      <c r="O46" s="58">
+      <c r="O46" s="57">
         <f t="shared" si="18"/>
         <v>57.400000000000006</v>
       </c>
-      <c r="P46" s="58">
+      <c r="P46" s="57">
         <f t="shared" si="19"/>
         <v>68.88000000000001</v>
       </c>
-      <c r="Q46" s="95">
+      <c r="Q46" s="92">
         <f t="shared" si="20"/>
         <v>80.360000000000014</v>
       </c>
-      <c r="R46" s="58">
+      <c r="R46" s="57">
         <f t="shared" si="21"/>
         <v>91.84</v>
       </c>
-      <c r="S46" s="58">
+      <c r="S46" s="57">
         <f t="shared" si="22"/>
         <v>103.32000000000002</v>
       </c>
-      <c r="T46" s="58">
+      <c r="T46" s="57">
         <f t="shared" si="23"/>
         <v>114.80000000000001</v>
       </c>
-      <c r="U46" s="97">
+      <c r="U46" s="94">
         <f t="shared" si="24"/>
         <v>126.28</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I47" s="24">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I47" s="23">
         <v>159</v>
       </c>
-      <c r="J47" s="25"/>
-      <c r="K47" s="58">
+      <c r="J47" s="24"/>
+      <c r="K47" s="57">
         <f t="shared" si="14"/>
         <v>11.13</v>
       </c>
-      <c r="L47" s="58">
+      <c r="L47" s="57">
         <f t="shared" si="15"/>
         <v>22.26</v>
       </c>
-      <c r="M47" s="58">
+      <c r="M47" s="57">
         <f t="shared" si="16"/>
         <v>33.39</v>
       </c>
-      <c r="N47" s="58">
+      <c r="N47" s="57">
         <f t="shared" si="17"/>
         <v>44.52</v>
       </c>
-      <c r="O47" s="58">
+      <c r="O47" s="57">
         <f t="shared" si="18"/>
         <v>55.650000000000006</v>
       </c>
-      <c r="P47" s="58">
+      <c r="P47" s="57">
         <f t="shared" si="19"/>
         <v>66.78</v>
       </c>
-      <c r="Q47" s="58">
+      <c r="Q47" s="57">
         <f t="shared" si="20"/>
         <v>77.910000000000011</v>
       </c>
-      <c r="R47" s="58">
+      <c r="R47" s="57">
         <f t="shared" si="21"/>
         <v>89.04</v>
       </c>
-      <c r="S47" s="95">
+      <c r="S47" s="92">
         <f t="shared" si="22"/>
         <v>100.17000000000002</v>
       </c>
-      <c r="T47" s="58">
+      <c r="T47" s="57">
         <f t="shared" si="23"/>
         <v>111.30000000000001</v>
       </c>
-      <c r="U47" s="59">
+      <c r="U47" s="58">
         <f t="shared" si="24"/>
         <v>122.43</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I48" s="24">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="I48" s="23">
         <v>154</v>
       </c>
-      <c r="J48" s="25"/>
-      <c r="K48" s="58">
+      <c r="J48" s="24"/>
+      <c r="K48" s="57">
         <f t="shared" si="14"/>
         <v>10.780000000000001</v>
       </c>
-      <c r="L48" s="58">
+      <c r="L48" s="57">
         <f t="shared" si="15"/>
         <v>21.560000000000002</v>
       </c>
-      <c r="M48" s="58">
+      <c r="M48" s="57">
         <f t="shared" si="16"/>
         <v>32.340000000000003</v>
       </c>
-      <c r="N48" s="58">
+      <c r="N48" s="57">
         <f t="shared" si="17"/>
         <v>43.120000000000005</v>
       </c>
-      <c r="O48" s="58">
+      <c r="O48" s="57">
         <f t="shared" si="18"/>
         <v>53.900000000000006</v>
       </c>
-      <c r="P48" s="58">
+      <c r="P48" s="57">
         <f t="shared" si="19"/>
         <v>64.680000000000007</v>
       </c>
-      <c r="Q48" s="95">
+      <c r="Q48" s="92">
         <f t="shared" si="20"/>
         <v>75.460000000000008</v>
       </c>
-      <c r="R48" s="58">
+      <c r="R48" s="57">
         <f t="shared" si="21"/>
         <v>86.240000000000009</v>
       </c>
-      <c r="S48" s="58">
+      <c r="S48" s="57">
         <f t="shared" si="22"/>
         <v>97.020000000000024</v>
       </c>
-      <c r="T48" s="58">
+      <c r="T48" s="57">
         <f t="shared" si="23"/>
         <v>107.80000000000001</v>
       </c>
-      <c r="U48" s="59">
+      <c r="U48" s="58">
         <f t="shared" si="24"/>
         <v>118.58</v>
       </c>
     </row>
-    <row r="49" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I49" s="24">
+    <row r="49" spans="9:21" x14ac:dyDescent="0.35">
+      <c r="I49" s="23">
         <v>143</v>
       </c>
-      <c r="J49" s="25"/>
-      <c r="K49" s="58">
+      <c r="J49" s="24"/>
+      <c r="K49" s="57">
         <f t="shared" si="14"/>
         <v>10.010000000000002</v>
       </c>
-      <c r="L49" s="58">
+      <c r="L49" s="57">
         <f t="shared" si="15"/>
         <v>20.020000000000003</v>
       </c>
-      <c r="M49" s="58">
+      <c r="M49" s="57">
         <f t="shared" si="16"/>
         <v>30.03</v>
       </c>
-      <c r="N49" s="58">
+      <c r="N49" s="57">
         <f t="shared" si="17"/>
         <v>40.040000000000006</v>
       </c>
-      <c r="O49" s="95">
+      <c r="O49" s="92">
         <f t="shared" si="18"/>
         <v>50.050000000000004</v>
       </c>
-      <c r="P49" s="58">
+      <c r="P49" s="57">
         <f t="shared" si="19"/>
         <v>60.06</v>
       </c>
-      <c r="Q49" s="95">
+      <c r="Q49" s="92">
         <f t="shared" si="20"/>
         <v>70.070000000000007</v>
       </c>
-      <c r="R49" s="58">
+      <c r="R49" s="57">
         <f t="shared" si="21"/>
         <v>80.080000000000013</v>
       </c>
-      <c r="S49" s="58">
+      <c r="S49" s="57">
         <f t="shared" si="22"/>
         <v>90.090000000000018</v>
       </c>
-      <c r="T49" s="95">
+      <c r="T49" s="92">
         <f t="shared" si="23"/>
         <v>100.10000000000001</v>
       </c>
-      <c r="U49" s="59">
+      <c r="U49" s="58">
         <f t="shared" si="24"/>
         <v>110.11</v>
       </c>
     </row>
-    <row r="50" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I50" s="24">
+    <row r="50" spans="9:21" x14ac:dyDescent="0.35">
+      <c r="I50" s="23">
         <v>178</v>
       </c>
-      <c r="J50" s="25"/>
-      <c r="K50" s="58">
+      <c r="J50" s="24"/>
+      <c r="K50" s="57">
         <f t="shared" si="14"/>
         <v>12.46</v>
       </c>
-      <c r="L50" s="58">
+      <c r="L50" s="57">
         <f t="shared" si="15"/>
         <v>24.92</v>
       </c>
-      <c r="M50" s="58">
+      <c r="M50" s="57">
         <f t="shared" si="16"/>
         <v>37.380000000000003</v>
       </c>
-      <c r="N50" s="58">
+      <c r="N50" s="57">
         <f t="shared" si="17"/>
         <v>49.84</v>
       </c>
-      <c r="O50" s="58">
+      <c r="O50" s="57">
         <f t="shared" si="18"/>
         <v>62.300000000000004</v>
       </c>
-      <c r="P50" s="58">
+      <c r="P50" s="57">
         <f t="shared" si="19"/>
         <v>74.760000000000005</v>
       </c>
-      <c r="Q50" s="58">
+      <c r="Q50" s="57">
         <f t="shared" si="20"/>
         <v>87.220000000000013</v>
       </c>
-      <c r="R50" s="58">
+      <c r="R50" s="57">
         <f t="shared" si="21"/>
         <v>99.68</v>
       </c>
-      <c r="S50" s="58">
+      <c r="S50" s="57">
         <f t="shared" si="22"/>
         <v>112.14000000000001</v>
       </c>
-      <c r="T50" s="58">
+      <c r="T50" s="57">
         <f t="shared" si="23"/>
         <v>124.60000000000001</v>
       </c>
-      <c r="U50" s="59">
+      <c r="U50" s="58">
         <f t="shared" si="24"/>
         <v>137.06</v>
       </c>
     </row>
-    <row r="51" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I51" s="24">
+    <row r="51" spans="9:21" x14ac:dyDescent="0.35">
+      <c r="I51" s="23">
         <v>130</v>
       </c>
-      <c r="J51" s="25"/>
-      <c r="K51" s="58">
+      <c r="J51" s="24"/>
+      <c r="K51" s="57">
         <f t="shared" si="14"/>
         <v>9.1000000000000014</v>
       </c>
-      <c r="L51" s="58">
+      <c r="L51" s="57">
         <f t="shared" si="15"/>
         <v>18.200000000000003</v>
       </c>
-      <c r="M51" s="58">
+      <c r="M51" s="57">
         <f t="shared" si="16"/>
         <v>27.300000000000004</v>
       </c>
-      <c r="N51" s="58">
+      <c r="N51" s="57">
         <f t="shared" si="17"/>
         <v>36.400000000000006</v>
       </c>
-      <c r="O51" s="58">
+      <c r="O51" s="57">
         <f t="shared" si="18"/>
         <v>45.500000000000007</v>
       </c>
-      <c r="P51" s="58">
+      <c r="P51" s="57">
         <f t="shared" si="19"/>
         <v>54.600000000000009</v>
       </c>
-      <c r="Q51" s="58">
+      <c r="Q51" s="57">
         <f t="shared" si="20"/>
         <v>63.7</v>
       </c>
-      <c r="R51" s="58">
+      <c r="R51" s="57">
         <f t="shared" si="21"/>
         <v>72.800000000000011</v>
       </c>
-      <c r="S51" s="58">
+      <c r="S51" s="57">
         <f t="shared" si="22"/>
         <v>81.90000000000002</v>
       </c>
-      <c r="T51" s="58">
+      <c r="T51" s="57">
         <f t="shared" si="23"/>
         <v>91.000000000000014</v>
       </c>
-      <c r="U51" s="97">
+      <c r="U51" s="94">
         <f t="shared" si="24"/>
         <v>100.10000000000001</v>
       </c>
     </row>
-    <row r="52" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I52" s="24">
+    <row r="52" spans="9:21" x14ac:dyDescent="0.35">
+      <c r="I52" s="23">
         <v>120</v>
       </c>
-      <c r="J52" s="25"/>
-      <c r="K52" s="58">
+      <c r="J52" s="24"/>
+      <c r="K52" s="57">
         <f t="shared" si="14"/>
         <v>8.4</v>
       </c>
-      <c r="L52" s="58">
+      <c r="L52" s="57">
         <f t="shared" si="15"/>
         <v>16.8</v>
       </c>
-      <c r="M52" s="58">
+      <c r="M52" s="57">
         <f t="shared" si="16"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="N52" s="58">
+      <c r="N52" s="57">
         <f t="shared" si="17"/>
         <v>33.6</v>
       </c>
-      <c r="O52" s="58">
+      <c r="O52" s="57">
         <f t="shared" si="18"/>
         <v>42.000000000000007</v>
       </c>
-      <c r="P52" s="95">
+      <c r="P52" s="92">
         <f t="shared" si="19"/>
         <v>50.400000000000006</v>
       </c>
-      <c r="Q52" s="58">
+      <c r="Q52" s="57">
         <f t="shared" si="20"/>
         <v>58.800000000000004</v>
       </c>
-      <c r="R52" s="58">
+      <c r="R52" s="57">
         <f t="shared" si="21"/>
         <v>67.2</v>
       </c>
-      <c r="S52" s="58">
+      <c r="S52" s="57">
         <f t="shared" si="22"/>
         <v>75.600000000000009</v>
       </c>
-      <c r="T52" s="58">
+      <c r="T52" s="57">
         <f t="shared" si="23"/>
         <v>84.000000000000014</v>
       </c>
-      <c r="U52" s="59">
+      <c r="U52" s="58">
         <f t="shared" si="24"/>
         <v>92.4</v>
       </c>
     </row>
-    <row r="53" spans="9:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I53" s="26">
+    <row r="53" spans="9:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I53" s="25">
         <v>103</v>
       </c>
-      <c r="J53" s="27"/>
-      <c r="K53" s="60">
+      <c r="J53" s="26"/>
+      <c r="K53" s="59">
         <f t="shared" si="14"/>
         <v>7.2100000000000009</v>
       </c>
-      <c r="L53" s="60">
+      <c r="L53" s="59">
         <f t="shared" si="15"/>
         <v>14.420000000000002</v>
       </c>
-      <c r="M53" s="60">
+      <c r="M53" s="59">
         <f t="shared" si="16"/>
         <v>21.630000000000003</v>
       </c>
-      <c r="N53" s="60">
+      <c r="N53" s="59">
         <f t="shared" si="17"/>
         <v>28.840000000000003</v>
       </c>
-      <c r="O53" s="60">
+      <c r="O53" s="59">
         <f t="shared" si="18"/>
         <v>36.050000000000004</v>
       </c>
-      <c r="P53" s="60">
+      <c r="P53" s="59">
         <f t="shared" si="19"/>
         <v>43.260000000000005</v>
       </c>
-      <c r="Q53" s="96">
+      <c r="Q53" s="93">
         <f t="shared" si="20"/>
         <v>50.470000000000006</v>
       </c>
-      <c r="R53" s="60">
+      <c r="R53" s="59">
         <f t="shared" si="21"/>
         <v>57.680000000000007</v>
       </c>
-      <c r="S53" s="60">
+      <c r="S53" s="59">
         <f t="shared" si="22"/>
         <v>64.890000000000015</v>
       </c>
-      <c r="T53" s="60">
+      <c r="T53" s="59">
         <f t="shared" si="23"/>
         <v>72.100000000000009</v>
       </c>
-      <c r="U53" s="61">
+      <c r="U53" s="60">
         <f t="shared" si="24"/>
         <v>79.31</v>
       </c>
     </row>
-    <row r="54" spans="9:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="O54" s="5"/>
       <c r="Q54" s="5"/>
       <c r="U54" s="5"/>
     </row>
-    <row r="55" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:21" x14ac:dyDescent="0.35">
       <c r="O55" s="5"/>
       <c r="Q55" s="5"/>
       <c r="U55" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E5:F5"/>
@@ -4235,6 +4236,11 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="K4:U21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -4243,7 +4249,7 @@
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3">
-      <formula1>"0.0,0.3"</formula1>
+      <formula1>"0.0,0.33"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3 D25">
       <formula1>"0.00,0.10,0.13,0.15,0.19,0.24,0.33"</formula1>

</xml_diff>